<commit_message>
changed dir names, confirmed requirements.txt (1 was missing --> now added)
</commit_message>
<xml_diff>
--- a/output/scores.xlsx
+++ b/output/scores.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -474,13 +474,13 @@
         <v>20753</v>
       </c>
       <c r="B3" t="n">
-        <v>8264.570374999999</v>
+        <v>8269.67175</v>
       </c>
       <c r="C3" t="n">
         <v>0</v>
       </c>
       <c r="D3" t="n">
-        <v>6611.6563</v>
+        <v>6615.7374</v>
       </c>
     </row>
     <row r="4">
@@ -488,13 +488,13 @@
         <v>10216</v>
       </c>
       <c r="B4" t="n">
-        <v>8255.739475</v>
+        <v>8260.840875</v>
       </c>
       <c r="C4" t="n">
         <v>0</v>
       </c>
       <c r="D4" t="n">
-        <v>6604.59158</v>
+        <v>6608.6727</v>
       </c>
     </row>
     <row r="5">
@@ -502,13 +502,13 @@
         <v>19359</v>
       </c>
       <c r="B5" t="n">
-        <v>8247.27045</v>
+        <v>8252.371825</v>
       </c>
       <c r="C5" t="n">
         <v>0</v>
       </c>
       <c r="D5" t="n">
-        <v>6597.816360000001</v>
+        <v>6601.89746</v>
       </c>
     </row>
     <row r="6">
@@ -516,13 +516,13 @@
         <v>27008</v>
       </c>
       <c r="B6" t="n">
-        <v>8237.291275</v>
+        <v>8242.392675000001</v>
       </c>
       <c r="C6" t="n">
         <v>0</v>
       </c>
       <c r="D6" t="n">
-        <v>6589.83302</v>
+        <v>6593.914140000001</v>
       </c>
     </row>
     <row r="7">
@@ -530,13 +530,13 @@
         <v>27734</v>
       </c>
       <c r="B7" t="n">
-        <v>8231.465674999999</v>
+        <v>8236.567075000001</v>
       </c>
       <c r="C7" t="n">
         <v>0</v>
       </c>
       <c r="D7" t="n">
-        <v>6585.17254</v>
+        <v>6589.253660000001</v>
       </c>
     </row>
     <row r="8">
@@ -544,13 +544,13 @@
         <v>21625</v>
       </c>
       <c r="B8" t="n">
-        <v>8221.555375</v>
+        <v>8226.656775000001</v>
       </c>
       <c r="C8" t="n">
         <v>0</v>
       </c>
       <c r="D8" t="n">
-        <v>6577.2443</v>
+        <v>6581.325420000001</v>
       </c>
     </row>
     <row r="9">
@@ -558,13 +558,13 @@
         <v>957</v>
       </c>
       <c r="B9" t="n">
-        <v>8218.5414</v>
+        <v>8223.6428</v>
       </c>
       <c r="C9" t="n">
         <v>0</v>
       </c>
       <c r="D9" t="n">
-        <v>6574.83312</v>
+        <v>6578.91424</v>
       </c>
     </row>
     <row r="10">
@@ -572,13 +572,13 @@
         <v>9075</v>
       </c>
       <c r="B10" t="n">
-        <v>8212.195175000001</v>
+        <v>8217.296549999999</v>
       </c>
       <c r="C10" t="n">
         <v>0</v>
       </c>
       <c r="D10" t="n">
-        <v>6569.756140000001</v>
+        <v>6573.83724</v>
       </c>
     </row>
     <row r="11">
@@ -586,13 +586,13 @@
         <v>12511</v>
       </c>
       <c r="B11" t="n">
-        <v>8208.7078</v>
+        <v>8215.188525</v>
       </c>
       <c r="C11" t="n">
         <v>0</v>
       </c>
       <c r="D11" t="n">
-        <v>6566.966240000001</v>
+        <v>6572.15082</v>
       </c>
     </row>
     <row r="12">
@@ -600,13 +600,13 @@
         <v>5329</v>
       </c>
       <c r="B12" t="n">
-        <v>8201.063775000001</v>
+        <v>8206.165175</v>
       </c>
       <c r="C12" t="n">
         <v>0</v>
       </c>
       <c r="D12" t="n">
-        <v>6560.851020000001</v>
+        <v>6564.932140000001</v>
       </c>
     </row>
     <row r="13">
@@ -614,13 +614,13 @@
         <v>3045</v>
       </c>
       <c r="B13" t="n">
-        <v>8198.367675</v>
+        <v>8203.469075000001</v>
       </c>
       <c r="C13" t="n">
         <v>0</v>
       </c>
       <c r="D13" t="n">
-        <v>6558.69414</v>
+        <v>6562.775260000001</v>
       </c>
     </row>
     <row r="14">
@@ -628,13 +628,13 @@
         <v>8057</v>
       </c>
       <c r="B14" t="n">
-        <v>8196.932150000001</v>
+        <v>8202.033500000001</v>
       </c>
       <c r="C14" t="n">
         <v>0</v>
       </c>
       <c r="D14" t="n">
-        <v>6557.545720000001</v>
+        <v>6561.626800000002</v>
       </c>
     </row>
     <row r="15">
@@ -642,13 +642,13 @@
         <v>2469</v>
       </c>
       <c r="B15" t="n">
-        <v>8195.285175000001</v>
+        <v>8200.3866</v>
       </c>
       <c r="C15" t="n">
         <v>0</v>
       </c>
       <c r="D15" t="n">
-        <v>6556.228140000001</v>
+        <v>6560.30928</v>
       </c>
     </row>
     <row r="16">
@@ -656,13 +656,13 @@
         <v>7197</v>
       </c>
       <c r="B16" t="n">
-        <v>8195.024300000001</v>
+        <v>8200.125700000001</v>
       </c>
       <c r="C16" t="n">
         <v>0</v>
       </c>
       <c r="D16" t="n">
-        <v>6556.019440000001</v>
+        <v>6560.100560000001</v>
       </c>
     </row>
     <row r="17">
@@ -670,13 +670,13 @@
         <v>9205</v>
       </c>
       <c r="B17" t="n">
-        <v>8194.159374999999</v>
+        <v>8199.260775000001</v>
       </c>
       <c r="C17" t="n">
         <v>0</v>
       </c>
       <c r="D17" t="n">
-        <v>6555.327499999999</v>
+        <v>6559.408620000001</v>
       </c>
     </row>
     <row r="18">
@@ -684,13 +684,13 @@
         <v>24463</v>
       </c>
       <c r="B18" t="n">
-        <v>8193.869475</v>
+        <v>8198.970875000001</v>
       </c>
       <c r="C18" t="n">
         <v>0</v>
       </c>
       <c r="D18" t="n">
-        <v>6555.09558</v>
+        <v>6559.176700000001</v>
       </c>
     </row>
     <row r="19">
@@ -698,13 +698,13 @@
         <v>7553</v>
       </c>
       <c r="B19" t="n">
-        <v>8190.853675</v>
+        <v>8195.955075</v>
       </c>
       <c r="C19" t="n">
         <v>0</v>
       </c>
       <c r="D19" t="n">
-        <v>6552.682940000001</v>
+        <v>6556.76406</v>
       </c>
     </row>
     <row r="20">
@@ -712,13 +712,13 @@
         <v>1770</v>
       </c>
       <c r="B20" t="n">
-        <v>8189.711875</v>
+        <v>8194.813275</v>
       </c>
       <c r="C20" t="n">
         <v>0</v>
       </c>
       <c r="D20" t="n">
-        <v>6551.7695</v>
+        <v>6555.850620000001</v>
       </c>
     </row>
     <row r="21">
@@ -726,13 +726,13 @@
         <v>29143</v>
       </c>
       <c r="B21" t="n">
-        <v>8189.482375</v>
+        <v>8194.583775000001</v>
       </c>
       <c r="C21" t="n">
         <v>0</v>
       </c>
       <c r="D21" t="n">
-        <v>6551.5859</v>
+        <v>6555.667020000001</v>
       </c>
     </row>
     <row r="22">
@@ -740,13 +740,13 @@
         <v>30543</v>
       </c>
       <c r="B22" t="n">
-        <v>8189.482375</v>
+        <v>8194.583775000001</v>
       </c>
       <c r="C22" t="n">
         <v>0</v>
       </c>
       <c r="D22" t="n">
-        <v>6551.5859</v>
+        <v>6555.667020000001</v>
       </c>
     </row>
     <row r="23">
@@ -754,13 +754,13 @@
         <v>12264</v>
       </c>
       <c r="B23" t="n">
-        <v>8186.711875</v>
+        <v>8191.8133</v>
       </c>
       <c r="C23" t="n">
         <v>0</v>
       </c>
       <c r="D23" t="n">
-        <v>6549.369500000001</v>
+        <v>6553.45064</v>
       </c>
     </row>
     <row r="24">
@@ -768,13 +768,13 @@
         <v>11990</v>
       </c>
       <c r="B24" t="n">
-        <v>8184.5831</v>
+        <v>8189.68445</v>
       </c>
       <c r="C24" t="n">
         <v>0</v>
       </c>
       <c r="D24" t="n">
-        <v>6547.66648</v>
+        <v>6551.74756</v>
       </c>
     </row>
     <row r="25">
@@ -782,13 +782,13 @@
         <v>4340</v>
       </c>
       <c r="B25" t="n">
-        <v>8183.953724999999</v>
+        <v>8189.055125</v>
       </c>
       <c r="C25" t="n">
         <v>0</v>
       </c>
       <c r="D25" t="n">
-        <v>6547.16298</v>
+        <v>6551.2441</v>
       </c>
     </row>
     <row r="26">
@@ -796,13 +796,13 @@
         <v>9208</v>
       </c>
       <c r="B26" t="n">
-        <v>8183.748825</v>
+        <v>8188.850224999999</v>
       </c>
       <c r="C26" t="n">
         <v>0</v>
       </c>
       <c r="D26" t="n">
-        <v>6546.99906</v>
+        <v>6551.08018</v>
       </c>
     </row>
     <row r="27">
@@ -810,13 +810,13 @@
         <v>12696</v>
       </c>
       <c r="B27" t="n">
-        <v>8182.929075</v>
+        <v>8188.030475</v>
       </c>
       <c r="C27" t="n">
         <v>0</v>
       </c>
       <c r="D27" t="n">
-        <v>6546.343260000001</v>
+        <v>6550.42438</v>
       </c>
     </row>
     <row r="28">
@@ -824,13 +824,13 @@
         <v>7535</v>
       </c>
       <c r="B28" t="n">
-        <v>8181.593774999999</v>
+        <v>8186.695175</v>
       </c>
       <c r="C28" t="n">
         <v>0</v>
       </c>
       <c r="D28" t="n">
-        <v>6545.27502</v>
+        <v>6549.35614</v>
       </c>
     </row>
     <row r="29">
@@ -838,13 +838,13 @@
         <v>25668</v>
       </c>
       <c r="B29" t="n">
-        <v>8175.9372</v>
+        <v>8181.038549999999</v>
       </c>
       <c r="C29" t="n">
         <v>0</v>
       </c>
       <c r="D29" t="n">
-        <v>6540.749760000001</v>
+        <v>6544.83084</v>
       </c>
     </row>
     <row r="30">
@@ -852,13 +852,13 @@
         <v>29063</v>
       </c>
       <c r="B30" t="n">
-        <v>8175.203775</v>
+        <v>8180.305199999999</v>
       </c>
       <c r="C30" t="n">
         <v>0</v>
       </c>
       <c r="D30" t="n">
-        <v>6540.16302</v>
+        <v>6544.244159999999</v>
       </c>
     </row>
     <row r="31">
@@ -866,13 +866,13 @@
         <v>13548</v>
       </c>
       <c r="B31" t="n">
-        <v>8173.580675</v>
+        <v>8178.682075</v>
       </c>
       <c r="C31" t="n">
         <v>0</v>
       </c>
       <c r="D31" t="n">
-        <v>6538.86454</v>
+        <v>6542.94566</v>
       </c>
     </row>
     <row r="32">
@@ -880,13 +880,13 @@
         <v>13554</v>
       </c>
       <c r="B32" t="n">
-        <v>8171.676975</v>
+        <v>8176.778399999999</v>
       </c>
       <c r="C32" t="n">
         <v>0</v>
       </c>
       <c r="D32" t="n">
-        <v>6537.34158</v>
+        <v>6541.42272</v>
       </c>
     </row>
     <row r="33">
@@ -894,83 +894,83 @@
         <v>15319</v>
       </c>
       <c r="B33" t="n">
-        <v>8171.637</v>
+        <v>8176.7384</v>
       </c>
       <c r="C33" t="n">
         <v>0</v>
       </c>
       <c r="D33" t="n">
-        <v>6537.309600000001</v>
+        <v>6541.39072</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>16823</v>
+        <v>9010</v>
       </c>
       <c r="B34" t="n">
-        <v>8170.810575</v>
+        <v>8176.292425</v>
       </c>
       <c r="C34" t="n">
         <v>0</v>
       </c>
       <c r="D34" t="n">
-        <v>6536.64846</v>
+        <v>6541.03394</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>14382</v>
+        <v>16823</v>
       </c>
       <c r="B35" t="n">
-        <v>8170.660974999999</v>
+        <v>8175.911975000001</v>
       </c>
       <c r="C35" t="n">
         <v>0</v>
       </c>
       <c r="D35" t="n">
-        <v>6536.52878</v>
+        <v>6540.729580000001</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>17542</v>
+        <v>14382</v>
       </c>
       <c r="B36" t="n">
-        <v>8170.5177</v>
+        <v>8175.7624</v>
       </c>
       <c r="C36" t="n">
         <v>0</v>
       </c>
       <c r="D36" t="n">
-        <v>6536.41416</v>
+        <v>6540.60992</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>13703</v>
+        <v>17542</v>
       </c>
       <c r="B37" t="n">
-        <v>8170.510174999999</v>
+        <v>8175.6191</v>
       </c>
       <c r="C37" t="n">
         <v>0</v>
       </c>
       <c r="D37" t="n">
-        <v>6536.40814</v>
+        <v>6540.49528</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>9010</v>
+        <v>13703</v>
       </c>
       <c r="B38" t="n">
-        <v>8169.899625</v>
+        <v>8175.611575000001</v>
       </c>
       <c r="C38" t="n">
         <v>0</v>
       </c>
       <c r="D38" t="n">
-        <v>6535.9197</v>
+        <v>6540.489260000001</v>
       </c>
     </row>
     <row r="39">
@@ -978,13 +978,13 @@
         <v>7897</v>
       </c>
       <c r="B39" t="n">
-        <v>8168.936775</v>
+        <v>8174.038175</v>
       </c>
       <c r="C39" t="n">
         <v>0</v>
       </c>
       <c r="D39" t="n">
-        <v>6535.149420000001</v>
+        <v>6539.23054</v>
       </c>
     </row>
     <row r="40">
@@ -992,13 +992,13 @@
         <v>5642</v>
       </c>
       <c r="B40" t="n">
-        <v>8168.486225</v>
+        <v>8173.587624999999</v>
       </c>
       <c r="C40" t="n">
         <v>0</v>
       </c>
       <c r="D40" t="n">
-        <v>6534.78898</v>
+        <v>6538.8701</v>
       </c>
     </row>
     <row r="41">
@@ -1006,13 +1006,13 @@
         <v>3559</v>
       </c>
       <c r="B41" t="n">
-        <v>8162.813474999999</v>
+        <v>8167.9149</v>
       </c>
       <c r="C41" t="n">
         <v>0</v>
       </c>
       <c r="D41" t="n">
-        <v>6530.250779999999</v>
+        <v>6534.331920000001</v>
       </c>
     </row>
     <row r="42">
@@ -1020,13 +1020,13 @@
         <v>2745</v>
       </c>
       <c r="B42" t="n">
-        <v>8162.813474999999</v>
+        <v>8167.9149</v>
       </c>
       <c r="C42" t="n">
         <v>0</v>
       </c>
       <c r="D42" t="n">
-        <v>6530.250779999999</v>
+        <v>6534.331920000001</v>
       </c>
     </row>
     <row r="43">
@@ -1034,13 +1034,13 @@
         <v>6457</v>
       </c>
       <c r="B43" t="n">
-        <v>8162.406774999999</v>
+        <v>8167.5082</v>
       </c>
       <c r="C43" t="n">
         <v>0</v>
       </c>
       <c r="D43" t="n">
-        <v>6529.92542</v>
+        <v>6534.006560000001</v>
       </c>
     </row>
     <row r="44">
@@ -1048,13 +1048,13 @@
         <v>11722</v>
       </c>
       <c r="B44" t="n">
-        <v>8162.18745</v>
+        <v>8167.288825</v>
       </c>
       <c r="C44" t="n">
         <v>0</v>
       </c>
       <c r="D44" t="n">
-        <v>6529.749960000001</v>
+        <v>6533.83106</v>
       </c>
     </row>
     <row r="45">
@@ -1062,13 +1062,13 @@
         <v>481</v>
       </c>
       <c r="B45" t="n">
-        <v>8161.898099999999</v>
+        <v>8166.9995</v>
       </c>
       <c r="C45" t="n">
         <v>0</v>
       </c>
       <c r="D45" t="n">
-        <v>6529.51848</v>
+        <v>6533.5996</v>
       </c>
     </row>
     <row r="46">
@@ -1076,13 +1076,13 @@
         <v>21249</v>
       </c>
       <c r="B46" t="n">
-        <v>8161.816475</v>
+        <v>8166.917875000001</v>
       </c>
       <c r="C46" t="n">
         <v>0</v>
       </c>
       <c r="D46" t="n">
-        <v>6529.45318</v>
+        <v>6533.534300000001</v>
       </c>
     </row>
     <row r="47">
@@ -1090,13 +1090,13 @@
         <v>20630</v>
       </c>
       <c r="B47" t="n">
-        <v>8161.525575</v>
+        <v>8166.627</v>
       </c>
       <c r="C47" t="n">
         <v>0</v>
       </c>
       <c r="D47" t="n">
-        <v>6529.22046</v>
+        <v>6533.301600000001</v>
       </c>
     </row>
     <row r="48">
@@ -1104,13 +1104,13 @@
         <v>17724</v>
       </c>
       <c r="B48" t="n">
-        <v>8159.088575</v>
+        <v>8164.18995</v>
       </c>
       <c r="C48" t="n">
         <v>0</v>
       </c>
       <c r="D48" t="n">
-        <v>6527.270860000001</v>
+        <v>6531.35196</v>
       </c>
     </row>
     <row r="49">
@@ -1118,13 +1118,13 @@
         <v>865</v>
       </c>
       <c r="B49" t="n">
-        <v>8157.561675</v>
+        <v>8162.663074999999</v>
       </c>
       <c r="C49" t="n">
         <v>0</v>
       </c>
       <c r="D49" t="n">
-        <v>6526.04934</v>
+        <v>6530.13046</v>
       </c>
     </row>
     <row r="50">
@@ -1132,13 +1132,13 @@
         <v>17762</v>
       </c>
       <c r="B50" t="n">
-        <v>8155.283574999999</v>
+        <v>8160.384975</v>
       </c>
       <c r="C50" t="n">
         <v>0</v>
       </c>
       <c r="D50" t="n">
-        <v>6524.22686</v>
+        <v>6528.30798</v>
       </c>
     </row>
     <row r="51">
@@ -1146,713 +1146,713 @@
         <v>20315</v>
       </c>
       <c r="B51" t="n">
-        <v>8154.441375</v>
+        <v>8159.542799999999</v>
       </c>
       <c r="C51" t="n">
         <v>0</v>
       </c>
       <c r="D51" t="n">
-        <v>6523.553100000001</v>
+        <v>6527.634239999999</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="n">
-        <v>30685</v>
+        <v>655</v>
       </c>
       <c r="B52" t="n">
         <v>0</v>
       </c>
       <c r="C52" t="n">
-        <v>0.9105198383331299</v>
+        <v>109.2084465026855</v>
       </c>
       <c r="D52" t="n">
-        <v>0.1046835505118303</v>
+        <v>0.001814742938011801</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="n">
-        <v>30617</v>
+        <v>656</v>
       </c>
       <c r="B53" t="n">
         <v>0</v>
       </c>
       <c r="C53" t="n">
-        <v>0.9107993841171265</v>
+        <v>114.0045280456543</v>
       </c>
       <c r="D53" t="n">
-        <v>0.1046682355366201</v>
+        <v>0.001739061960417805</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="n">
-        <v>30569</v>
+        <v>1633</v>
       </c>
       <c r="B54" t="n">
         <v>0</v>
       </c>
       <c r="C54" t="n">
-        <v>0.9115665256977081</v>
+        <v>114.2370700836182</v>
       </c>
       <c r="D54" t="n">
-        <v>0.1046262305346666</v>
+        <v>0.001735552629504345</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="n">
-        <v>30684</v>
+        <v>1974</v>
       </c>
       <c r="B55" t="n">
         <v>0</v>
       </c>
       <c r="C55" t="n">
-        <v>0.9115714430809021</v>
+        <v>114.6579132080078</v>
       </c>
       <c r="D55" t="n">
-        <v>0.1046259613910415</v>
+        <v>0.001729237494025204</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="n">
-        <v>30576</v>
+        <v>1626</v>
       </c>
       <c r="B56" t="n">
         <v>0</v>
       </c>
       <c r="C56" t="n">
-        <v>0.91169806321462</v>
+        <v>115.8846416473389</v>
       </c>
       <c r="D56" t="n">
-        <v>0.1046190315554798</v>
+        <v>0.00171108878960706</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="n">
-        <v>30618</v>
+        <v>1631</v>
       </c>
       <c r="B57" t="n">
         <v>0</v>
       </c>
       <c r="C57" t="n">
-        <v>0.9121070702870687</v>
+        <v>116.0007553100586</v>
       </c>
       <c r="D57" t="n">
-        <v>0.1045966531413817</v>
+        <v>0.001709390674188288</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="n">
-        <v>30612</v>
+        <v>1632</v>
       </c>
       <c r="B58" t="n">
         <v>0</v>
       </c>
       <c r="C58" t="n">
-        <v>0.91211998462677</v>
+        <v>116.4884853363037</v>
       </c>
       <c r="D58" t="n">
-        <v>0.1045959467020781</v>
+        <v>0.001702294479561227</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="n">
-        <v>30585</v>
+        <v>2386</v>
       </c>
       <c r="B59" t="n">
         <v>0</v>
       </c>
       <c r="C59" t="n">
-        <v>0.9121749003728231</v>
+        <v>116.6506271362305</v>
       </c>
       <c r="D59" t="n">
-        <v>0.1045929428113534</v>
+        <v>0.001699948439445336</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="n">
-        <v>30598</v>
+        <v>2435</v>
       </c>
       <c r="B60" t="n">
         <v>0</v>
       </c>
       <c r="C60" t="n">
-        <v>0.9123560388882955</v>
+        <v>116.9381294250488</v>
       </c>
       <c r="D60" t="n">
-        <v>0.1045830357595259</v>
+        <v>0.001695804410117447</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="n">
-        <v>30631</v>
+        <v>1692</v>
       </c>
       <c r="B61" t="n">
         <v>0</v>
       </c>
       <c r="C61" t="n">
-        <v>0.9124458432197571</v>
+        <v>116.9381294250488</v>
       </c>
       <c r="D61" t="n">
-        <v>0.1045781247657627</v>
+        <v>0.001695804410117447</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="n">
-        <v>30614</v>
+        <v>1241</v>
       </c>
       <c r="B62" t="n">
         <v>0</v>
       </c>
       <c r="C62" t="n">
-        <v>0.91261887550354</v>
+        <v>117.1836185455322</v>
       </c>
       <c r="D62" t="n">
-        <v>0.1045686637110833</v>
+        <v>0.001692281912344278</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="n">
-        <v>30679</v>
+        <v>1607</v>
       </c>
       <c r="B63" t="n">
         <v>0</v>
       </c>
       <c r="C63" t="n">
-        <v>0.9126254121462504</v>
+        <v>117.3836936950684</v>
       </c>
       <c r="D63" t="n">
-        <v>0.1045683063342603</v>
+        <v>0.001689421860033851</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="n">
-        <v>30646</v>
+        <v>2193</v>
       </c>
       <c r="B64" t="n">
         <v>0</v>
       </c>
       <c r="C64" t="n">
-        <v>0.9129225015640259</v>
+        <v>117.7448997497559</v>
       </c>
       <c r="D64" t="n">
-        <v>0.1045520661900719</v>
+        <v>0.001684282865381856</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="n">
-        <v>30640</v>
+        <v>659</v>
       </c>
       <c r="B65" t="n">
         <v>0</v>
       </c>
       <c r="C65" t="n">
-        <v>0.9129990935325623</v>
+        <v>118.1202259063721</v>
       </c>
       <c r="D65" t="n">
-        <v>0.1045478801721114</v>
+        <v>0.00167897599654654</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="n">
-        <v>30620</v>
+        <v>1629</v>
       </c>
       <c r="B66" t="n">
         <v>0</v>
       </c>
       <c r="C66" t="n">
-        <v>0.9139178991317749</v>
+        <v>118.4642562866211</v>
       </c>
       <c r="D66" t="n">
-        <v>0.1044976903610795</v>
+        <v>0.001674140920612739</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="n">
-        <v>30648</v>
+        <v>2313</v>
       </c>
       <c r="B67" t="n">
         <v>0</v>
       </c>
       <c r="C67" t="n">
-        <v>0.9139236410458883</v>
+        <v>118.5307502746582</v>
       </c>
       <c r="D67" t="n">
-        <v>0.1044973768601904</v>
+        <v>0.001673209609581127</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="n">
-        <v>30601</v>
+        <v>1616</v>
       </c>
       <c r="B68" t="n">
         <v>0</v>
       </c>
       <c r="C68" t="n">
-        <v>0.9142172733942667</v>
+        <v>118.7935085296631</v>
       </c>
       <c r="D68" t="n">
-        <v>0.1044813474310377</v>
+        <v>0.001669539547299229</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="n">
-        <v>30591</v>
+        <v>1628</v>
       </c>
       <c r="B69" t="n">
         <v>0</v>
       </c>
       <c r="C69" t="n">
-        <v>0.9142565280199051</v>
+        <v>118.879114151001</v>
       </c>
       <c r="D69" t="n">
-        <v>0.1044792048884267</v>
+        <v>0.00166834732986163</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="n">
-        <v>30607</v>
+        <v>1943</v>
       </c>
       <c r="B70" t="n">
         <v>0</v>
       </c>
       <c r="C70" t="n">
-        <v>0.914280116558075</v>
+        <v>119.0222949981689</v>
       </c>
       <c r="D70" t="n">
-        <v>0.1044779174531704</v>
+        <v>0.00166635707143453</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="n">
-        <v>32545</v>
+        <v>1615</v>
       </c>
       <c r="B71" t="n">
         <v>0</v>
       </c>
       <c r="C71" t="n">
-        <v>0.9142822027206421</v>
+        <v>119.2150344848633</v>
       </c>
       <c r="D71" t="n">
-        <v>0.1044778035943464</v>
+        <v>0.001663685418858178</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="n">
-        <v>30664</v>
+        <v>1608</v>
       </c>
       <c r="B72" t="n">
         <v>0</v>
       </c>
       <c r="C72" t="n">
-        <v>0.9143588145573934</v>
+        <v>119.6412525177002</v>
       </c>
       <c r="D72" t="n">
-        <v>0.1044736224364713</v>
+        <v>0.00165780772187073</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="n">
-        <v>30981</v>
+        <v>248</v>
       </c>
       <c r="B73" t="n">
         <v>0</v>
       </c>
       <c r="C73" t="n">
-        <v>0.9144829511642456</v>
+        <v>119.9710464477539</v>
       </c>
       <c r="D73" t="n">
-        <v>0.1044668482831748</v>
+        <v>0.00165328816996204</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="n">
-        <v>30604</v>
+        <v>2186</v>
       </c>
       <c r="B74" t="n">
         <v>0</v>
       </c>
       <c r="C74" t="n">
-        <v>0.9145292043685913</v>
+        <v>120.440803527832</v>
       </c>
       <c r="D74" t="n">
-        <v>0.1044643244634963</v>
+        <v>0.001646892923877629</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="n">
-        <v>30584</v>
+        <v>1236</v>
       </c>
       <c r="B75" t="n">
         <v>0</v>
       </c>
       <c r="C75" t="n">
-        <v>0.9146390358606974</v>
+        <v>120.6479911804199</v>
       </c>
       <c r="D75" t="n">
-        <v>0.1044583319644337</v>
+        <v>0.001644087979252973</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="n">
-        <v>33283</v>
+        <v>1630</v>
       </c>
       <c r="B76" t="n">
         <v>0</v>
       </c>
       <c r="C76" t="n">
-        <v>0.914705753326416</v>
+        <v>120.7178001403809</v>
       </c>
       <c r="D76" t="n">
-        <v>0.1044546921387478</v>
+        <v>0.001643145043447498</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="n">
-        <v>30687</v>
+        <v>206</v>
       </c>
       <c r="B77" t="n">
         <v>0</v>
       </c>
       <c r="C77" t="n">
-        <v>0.9147300720214844</v>
+        <v>120.7469482421875</v>
       </c>
       <c r="D77" t="n">
-        <v>0.1044533654756094</v>
+        <v>0.001642751649118515</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="n">
-        <v>30668</v>
+        <v>1622</v>
       </c>
       <c r="B78" t="n">
         <v>0</v>
       </c>
       <c r="C78" t="n">
-        <v>0.9147317409515381</v>
+        <v>120.889347076416</v>
       </c>
       <c r="D78" t="n">
-        <v>0.1044532744313356</v>
+        <v>0.001640832482879854</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="n">
-        <v>31737</v>
+        <v>1175</v>
       </c>
       <c r="B79" t="n">
         <v>0</v>
       </c>
       <c r="C79" t="n">
-        <v>0.9148092269897461</v>
+        <v>120.9107322692871</v>
       </c>
       <c r="D79" t="n">
-        <v>0.1044490475505062</v>
+        <v>0.001640544653265001</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="n">
-        <v>31284</v>
+        <v>246</v>
       </c>
       <c r="B80" t="n">
         <v>0</v>
       </c>
       <c r="C80" t="n">
-        <v>0.9148101210594177</v>
+        <v>121.2291259765625</v>
       </c>
       <c r="D80" t="n">
-        <v>0.1044489987808007</v>
+        <v>0.001636271211154288</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="n">
-        <v>32799</v>
+        <v>239</v>
       </c>
       <c r="B81" t="n">
         <v>0</v>
       </c>
       <c r="C81" t="n">
-        <v>0.9148272275924683</v>
+        <v>121.4860153198242</v>
       </c>
       <c r="D81" t="n">
-        <v>0.1044480656625413</v>
+        <v>0.001632839467246758</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="n">
-        <v>30691</v>
+        <v>2181</v>
       </c>
       <c r="B82" t="n">
         <v>0</v>
       </c>
       <c r="C82" t="n">
-        <v>0.9148518045743307</v>
+        <v>121.914644241333</v>
       </c>
       <c r="D82" t="n">
-        <v>0.1044467250793122</v>
+        <v>0.001627145416516165</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="n">
-        <v>30985</v>
+        <v>657</v>
       </c>
       <c r="B83" t="n">
         <v>0</v>
       </c>
       <c r="C83" t="n">
-        <v>0.9153034687042236</v>
+        <v>122.028247833252</v>
       </c>
       <c r="D83" t="n">
-        <v>0.1044220946017018</v>
+        <v>0.001625642919592521</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="n">
-        <v>30649</v>
+        <v>1198</v>
       </c>
       <c r="B84" t="n">
         <v>0</v>
       </c>
       <c r="C84" t="n">
-        <v>0.915366142988205</v>
+        <v>122.0571556091309</v>
       </c>
       <c r="D84" t="n">
-        <v>0.1044186777197469</v>
+        <v>0.001625261034273085</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="n">
-        <v>32866</v>
+        <v>1612</v>
       </c>
       <c r="B85" t="n">
         <v>0</v>
       </c>
       <c r="C85" t="n">
-        <v>0.9154995679855347</v>
+        <v>122.0822982788086</v>
       </c>
       <c r="D85" t="n">
-        <v>0.1044114043890561</v>
+        <v>0.001624929033636956</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="n">
-        <v>32870</v>
+        <v>1174</v>
       </c>
       <c r="B86" t="n">
         <v>0</v>
       </c>
       <c r="C86" t="n">
-        <v>0.9156795740127563</v>
+        <v>122.2451496124268</v>
       </c>
       <c r="D86" t="n">
-        <v>0.1044015934152609</v>
+        <v>0.001622781915790981</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="n">
-        <v>32725</v>
+        <v>215</v>
       </c>
       <c r="B87" t="n">
         <v>0</v>
       </c>
       <c r="C87" t="n">
-        <v>0.9157245755195618</v>
+        <v>122.2786521911621</v>
       </c>
       <c r="D87" t="n">
-        <v>0.1043991409598941</v>
+        <v>0.001622340903677872</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="n">
-        <v>32872</v>
+        <v>1029</v>
       </c>
       <c r="B88" t="n">
         <v>0</v>
       </c>
       <c r="C88" t="n">
-        <v>0.9157490928967794</v>
+        <v>122.4564075469971</v>
       </c>
       <c r="D88" t="n">
-        <v>0.1043978048803784</v>
+        <v>0.001620005020183861</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="n">
-        <v>30638</v>
+        <v>224</v>
       </c>
       <c r="B89" t="n">
         <v>0</v>
       </c>
       <c r="C89" t="n">
-        <v>0.9162121415138245</v>
+        <v>122.6510715484619</v>
       </c>
       <c r="D89" t="n">
-        <v>0.1043725773713125</v>
+        <v>0.001617454644714624</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="n">
-        <v>32863</v>
+        <v>658</v>
       </c>
       <c r="B90" t="n">
         <v>0</v>
       </c>
       <c r="C90" t="n">
-        <v>0.9162736982107162</v>
+        <v>122.9752807617188</v>
       </c>
       <c r="D90" t="n">
-        <v>0.1043692245981073</v>
+        <v>0.001613224820070391</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="n">
-        <v>30647</v>
+        <v>243</v>
       </c>
       <c r="B91" t="n">
         <v>0</v>
       </c>
       <c r="C91" t="n">
-        <v>0.9163342316945394</v>
+        <v>122.9805431365967</v>
       </c>
       <c r="D91" t="n">
-        <v>0.1043659277657154</v>
+        <v>0.001613156346473238</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="n">
-        <v>31686</v>
+        <v>644</v>
       </c>
       <c r="B92" t="n">
         <v>0</v>
       </c>
       <c r="C92" t="n">
-        <v>0.9163768291473389</v>
+        <v>123.3243179321289</v>
       </c>
       <c r="D92" t="n">
-        <v>0.1043636079074212</v>
+        <v>0.001608695734885784</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="n">
-        <v>30610</v>
+        <v>1623</v>
       </c>
       <c r="B93" t="n">
         <v>0</v>
       </c>
       <c r="C93" t="n">
-        <v>0.9164423147837321</v>
+        <v>123.3813991546631</v>
       </c>
       <c r="D93" t="n">
-        <v>0.1043600417592375</v>
+        <v>0.00160795747080565</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="n">
-        <v>32540</v>
+        <v>1606</v>
       </c>
       <c r="B94" t="n">
         <v>0</v>
       </c>
       <c r="C94" t="n">
-        <v>0.9164541363716125</v>
+        <v>123.4977226257324</v>
       </c>
       <c r="D94" t="n">
-        <v>0.1043593980175577</v>
+        <v>0.001606455088349239</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="n">
-        <v>30645</v>
+        <v>1907</v>
       </c>
       <c r="B95" t="n">
         <v>0</v>
       </c>
       <c r="C95" t="n">
-        <v>0.9164692163467407</v>
+        <v>123.7233867645264</v>
       </c>
       <c r="D95" t="n">
-        <v>0.1043585768527234</v>
+        <v>0.001603548501914829</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="n">
-        <v>32804</v>
+        <v>229</v>
       </c>
       <c r="B96" t="n">
         <v>0</v>
       </c>
       <c r="C96" t="n">
-        <v>0.9165424108505249</v>
+        <v>123.8089752197266</v>
       </c>
       <c r="D96" t="n">
-        <v>0.1043545913034316</v>
+        <v>0.00160244885953033</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="n">
-        <v>32869</v>
+        <v>1617</v>
       </c>
       <c r="B97" t="n">
         <v>0</v>
       </c>
       <c r="C97" t="n">
-        <v>0.9165677428245544</v>
+        <v>123.8158950805664</v>
       </c>
       <c r="D97" t="n">
-        <v>0.1043532120107838</v>
+        <v>0.001602360018897462</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="n">
-        <v>31801</v>
+        <v>1611</v>
       </c>
       <c r="B98" t="n">
         <v>0</v>
       </c>
       <c r="C98" t="n">
-        <v>0.9166028499603271</v>
+        <v>123.8311805725098</v>
       </c>
       <c r="D98" t="n">
-        <v>0.1043513005337229</v>
+        <v>0.001602163811018574</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="n">
-        <v>31864</v>
+        <v>1145</v>
       </c>
       <c r="B99" t="n">
         <v>0</v>
       </c>
       <c r="C99" t="n">
-        <v>0.9166196584701538</v>
+        <v>123.8582515716553</v>
       </c>
       <c r="D99" t="n">
-        <v>0.1043503853861334</v>
+        <v>0.001601816439702597</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="n">
-        <v>30656</v>
+        <v>1625</v>
       </c>
       <c r="B100" t="n">
         <v>0</v>
       </c>
       <c r="C100" t="n">
-        <v>0.9166521728038788</v>
+        <v>123.9412727355957</v>
       </c>
       <c r="D100" t="n">
-        <v>0.104348615172788</v>
+        <v>0.001600752062316875</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="n">
-        <v>32965</v>
+        <v>649</v>
       </c>
       <c r="B101" t="n">
         <v>0</v>
       </c>
       <c r="C101" t="n">
-        <v>0.9167695045471191</v>
+        <v>124.1615924835205</v>
       </c>
       <c r="D101" t="n">
-        <v>0.1043422276520695</v>
+        <v>0.001597934286640953</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added validation compared to IPA
</commit_message>
<xml_diff>
--- a/output/scores.xlsx
+++ b/output/scores.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -460,13 +460,13 @@
         <v>21475</v>
       </c>
       <c r="B2" t="n">
-        <v>8293.129499999999</v>
+        <v>8244.1301</v>
       </c>
       <c r="C2" t="n">
         <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>6634.5036</v>
+        <v>6595.304080000001</v>
       </c>
     </row>
     <row r="3">
@@ -474,13 +474,13 @@
         <v>20753</v>
       </c>
       <c r="B3" t="n">
-        <v>8269.67175</v>
+        <v>8237.045725</v>
       </c>
       <c r="C3" t="n">
         <v>0</v>
       </c>
       <c r="D3" t="n">
-        <v>6615.7374</v>
+        <v>6589.63658</v>
       </c>
     </row>
     <row r="4">
@@ -488,13 +488,13 @@
         <v>10216</v>
       </c>
       <c r="B4" t="n">
-        <v>8260.840875</v>
+        <v>8228.214875</v>
       </c>
       <c r="C4" t="n">
         <v>0</v>
       </c>
       <c r="D4" t="n">
-        <v>6608.6727</v>
+        <v>6582.5719</v>
       </c>
     </row>
     <row r="5">
@@ -502,13 +502,13 @@
         <v>19359</v>
       </c>
       <c r="B5" t="n">
-        <v>8252.371825</v>
+        <v>8219.745825</v>
       </c>
       <c r="C5" t="n">
         <v>0</v>
       </c>
       <c r="D5" t="n">
-        <v>6601.89746</v>
+        <v>6575.79666</v>
       </c>
     </row>
     <row r="6">
@@ -516,13 +516,13 @@
         <v>27008</v>
       </c>
       <c r="B6" t="n">
-        <v>8242.392675000001</v>
+        <v>8209.766650000001</v>
       </c>
       <c r="C6" t="n">
         <v>0</v>
       </c>
       <c r="D6" t="n">
-        <v>6593.914140000001</v>
+        <v>6567.813320000001</v>
       </c>
     </row>
     <row r="7">
@@ -530,13 +530,13 @@
         <v>27734</v>
       </c>
       <c r="B7" t="n">
-        <v>8236.567075000001</v>
+        <v>8203.941075000001</v>
       </c>
       <c r="C7" t="n">
         <v>0</v>
       </c>
       <c r="D7" t="n">
-        <v>6589.253660000001</v>
+        <v>6563.152860000001</v>
       </c>
     </row>
     <row r="8">
@@ -544,13 +544,13 @@
         <v>21625</v>
       </c>
       <c r="B8" t="n">
-        <v>8226.656775000001</v>
+        <v>8194.030774999999</v>
       </c>
       <c r="C8" t="n">
         <v>0</v>
       </c>
       <c r="D8" t="n">
-        <v>6581.325420000001</v>
+        <v>6555.22462</v>
       </c>
     </row>
     <row r="9">
@@ -558,13 +558,13 @@
         <v>957</v>
       </c>
       <c r="B9" t="n">
-        <v>8223.6428</v>
+        <v>8191.016825</v>
       </c>
       <c r="C9" t="n">
         <v>0</v>
       </c>
       <c r="D9" t="n">
-        <v>6578.91424</v>
+        <v>6552.81346</v>
       </c>
     </row>
     <row r="10">
@@ -572,13 +572,13 @@
         <v>9075</v>
       </c>
       <c r="B10" t="n">
-        <v>8217.296549999999</v>
+        <v>8184.670525</v>
       </c>
       <c r="C10" t="n">
         <v>0</v>
       </c>
       <c r="D10" t="n">
-        <v>6573.83724</v>
+        <v>6547.73642</v>
       </c>
     </row>
     <row r="11">
@@ -586,13 +586,13 @@
         <v>12511</v>
       </c>
       <c r="B11" t="n">
-        <v>8215.188525</v>
+        <v>8181.183225</v>
       </c>
       <c r="C11" t="n">
         <v>0</v>
       </c>
       <c r="D11" t="n">
-        <v>6572.15082</v>
+        <v>6544.94658</v>
       </c>
     </row>
     <row r="12">
@@ -600,13 +600,13 @@
         <v>5329</v>
       </c>
       <c r="B12" t="n">
-        <v>8206.165175</v>
+        <v>8173.53915</v>
       </c>
       <c r="C12" t="n">
         <v>0</v>
       </c>
       <c r="D12" t="n">
-        <v>6564.932140000001</v>
+        <v>6538.83132</v>
       </c>
     </row>
     <row r="13">
@@ -614,13 +614,13 @@
         <v>3045</v>
       </c>
       <c r="B13" t="n">
-        <v>8203.469075000001</v>
+        <v>8170.843075000001</v>
       </c>
       <c r="C13" t="n">
         <v>0</v>
       </c>
       <c r="D13" t="n">
-        <v>6562.775260000001</v>
+        <v>6536.674460000001</v>
       </c>
     </row>
     <row r="14">
@@ -628,13 +628,13 @@
         <v>8057</v>
       </c>
       <c r="B14" t="n">
-        <v>8202.033500000001</v>
+        <v>8169.407525</v>
       </c>
       <c r="C14" t="n">
         <v>0</v>
       </c>
       <c r="D14" t="n">
-        <v>6561.626800000002</v>
+        <v>6535.52602</v>
       </c>
     </row>
     <row r="15">
@@ -642,13 +642,13 @@
         <v>2469</v>
       </c>
       <c r="B15" t="n">
-        <v>8200.3866</v>
+        <v>8167.7606</v>
       </c>
       <c r="C15" t="n">
         <v>0</v>
       </c>
       <c r="D15" t="n">
-        <v>6560.30928</v>
+        <v>6534.20848</v>
       </c>
     </row>
     <row r="16">
@@ -656,13 +656,13 @@
         <v>7197</v>
       </c>
       <c r="B16" t="n">
-        <v>8200.125700000001</v>
+        <v>8167.499725</v>
       </c>
       <c r="C16" t="n">
         <v>0</v>
       </c>
       <c r="D16" t="n">
-        <v>6560.100560000001</v>
+        <v>6533.99978</v>
       </c>
     </row>
     <row r="17">
@@ -670,13 +670,13 @@
         <v>9205</v>
       </c>
       <c r="B17" t="n">
-        <v>8199.260775000001</v>
+        <v>8166.634775</v>
       </c>
       <c r="C17" t="n">
         <v>0</v>
       </c>
       <c r="D17" t="n">
-        <v>6559.408620000001</v>
+        <v>6533.307820000001</v>
       </c>
     </row>
     <row r="18">
@@ -684,13 +684,13 @@
         <v>24463</v>
       </c>
       <c r="B18" t="n">
-        <v>8198.970875000001</v>
+        <v>8166.344875000001</v>
       </c>
       <c r="C18" t="n">
         <v>0</v>
       </c>
       <c r="D18" t="n">
-        <v>6559.176700000001</v>
+        <v>6533.075900000001</v>
       </c>
     </row>
     <row r="19">
@@ -698,13 +698,13 @@
         <v>7553</v>
       </c>
       <c r="B19" t="n">
-        <v>8195.955075</v>
+        <v>8163.329075</v>
       </c>
       <c r="C19" t="n">
         <v>0</v>
       </c>
       <c r="D19" t="n">
-        <v>6556.76406</v>
+        <v>6530.66326</v>
       </c>
     </row>
     <row r="20">
@@ -712,13 +712,13 @@
         <v>1770</v>
       </c>
       <c r="B20" t="n">
-        <v>8194.813275</v>
+        <v>8162.187249999999</v>
       </c>
       <c r="C20" t="n">
         <v>0</v>
       </c>
       <c r="D20" t="n">
-        <v>6555.850620000001</v>
+        <v>6529.7498</v>
       </c>
     </row>
     <row r="21">
@@ -726,13 +726,13 @@
         <v>29143</v>
       </c>
       <c r="B21" t="n">
-        <v>8194.583775000001</v>
+        <v>8161.957775</v>
       </c>
       <c r="C21" t="n">
         <v>0</v>
       </c>
       <c r="D21" t="n">
-        <v>6555.667020000001</v>
+        <v>6529.566220000001</v>
       </c>
     </row>
     <row r="22">
@@ -740,13 +740,13 @@
         <v>30543</v>
       </c>
       <c r="B22" t="n">
-        <v>8194.583775000001</v>
+        <v>8161.957775</v>
       </c>
       <c r="C22" t="n">
         <v>0</v>
       </c>
       <c r="D22" t="n">
-        <v>6555.667020000001</v>
+        <v>6529.566220000001</v>
       </c>
     </row>
     <row r="23">
@@ -754,13 +754,13 @@
         <v>12264</v>
       </c>
       <c r="B23" t="n">
-        <v>8191.8133</v>
+        <v>8159.1873</v>
       </c>
       <c r="C23" t="n">
         <v>0</v>
       </c>
       <c r="D23" t="n">
-        <v>6553.45064</v>
+        <v>6527.34984</v>
       </c>
     </row>
     <row r="24">
@@ -768,55 +768,55 @@
         <v>11990</v>
       </c>
       <c r="B24" t="n">
-        <v>8189.68445</v>
+        <v>8155.97275</v>
       </c>
       <c r="C24" t="n">
         <v>0</v>
       </c>
       <c r="D24" t="n">
-        <v>6551.74756</v>
+        <v>6524.778200000001</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>4340</v>
+        <v>12696</v>
       </c>
       <c r="B25" t="n">
-        <v>8189.055125</v>
+        <v>8155.404474999999</v>
       </c>
       <c r="C25" t="n">
         <v>0</v>
       </c>
       <c r="D25" t="n">
-        <v>6551.2441</v>
+        <v>6524.32358</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>9208</v>
+        <v>4340</v>
       </c>
       <c r="B26" t="n">
-        <v>8188.850224999999</v>
+        <v>8155.3434</v>
       </c>
       <c r="C26" t="n">
         <v>0</v>
       </c>
       <c r="D26" t="n">
-        <v>6551.08018</v>
+        <v>6524.27472</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>12696</v>
+        <v>9208</v>
       </c>
       <c r="B27" t="n">
-        <v>8188.030475</v>
+        <v>8155.138499999999</v>
       </c>
       <c r="C27" t="n">
         <v>0</v>
       </c>
       <c r="D27" t="n">
-        <v>6550.42438</v>
+        <v>6524.110799999999</v>
       </c>
     </row>
     <row r="28">
@@ -824,41 +824,41 @@
         <v>7535</v>
       </c>
       <c r="B28" t="n">
-        <v>8186.695175</v>
+        <v>8154.069175000001</v>
       </c>
       <c r="C28" t="n">
         <v>0</v>
       </c>
       <c r="D28" t="n">
-        <v>6549.35614</v>
+        <v>6523.255340000001</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>25668</v>
+        <v>29063</v>
       </c>
       <c r="B29" t="n">
-        <v>8181.038549999999</v>
+        <v>8147.679225</v>
       </c>
       <c r="C29" t="n">
         <v>0</v>
       </c>
       <c r="D29" t="n">
-        <v>6544.83084</v>
+        <v>6518.14338</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>29063</v>
+        <v>25668</v>
       </c>
       <c r="B30" t="n">
-        <v>8180.305199999999</v>
+        <v>8147.32685</v>
       </c>
       <c r="C30" t="n">
         <v>0</v>
       </c>
       <c r="D30" t="n">
-        <v>6544.244159999999</v>
+        <v>6517.86148</v>
       </c>
     </row>
     <row r="31">
@@ -866,13 +866,13 @@
         <v>13548</v>
       </c>
       <c r="B31" t="n">
-        <v>8178.682075</v>
+        <v>8146.056075</v>
       </c>
       <c r="C31" t="n">
         <v>0</v>
       </c>
       <c r="D31" t="n">
-        <v>6542.94566</v>
+        <v>6516.844860000001</v>
       </c>
     </row>
     <row r="32">
@@ -880,13 +880,13 @@
         <v>13554</v>
       </c>
       <c r="B32" t="n">
-        <v>8176.778399999999</v>
+        <v>8144.152425</v>
       </c>
       <c r="C32" t="n">
         <v>0</v>
       </c>
       <c r="D32" t="n">
-        <v>6541.42272</v>
+        <v>6515.321940000001</v>
       </c>
     </row>
     <row r="33">
@@ -894,83 +894,83 @@
         <v>15319</v>
       </c>
       <c r="B33" t="n">
-        <v>8176.7384</v>
+        <v>8144.112425</v>
       </c>
       <c r="C33" t="n">
         <v>0</v>
       </c>
       <c r="D33" t="n">
-        <v>6541.39072</v>
+        <v>6515.289940000001</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>9010</v>
+        <v>16823</v>
       </c>
       <c r="B34" t="n">
-        <v>8176.292425</v>
+        <v>8143.285975000001</v>
       </c>
       <c r="C34" t="n">
         <v>0</v>
       </c>
       <c r="D34" t="n">
-        <v>6541.03394</v>
+        <v>6514.628780000001</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>16823</v>
+        <v>14382</v>
       </c>
       <c r="B35" t="n">
-        <v>8175.911975000001</v>
+        <v>8143.136425000001</v>
       </c>
       <c r="C35" t="n">
         <v>0</v>
       </c>
       <c r="D35" t="n">
-        <v>6540.729580000001</v>
+        <v>6514.509140000001</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>14382</v>
+        <v>17542</v>
       </c>
       <c r="B36" t="n">
-        <v>8175.7624</v>
+        <v>8142.993125000001</v>
       </c>
       <c r="C36" t="n">
         <v>0</v>
       </c>
       <c r="D36" t="n">
-        <v>6540.60992</v>
+        <v>6514.394500000001</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>17542</v>
+        <v>13703</v>
       </c>
       <c r="B37" t="n">
-        <v>8175.6191</v>
+        <v>8142.985575000001</v>
       </c>
       <c r="C37" t="n">
         <v>0</v>
       </c>
       <c r="D37" t="n">
-        <v>6540.49528</v>
+        <v>6514.388460000001</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>13703</v>
+        <v>9010</v>
       </c>
       <c r="B38" t="n">
-        <v>8175.611575000001</v>
+        <v>8142.37505</v>
       </c>
       <c r="C38" t="n">
         <v>0</v>
       </c>
       <c r="D38" t="n">
-        <v>6540.489260000001</v>
+        <v>6513.90004</v>
       </c>
     </row>
     <row r="39">
@@ -978,13 +978,13 @@
         <v>7897</v>
       </c>
       <c r="B39" t="n">
-        <v>8174.038175</v>
+        <v>8140.395675</v>
       </c>
       <c r="C39" t="n">
         <v>0</v>
       </c>
       <c r="D39" t="n">
-        <v>6539.23054</v>
+        <v>6512.31654</v>
       </c>
     </row>
     <row r="40">
@@ -992,13 +992,13 @@
         <v>5642</v>
       </c>
       <c r="B40" t="n">
-        <v>8173.587624999999</v>
+        <v>8139.91165</v>
       </c>
       <c r="C40" t="n">
         <v>0</v>
       </c>
       <c r="D40" t="n">
-        <v>6538.8701</v>
+        <v>6511.92932</v>
       </c>
     </row>
     <row r="41">
@@ -1006,13 +1006,13 @@
         <v>3559</v>
       </c>
       <c r="B41" t="n">
-        <v>8167.9149</v>
+        <v>8135.288925000001</v>
       </c>
       <c r="C41" t="n">
         <v>0</v>
       </c>
       <c r="D41" t="n">
-        <v>6534.331920000001</v>
+        <v>6508.231140000001</v>
       </c>
     </row>
     <row r="42">
@@ -1020,13 +1020,13 @@
         <v>2745</v>
       </c>
       <c r="B42" t="n">
-        <v>8167.9149</v>
+        <v>8135.288925000001</v>
       </c>
       <c r="C42" t="n">
         <v>0</v>
       </c>
       <c r="D42" t="n">
-        <v>6534.331920000001</v>
+        <v>6508.231140000001</v>
       </c>
     </row>
     <row r="43">
@@ -1034,13 +1034,13 @@
         <v>6457</v>
       </c>
       <c r="B43" t="n">
-        <v>8167.5082</v>
+        <v>8134.8822</v>
       </c>
       <c r="C43" t="n">
         <v>0</v>
       </c>
       <c r="D43" t="n">
-        <v>6534.006560000001</v>
+        <v>6507.905760000001</v>
       </c>
     </row>
     <row r="44">
@@ -1048,13 +1048,13 @@
         <v>11722</v>
       </c>
       <c r="B44" t="n">
-        <v>8167.288825</v>
+        <v>8134.662824999999</v>
       </c>
       <c r="C44" t="n">
         <v>0</v>
       </c>
       <c r="D44" t="n">
-        <v>6533.83106</v>
+        <v>6507.73026</v>
       </c>
     </row>
     <row r="45">
@@ -1062,13 +1062,13 @@
         <v>481</v>
       </c>
       <c r="B45" t="n">
-        <v>8166.9995</v>
+        <v>8134.373525</v>
       </c>
       <c r="C45" t="n">
         <v>0</v>
       </c>
       <c r="D45" t="n">
-        <v>6533.5996</v>
+        <v>6507.498820000001</v>
       </c>
     </row>
     <row r="46">
@@ -1076,13 +1076,13 @@
         <v>21249</v>
       </c>
       <c r="B46" t="n">
-        <v>8166.917875000001</v>
+        <v>8134.291875</v>
       </c>
       <c r="C46" t="n">
         <v>0</v>
       </c>
       <c r="D46" t="n">
-        <v>6533.534300000001</v>
+        <v>6507.4335</v>
       </c>
     </row>
     <row r="47">
@@ -1090,13 +1090,13 @@
         <v>20630</v>
       </c>
       <c r="B47" t="n">
-        <v>8166.627</v>
+        <v>8134.001</v>
       </c>
       <c r="C47" t="n">
         <v>0</v>
       </c>
       <c r="D47" t="n">
-        <v>6533.301600000001</v>
+        <v>6507.200800000001</v>
       </c>
     </row>
     <row r="48">
@@ -1104,13 +1104,13 @@
         <v>17724</v>
       </c>
       <c r="B48" t="n">
-        <v>8164.18995</v>
+        <v>8131.56395</v>
       </c>
       <c r="C48" t="n">
         <v>0</v>
       </c>
       <c r="D48" t="n">
-        <v>6531.35196</v>
+        <v>6505.25116</v>
       </c>
     </row>
     <row r="49">
@@ -1118,13 +1118,13 @@
         <v>865</v>
       </c>
       <c r="B49" t="n">
-        <v>8162.663074999999</v>
+        <v>8130.037075</v>
       </c>
       <c r="C49" t="n">
         <v>0</v>
       </c>
       <c r="D49" t="n">
-        <v>6530.13046</v>
+        <v>6504.02966</v>
       </c>
     </row>
     <row r="50">
@@ -1132,13 +1132,13 @@
         <v>17762</v>
       </c>
       <c r="B50" t="n">
-        <v>8160.384975</v>
+        <v>8127.758975000001</v>
       </c>
       <c r="C50" t="n">
         <v>0</v>
       </c>
       <c r="D50" t="n">
-        <v>6528.30798</v>
+        <v>6502.207180000001</v>
       </c>
     </row>
     <row r="51">
@@ -1146,713 +1146,713 @@
         <v>20315</v>
       </c>
       <c r="B51" t="n">
-        <v>8159.542799999999</v>
+        <v>8126.9168</v>
       </c>
       <c r="C51" t="n">
         <v>0</v>
       </c>
       <c r="D51" t="n">
-        <v>6527.634239999999</v>
+        <v>6501.53344</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="n">
-        <v>655</v>
+        <v>30688</v>
       </c>
       <c r="B52" t="n">
         <v>0</v>
       </c>
       <c r="C52" t="n">
-        <v>109.2084465026855</v>
+        <v>0.9079063236713409</v>
       </c>
       <c r="D52" t="n">
-        <v>0.001814742938011801</v>
+        <v>0.1048269495826947</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="n">
-        <v>656</v>
+        <v>30684</v>
       </c>
       <c r="B53" t="n">
         <v>0</v>
       </c>
       <c r="C53" t="n">
-        <v>114.0045280456543</v>
+        <v>0.9088308215141296</v>
       </c>
       <c r="D53" t="n">
-        <v>0.001739061960417805</v>
+        <v>0.1047761790860833</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="n">
-        <v>1633</v>
+        <v>30569</v>
       </c>
       <c r="B54" t="n">
         <v>0</v>
       </c>
       <c r="C54" t="n">
-        <v>114.2370700836182</v>
+        <v>0.9088698029518127</v>
       </c>
       <c r="D54" t="n">
-        <v>0.001735552629504345</v>
+        <v>0.1047740394293663</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="n">
-        <v>1974</v>
+        <v>30576</v>
       </c>
       <c r="B55" t="n">
         <v>0</v>
       </c>
       <c r="C55" t="n">
-        <v>114.6579132080078</v>
+        <v>0.9090279142061869</v>
       </c>
       <c r="D55" t="n">
-        <v>0.001729237494025204</v>
+        <v>0.1047653617381305</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="n">
-        <v>1626</v>
+        <v>30585</v>
       </c>
       <c r="B56" t="n">
         <v>0</v>
       </c>
       <c r="C56" t="n">
-        <v>115.8846416473389</v>
+        <v>0.9092231591542562</v>
       </c>
       <c r="D56" t="n">
-        <v>0.00171108878960706</v>
+        <v>0.1047546480048962</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="n">
-        <v>1631</v>
+        <v>30646</v>
       </c>
       <c r="B57" t="n">
         <v>0</v>
       </c>
       <c r="C57" t="n">
-        <v>116.0007553100586</v>
+        <v>0.9094085693359375</v>
       </c>
       <c r="D57" t="n">
-        <v>0.001709390674188288</v>
+        <v>0.1047444759659568</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="n">
-        <v>1632</v>
+        <v>30598</v>
       </c>
       <c r="B58" t="n">
         <v>0</v>
       </c>
       <c r="C58" t="n">
-        <v>116.4884853363037</v>
+        <v>0.9095043937365214</v>
       </c>
       <c r="D58" t="n">
-        <v>0.001702294479561227</v>
+        <v>0.1047392195880941</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="n">
-        <v>2386</v>
+        <v>30679</v>
       </c>
       <c r="B59" t="n">
         <v>0</v>
       </c>
       <c r="C59" t="n">
-        <v>116.6506271362305</v>
+        <v>0.9095242420832316</v>
       </c>
       <c r="D59" t="n">
-        <v>0.001699948439445336</v>
+        <v>0.1047381308874122</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="n">
-        <v>2435</v>
+        <v>30573</v>
       </c>
       <c r="B60" t="n">
         <v>0</v>
       </c>
       <c r="C60" t="n">
-        <v>116.9381294250488</v>
+        <v>0.9096662998199463</v>
       </c>
       <c r="D60" t="n">
-        <v>0.001695804410117447</v>
+        <v>0.104730339546159</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="n">
-        <v>1692</v>
+        <v>30685</v>
       </c>
       <c r="B61" t="n">
         <v>0</v>
       </c>
       <c r="C61" t="n">
-        <v>116.9381294250488</v>
+        <v>0.9101585745811462</v>
       </c>
       <c r="D61" t="n">
-        <v>0.001695804410117447</v>
+        <v>0.1047033490629726</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="n">
-        <v>1241</v>
+        <v>30640</v>
       </c>
       <c r="B62" t="n">
         <v>0</v>
       </c>
       <c r="C62" t="n">
-        <v>117.1836185455322</v>
+        <v>0.9102955857912699</v>
       </c>
       <c r="D62" t="n">
-        <v>0.001692281912344278</v>
+        <v>0.1046958394751027</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="n">
-        <v>1607</v>
+        <v>30618</v>
       </c>
       <c r="B63" t="n">
         <v>0</v>
       </c>
       <c r="C63" t="n">
-        <v>117.3836936950684</v>
+        <v>0.9103342493375143</v>
       </c>
       <c r="D63" t="n">
-        <v>0.001689421860033851</v>
+        <v>0.1046937205200389</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="n">
-        <v>2193</v>
+        <v>30631</v>
       </c>
       <c r="B64" t="n">
         <v>0</v>
       </c>
       <c r="C64" t="n">
-        <v>117.7448997497559</v>
+        <v>0.9108180105686188</v>
       </c>
       <c r="D64" t="n">
-        <v>0.001684282865381856</v>
+        <v>0.104667215241751</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="n">
-        <v>659</v>
+        <v>30620</v>
       </c>
       <c r="B65" t="n">
         <v>0</v>
       </c>
       <c r="C65" t="n">
-        <v>118.1202259063721</v>
+        <v>0.9108424584070841</v>
       </c>
       <c r="D65" t="n">
-        <v>0.00167897599654654</v>
+        <v>0.1046658761009131</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="n">
-        <v>1629</v>
+        <v>30648</v>
       </c>
       <c r="B66" t="n">
         <v>0</v>
       </c>
       <c r="C66" t="n">
-        <v>118.4642562866211</v>
+        <v>0.9116328756014506</v>
       </c>
       <c r="D66" t="n">
-        <v>0.001674140920612739</v>
+        <v>0.1046225991154681</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="n">
-        <v>2313</v>
+        <v>30604</v>
       </c>
       <c r="B67" t="n">
         <v>0</v>
       </c>
       <c r="C67" t="n">
-        <v>118.5307502746582</v>
+        <v>0.9124908298254013</v>
       </c>
       <c r="D67" t="n">
-        <v>0.001673209609581127</v>
+        <v>0.1045756648246302</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="n">
-        <v>1616</v>
+        <v>30664</v>
       </c>
       <c r="B68" t="n">
         <v>0</v>
       </c>
       <c r="C68" t="n">
-        <v>118.7935085296631</v>
+        <v>0.9127305895090103</v>
       </c>
       <c r="D68" t="n">
-        <v>0.001669539547299229</v>
+        <v>0.1045625563249549</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="n">
-        <v>1628</v>
+        <v>30584</v>
       </c>
       <c r="B69" t="n">
         <v>0</v>
       </c>
       <c r="C69" t="n">
-        <v>118.879114151001</v>
+        <v>0.9127864092588425</v>
       </c>
       <c r="D69" t="n">
-        <v>0.00166834732986163</v>
+        <v>0.1045595049357838</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="n">
-        <v>1943</v>
+        <v>30601</v>
       </c>
       <c r="B70" t="n">
         <v>0</v>
       </c>
       <c r="C70" t="n">
-        <v>119.0222949981689</v>
+        <v>0.9129545241594315</v>
       </c>
       <c r="D70" t="n">
-        <v>0.00166635707143453</v>
+        <v>0.1045503160028761</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="n">
-        <v>1615</v>
+        <v>30614</v>
       </c>
       <c r="B71" t="n">
         <v>0</v>
       </c>
       <c r="C71" t="n">
-        <v>119.2150344848633</v>
+        <v>0.913024365901947</v>
       </c>
       <c r="D71" t="n">
-        <v>0.001663685418858178</v>
+        <v>0.1045464990226116</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="n">
-        <v>1608</v>
+        <v>30691</v>
       </c>
       <c r="B72" t="n">
         <v>0</v>
       </c>
       <c r="C72" t="n">
-        <v>119.6412525177002</v>
+        <v>0.9130336493253708</v>
       </c>
       <c r="D72" t="n">
-        <v>0.00165780772187073</v>
+        <v>0.1045459916873547</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="n">
-        <v>248</v>
+        <v>30668</v>
       </c>
       <c r="B73" t="n">
         <v>0</v>
       </c>
       <c r="C73" t="n">
-        <v>119.9710464477539</v>
+        <v>0.9131515324115753</v>
       </c>
       <c r="D73" t="n">
-        <v>0.00165328816996204</v>
+        <v>0.1045395498535837</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="n">
-        <v>2186</v>
+        <v>30591</v>
       </c>
       <c r="B74" t="n">
         <v>0</v>
       </c>
       <c r="C74" t="n">
-        <v>120.440803527832</v>
+        <v>0.9132043719291687</v>
       </c>
       <c r="D74" t="n">
-        <v>0.001646892923877629</v>
+        <v>0.1045366626453666</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="n">
-        <v>1236</v>
+        <v>30607</v>
       </c>
       <c r="B75" t="n">
         <v>0</v>
       </c>
       <c r="C75" t="n">
-        <v>120.6479911804199</v>
+        <v>0.9132615774869919</v>
       </c>
       <c r="D75" t="n">
-        <v>0.001644087979252973</v>
+        <v>0.1045335370517886</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="n">
-        <v>1630</v>
+        <v>30687</v>
       </c>
       <c r="B76" t="n">
         <v>0</v>
       </c>
       <c r="C76" t="n">
-        <v>120.7178001403809</v>
+        <v>0.9133206158876419</v>
       </c>
       <c r="D76" t="n">
-        <v>0.001643145043447498</v>
+        <v>0.1045303115114424</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="n">
-        <v>206</v>
+        <v>32520</v>
       </c>
       <c r="B77" t="n">
         <v>0</v>
       </c>
       <c r="C77" t="n">
-        <v>120.7469482421875</v>
+        <v>0.9133719603220621</v>
       </c>
       <c r="D77" t="n">
-        <v>0.001642751649118515</v>
+        <v>0.1045275064898179</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="n">
-        <v>1622</v>
+        <v>32872</v>
       </c>
       <c r="B78" t="n">
         <v>0</v>
       </c>
       <c r="C78" t="n">
-        <v>120.889347076416</v>
+        <v>0.9134237468242645</v>
       </c>
       <c r="D78" t="n">
-        <v>0.001640832482879854</v>
+        <v>0.1045246774698719</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="n">
-        <v>1175</v>
+        <v>32860</v>
       </c>
       <c r="B79" t="n">
         <v>0</v>
       </c>
       <c r="C79" t="n">
-        <v>120.9107322692871</v>
+        <v>0.9134385784467062</v>
       </c>
       <c r="D79" t="n">
-        <v>0.001640544653265001</v>
+        <v>0.1045238672685048</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="n">
-        <v>246</v>
+        <v>30649</v>
       </c>
       <c r="B80" t="n">
         <v>0</v>
       </c>
       <c r="C80" t="n">
-        <v>121.2291259765625</v>
+        <v>0.9137069284915924</v>
       </c>
       <c r="D80" t="n">
-        <v>0.001636271211154288</v>
+        <v>0.1045092103824082</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="n">
-        <v>239</v>
+        <v>30645</v>
       </c>
       <c r="B81" t="n">
         <v>0</v>
       </c>
       <c r="C81" t="n">
-        <v>121.4860153198242</v>
+        <v>0.9146003872156143</v>
       </c>
       <c r="D81" t="n">
-        <v>0.001632839467246758</v>
+        <v>0.1044604405887843</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="n">
-        <v>2181</v>
+        <v>30639</v>
       </c>
       <c r="B82" t="n">
         <v>0</v>
       </c>
       <c r="C82" t="n">
-        <v>121.914644241333</v>
+        <v>0.9146513938903809</v>
       </c>
       <c r="D82" t="n">
-        <v>0.001627145416516165</v>
+        <v>0.1044576577429168</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="n">
-        <v>657</v>
+        <v>30638</v>
       </c>
       <c r="B83" t="n">
         <v>0</v>
       </c>
       <c r="C83" t="n">
-        <v>122.028247833252</v>
+        <v>0.9146600514650345</v>
       </c>
       <c r="D83" t="n">
-        <v>0.001625642919592521</v>
+        <v>0.1044571854136543</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="n">
-        <v>1198</v>
+        <v>31864</v>
       </c>
       <c r="B84" t="n">
         <v>0</v>
       </c>
       <c r="C84" t="n">
-        <v>122.0571556091309</v>
+        <v>0.9147107005119324</v>
       </c>
       <c r="D84" t="n">
-        <v>0.001625261034273085</v>
+        <v>0.1044544222511142</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="n">
-        <v>1612</v>
+        <v>30610</v>
       </c>
       <c r="B85" t="n">
         <v>0</v>
       </c>
       <c r="C85" t="n">
-        <v>122.0822982788086</v>
+        <v>0.9147670269012451</v>
       </c>
       <c r="D85" t="n">
-        <v>0.001624929033636956</v>
+        <v>0.1044513495324124</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="n">
-        <v>1174</v>
+        <v>30647</v>
       </c>
       <c r="B86" t="n">
         <v>0</v>
       </c>
       <c r="C86" t="n">
-        <v>122.2451496124268</v>
+        <v>0.9148766547441483</v>
       </c>
       <c r="D86" t="n">
-        <v>0.001622781915790981</v>
+        <v>0.1044453696296812</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="n">
-        <v>215</v>
+        <v>32863</v>
       </c>
       <c r="B87" t="n">
         <v>0</v>
       </c>
       <c r="C87" t="n">
-        <v>122.2786521911621</v>
+        <v>0.9150209426879883</v>
       </c>
       <c r="D87" t="n">
-        <v>0.001622340903677872</v>
+        <v>0.104437500155624</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="n">
-        <v>1029</v>
+        <v>32725</v>
       </c>
       <c r="B88" t="n">
         <v>0</v>
       </c>
       <c r="C88" t="n">
-        <v>122.4564075469971</v>
+        <v>0.9153400957584381</v>
       </c>
       <c r="D88" t="n">
-        <v>0.001620005020183861</v>
+        <v>0.1044200977376834</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="n">
-        <v>224</v>
+        <v>30656</v>
       </c>
       <c r="B89" t="n">
         <v>0</v>
       </c>
       <c r="C89" t="n">
-        <v>122.6510715484619</v>
+        <v>0.9158814698457718</v>
       </c>
       <c r="D89" t="n">
-        <v>0.001617454644714624</v>
+        <v>0.1043905915620657</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="n">
-        <v>658</v>
+        <v>31745</v>
       </c>
       <c r="B90" t="n">
         <v>0</v>
       </c>
       <c r="C90" t="n">
-        <v>122.9752807617188</v>
+        <v>0.9160196185112</v>
       </c>
       <c r="D90" t="n">
-        <v>0.001613224820070391</v>
+        <v>0.1043830648015001</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="n">
-        <v>243</v>
+        <v>32965</v>
       </c>
       <c r="B91" t="n">
         <v>0</v>
       </c>
       <c r="C91" t="n">
-        <v>122.9805431365967</v>
+        <v>0.9161312580108643</v>
       </c>
       <c r="D91" t="n">
-        <v>0.001613156346473238</v>
+        <v>0.1043769831340364</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="n">
-        <v>644</v>
+        <v>32057</v>
       </c>
       <c r="B92" t="n">
         <v>0</v>
       </c>
       <c r="C92" t="n">
-        <v>123.3243179321289</v>
+        <v>0.9161312580108643</v>
       </c>
       <c r="D92" t="n">
-        <v>0.001608695734885784</v>
+        <v>0.1043769831340364</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="n">
-        <v>1623</v>
+        <v>30617</v>
       </c>
       <c r="B93" t="n">
         <v>0</v>
       </c>
       <c r="C93" t="n">
-        <v>123.3813991546631</v>
+        <v>0.9163000583648682</v>
       </c>
       <c r="D93" t="n">
-        <v>0.00160795747080565</v>
+        <v>0.1043677889206219</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="n">
-        <v>1606</v>
+        <v>30983</v>
       </c>
       <c r="B94" t="n">
         <v>0</v>
       </c>
       <c r="C94" t="n">
-        <v>123.4977226257324</v>
+        <v>0.9165835976600647</v>
       </c>
       <c r="D94" t="n">
-        <v>0.001606455088349239</v>
+        <v>0.1043523487544075</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="n">
-        <v>1907</v>
+        <v>32862</v>
       </c>
       <c r="B95" t="n">
         <v>0</v>
       </c>
       <c r="C95" t="n">
-        <v>123.7233867645264</v>
+        <v>0.9167401790618896</v>
       </c>
       <c r="D95" t="n">
-        <v>0.001603548501914829</v>
+        <v>0.1043438240533394</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="n">
-        <v>229</v>
+        <v>30634</v>
       </c>
       <c r="B96" t="n">
         <v>0</v>
       </c>
       <c r="C96" t="n">
-        <v>123.8089752197266</v>
+        <v>0.9169472008943558</v>
       </c>
       <c r="D96" t="n">
-        <v>0.00160244885953033</v>
+        <v>0.1043325553811235</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="n">
-        <v>1617</v>
+        <v>30663</v>
       </c>
       <c r="B97" t="n">
         <v>0</v>
       </c>
       <c r="C97" t="n">
-        <v>123.8158950805664</v>
+        <v>0.9169632196426392</v>
       </c>
       <c r="D97" t="n">
-        <v>0.001602360018897462</v>
+        <v>0.1043316835454381</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="n">
-        <v>1611</v>
+        <v>30612</v>
       </c>
       <c r="B98" t="n">
         <v>0</v>
       </c>
       <c r="C98" t="n">
-        <v>123.8311805725098</v>
+        <v>0.9171411991119385</v>
       </c>
       <c r="D98" t="n">
-        <v>0.001602163811018574</v>
+        <v>0.1043219978229274</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="n">
-        <v>1145</v>
+        <v>30654</v>
       </c>
       <c r="B99" t="n">
         <v>0</v>
       </c>
       <c r="C99" t="n">
-        <v>123.8582515716553</v>
+        <v>0.9172030538320541</v>
       </c>
       <c r="D99" t="n">
-        <v>0.001601816439702597</v>
+        <v>0.104318632082421</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="n">
-        <v>1625</v>
+        <v>30661</v>
       </c>
       <c r="B100" t="n">
         <v>0</v>
       </c>
       <c r="C100" t="n">
-        <v>123.9412727355957</v>
+        <v>0.9177192896604538</v>
       </c>
       <c r="D100" t="n">
-        <v>0.001600752062316875</v>
+        <v>0.1042905502793433</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="n">
-        <v>649</v>
+        <v>31281</v>
       </c>
       <c r="B101" t="n">
         <v>0</v>
       </c>
       <c r="C101" t="n">
-        <v>124.1615924835205</v>
+        <v>0.9177635312080383</v>
       </c>
       <c r="D101" t="n">
-        <v>0.001597934286640953</v>
+        <v>0.10428814436471</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added run_all file to run everything with 1 script
</commit_message>
<xml_diff>
--- a/output/scores.xlsx
+++ b/output/scores.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D101"/>
+  <dimension ref="A1:D51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -474,13 +474,13 @@
         <v>20753</v>
       </c>
       <c r="B3" t="n">
-        <v>8237.045725</v>
+        <v>8236.766274999998</v>
       </c>
       <c r="C3" t="n">
         <v>0</v>
       </c>
       <c r="D3" t="n">
-        <v>6589.63658</v>
+        <v>6589.413019999999</v>
       </c>
     </row>
     <row r="4">
@@ -488,13 +488,13 @@
         <v>10216</v>
       </c>
       <c r="B4" t="n">
-        <v>8228.214875</v>
+        <v>8227.9354</v>
       </c>
       <c r="C4" t="n">
         <v>0</v>
       </c>
       <c r="D4" t="n">
-        <v>6582.5719</v>
+        <v>6582.348320000001</v>
       </c>
     </row>
     <row r="5">
@@ -502,13 +502,13 @@
         <v>19359</v>
       </c>
       <c r="B5" t="n">
-        <v>8219.745825</v>
+        <v>8219.466375</v>
       </c>
       <c r="C5" t="n">
         <v>0</v>
       </c>
       <c r="D5" t="n">
-        <v>6575.79666</v>
+        <v>6575.573100000001</v>
       </c>
     </row>
     <row r="6">
@@ -516,13 +516,13 @@
         <v>27008</v>
       </c>
       <c r="B6" t="n">
-        <v>8209.766650000001</v>
+        <v>8209.4872</v>
       </c>
       <c r="C6" t="n">
         <v>0</v>
       </c>
       <c r="D6" t="n">
-        <v>6567.813320000001</v>
+        <v>6567.58976</v>
       </c>
     </row>
     <row r="7">
@@ -530,13 +530,13 @@
         <v>27734</v>
       </c>
       <c r="B7" t="n">
-        <v>8203.941075000001</v>
+        <v>8203.661599999999</v>
       </c>
       <c r="C7" t="n">
         <v>0</v>
       </c>
       <c r="D7" t="n">
-        <v>6563.152860000001</v>
+        <v>6562.92928</v>
       </c>
     </row>
     <row r="8">
@@ -544,13 +544,13 @@
         <v>21625</v>
       </c>
       <c r="B8" t="n">
-        <v>8194.030774999999</v>
+        <v>8193.7513</v>
       </c>
       <c r="C8" t="n">
         <v>0</v>
       </c>
       <c r="D8" t="n">
-        <v>6555.22462</v>
+        <v>6555.00104</v>
       </c>
     </row>
     <row r="9">
@@ -558,13 +558,13 @@
         <v>957</v>
       </c>
       <c r="B9" t="n">
-        <v>8191.016825</v>
+        <v>8190.737375</v>
       </c>
       <c r="C9" t="n">
         <v>0</v>
       </c>
       <c r="D9" t="n">
-        <v>6552.81346</v>
+        <v>6552.5899</v>
       </c>
     </row>
     <row r="10">
@@ -572,13 +572,13 @@
         <v>9075</v>
       </c>
       <c r="B10" t="n">
-        <v>8184.670525</v>
+        <v>8184.391075</v>
       </c>
       <c r="C10" t="n">
         <v>0</v>
       </c>
       <c r="D10" t="n">
-        <v>6547.73642</v>
+        <v>6547.51286</v>
       </c>
     </row>
     <row r="11">
@@ -586,13 +586,13 @@
         <v>12511</v>
       </c>
       <c r="B11" t="n">
-        <v>8181.183225</v>
+        <v>8180.90375</v>
       </c>
       <c r="C11" t="n">
         <v>0</v>
       </c>
       <c r="D11" t="n">
-        <v>6544.94658</v>
+        <v>6544.723000000001</v>
       </c>
     </row>
     <row r="12">
@@ -600,13 +600,13 @@
         <v>5329</v>
       </c>
       <c r="B12" t="n">
-        <v>8173.53915</v>
+        <v>8173.2597</v>
       </c>
       <c r="C12" t="n">
         <v>0</v>
       </c>
       <c r="D12" t="n">
-        <v>6538.83132</v>
+        <v>6538.60776</v>
       </c>
     </row>
     <row r="13">
@@ -614,13 +614,13 @@
         <v>3045</v>
       </c>
       <c r="B13" t="n">
-        <v>8170.843075000001</v>
+        <v>8170.563599999999</v>
       </c>
       <c r="C13" t="n">
         <v>0</v>
       </c>
       <c r="D13" t="n">
-        <v>6536.674460000001</v>
+        <v>6536.45088</v>
       </c>
     </row>
     <row r="14">
@@ -628,13 +628,13 @@
         <v>8057</v>
       </c>
       <c r="B14" t="n">
-        <v>8169.407525</v>
+        <v>8169.128075</v>
       </c>
       <c r="C14" t="n">
         <v>0</v>
       </c>
       <c r="D14" t="n">
-        <v>6535.52602</v>
+        <v>6535.30246</v>
       </c>
     </row>
     <row r="15">
@@ -642,13 +642,13 @@
         <v>2469</v>
       </c>
       <c r="B15" t="n">
-        <v>8167.7606</v>
+        <v>8167.481125</v>
       </c>
       <c r="C15" t="n">
         <v>0</v>
       </c>
       <c r="D15" t="n">
-        <v>6534.20848</v>
+        <v>6533.9849</v>
       </c>
     </row>
     <row r="16">
@@ -656,13 +656,13 @@
         <v>7197</v>
       </c>
       <c r="B16" t="n">
-        <v>8167.499725</v>
+        <v>8167.220275</v>
       </c>
       <c r="C16" t="n">
         <v>0</v>
       </c>
       <c r="D16" t="n">
-        <v>6533.99978</v>
+        <v>6533.77622</v>
       </c>
     </row>
     <row r="17">
@@ -670,13 +670,13 @@
         <v>9205</v>
       </c>
       <c r="B17" t="n">
-        <v>8166.634775</v>
+        <v>8166.3553</v>
       </c>
       <c r="C17" t="n">
         <v>0</v>
       </c>
       <c r="D17" t="n">
-        <v>6533.307820000001</v>
+        <v>6533.08424</v>
       </c>
     </row>
     <row r="18">
@@ -684,13 +684,13 @@
         <v>24463</v>
       </c>
       <c r="B18" t="n">
-        <v>8166.344875000001</v>
+        <v>8166.065399999999</v>
       </c>
       <c r="C18" t="n">
         <v>0</v>
       </c>
       <c r="D18" t="n">
-        <v>6533.075900000001</v>
+        <v>6532.85232</v>
       </c>
     </row>
     <row r="19">
@@ -698,13 +698,13 @@
         <v>7553</v>
       </c>
       <c r="B19" t="n">
-        <v>8163.329075</v>
+        <v>8163.0496</v>
       </c>
       <c r="C19" t="n">
         <v>0</v>
       </c>
       <c r="D19" t="n">
-        <v>6530.66326</v>
+        <v>6530.43968</v>
       </c>
     </row>
     <row r="20">
@@ -712,13 +712,13 @@
         <v>1770</v>
       </c>
       <c r="B20" t="n">
-        <v>8162.187249999999</v>
+        <v>8161.907799999999</v>
       </c>
       <c r="C20" t="n">
         <v>0</v>
       </c>
       <c r="D20" t="n">
-        <v>6529.7498</v>
+        <v>6529.526239999999</v>
       </c>
     </row>
     <row r="21">
@@ -726,13 +726,13 @@
         <v>29143</v>
       </c>
       <c r="B21" t="n">
-        <v>8161.957775</v>
+        <v>8161.6783</v>
       </c>
       <c r="C21" t="n">
         <v>0</v>
       </c>
       <c r="D21" t="n">
-        <v>6529.566220000001</v>
+        <v>6529.34264</v>
       </c>
     </row>
     <row r="22">
@@ -740,13 +740,13 @@
         <v>30543</v>
       </c>
       <c r="B22" t="n">
-        <v>8161.957775</v>
+        <v>8161.6783</v>
       </c>
       <c r="C22" t="n">
         <v>0</v>
       </c>
       <c r="D22" t="n">
-        <v>6529.566220000001</v>
+        <v>6529.34264</v>
       </c>
     </row>
     <row r="23">
@@ -754,13 +754,13 @@
         <v>12264</v>
       </c>
       <c r="B23" t="n">
-        <v>8159.1873</v>
+        <v>8158.907825</v>
       </c>
       <c r="C23" t="n">
         <v>0</v>
       </c>
       <c r="D23" t="n">
-        <v>6527.34984</v>
+        <v>6527.126260000001</v>
       </c>
     </row>
     <row r="24">
@@ -768,55 +768,55 @@
         <v>11990</v>
       </c>
       <c r="B24" t="n">
-        <v>8155.97275</v>
+        <v>8156.779025000001</v>
       </c>
       <c r="C24" t="n">
         <v>0</v>
       </c>
       <c r="D24" t="n">
-        <v>6524.778200000001</v>
+        <v>6525.423220000001</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>12696</v>
+        <v>4340</v>
       </c>
       <c r="B25" t="n">
-        <v>8155.404474999999</v>
+        <v>8156.149649999999</v>
       </c>
       <c r="C25" t="n">
         <v>0</v>
       </c>
       <c r="D25" t="n">
-        <v>6524.32358</v>
+        <v>6524.91972</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>4340</v>
+        <v>9208</v>
       </c>
       <c r="B26" t="n">
-        <v>8155.3434</v>
+        <v>8155.944750000001</v>
       </c>
       <c r="C26" t="n">
         <v>0</v>
       </c>
       <c r="D26" t="n">
-        <v>6524.27472</v>
+        <v>6524.755800000001</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>9208</v>
+        <v>12696</v>
       </c>
       <c r="B27" t="n">
-        <v>8155.138499999999</v>
+        <v>8155.125</v>
       </c>
       <c r="C27" t="n">
         <v>0</v>
       </c>
       <c r="D27" t="n">
-        <v>6524.110799999999</v>
+        <v>6524.1</v>
       </c>
     </row>
     <row r="28">
@@ -824,41 +824,41 @@
         <v>7535</v>
       </c>
       <c r="B28" t="n">
-        <v>8154.069175000001</v>
+        <v>8153.789699999999</v>
       </c>
       <c r="C28" t="n">
         <v>0</v>
       </c>
       <c r="D28" t="n">
-        <v>6523.255340000001</v>
+        <v>6523.03176</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>29063</v>
+        <v>25668</v>
       </c>
       <c r="B29" t="n">
-        <v>8147.679225</v>
+        <v>8148.133124999999</v>
       </c>
       <c r="C29" t="n">
         <v>0</v>
       </c>
       <c r="D29" t="n">
-        <v>6518.14338</v>
+        <v>6518.5065</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>25668</v>
+        <v>29063</v>
       </c>
       <c r="B30" t="n">
-        <v>8147.32685</v>
+        <v>8147.39975</v>
       </c>
       <c r="C30" t="n">
         <v>0</v>
       </c>
       <c r="D30" t="n">
-        <v>6517.86148</v>
+        <v>6517.919800000001</v>
       </c>
     </row>
     <row r="31">
@@ -866,13 +866,13 @@
         <v>13548</v>
       </c>
       <c r="B31" t="n">
-        <v>8146.056075</v>
+        <v>8145.776599999999</v>
       </c>
       <c r="C31" t="n">
         <v>0</v>
       </c>
       <c r="D31" t="n">
-        <v>6516.844860000001</v>
+        <v>6516.621279999999</v>
       </c>
     </row>
     <row r="32">
@@ -880,13 +880,13 @@
         <v>13554</v>
       </c>
       <c r="B32" t="n">
-        <v>8144.152425</v>
+        <v>8143.872975</v>
       </c>
       <c r="C32" t="n">
         <v>0</v>
       </c>
       <c r="D32" t="n">
-        <v>6515.321940000001</v>
+        <v>6515.09838</v>
       </c>
     </row>
     <row r="33">
@@ -894,13 +894,13 @@
         <v>15319</v>
       </c>
       <c r="B33" t="n">
-        <v>8144.112425</v>
+        <v>8143.832975</v>
       </c>
       <c r="C33" t="n">
         <v>0</v>
       </c>
       <c r="D33" t="n">
-        <v>6515.289940000001</v>
+        <v>6515.06638</v>
       </c>
     </row>
     <row r="34">
@@ -908,13 +908,13 @@
         <v>16823</v>
       </c>
       <c r="B34" t="n">
-        <v>8143.285975000001</v>
+        <v>8143.0065</v>
       </c>
       <c r="C34" t="n">
         <v>0</v>
       </c>
       <c r="D34" t="n">
-        <v>6514.628780000001</v>
+        <v>6514.405200000001</v>
       </c>
     </row>
     <row r="35">
@@ -922,13 +922,13 @@
         <v>14382</v>
       </c>
       <c r="B35" t="n">
-        <v>8143.136425000001</v>
+        <v>8142.856974999999</v>
       </c>
       <c r="C35" t="n">
         <v>0</v>
       </c>
       <c r="D35" t="n">
-        <v>6514.509140000001</v>
+        <v>6514.28558</v>
       </c>
     </row>
     <row r="36">
@@ -936,13 +936,13 @@
         <v>17542</v>
       </c>
       <c r="B36" t="n">
-        <v>8142.993125000001</v>
+        <v>8142.713675000001</v>
       </c>
       <c r="C36" t="n">
         <v>0</v>
       </c>
       <c r="D36" t="n">
-        <v>6514.394500000001</v>
+        <v>6514.170940000001</v>
       </c>
     </row>
     <row r="37">
@@ -950,13 +950,13 @@
         <v>13703</v>
       </c>
       <c r="B37" t="n">
-        <v>8142.985575000001</v>
+        <v>8142.7061</v>
       </c>
       <c r="C37" t="n">
         <v>0</v>
       </c>
       <c r="D37" t="n">
-        <v>6514.388460000001</v>
+        <v>6514.16488</v>
       </c>
     </row>
     <row r="38">
@@ -964,13 +964,13 @@
         <v>9010</v>
       </c>
       <c r="B38" t="n">
-        <v>8142.37505</v>
+        <v>8142.095574999999</v>
       </c>
       <c r="C38" t="n">
         <v>0</v>
       </c>
       <c r="D38" t="n">
-        <v>6513.90004</v>
+        <v>6513.67646</v>
       </c>
     </row>
     <row r="39">
@@ -978,13 +978,13 @@
         <v>7897</v>
       </c>
       <c r="B39" t="n">
-        <v>8140.395675</v>
+        <v>8141.1327</v>
       </c>
       <c r="C39" t="n">
         <v>0</v>
       </c>
       <c r="D39" t="n">
-        <v>6512.31654</v>
+        <v>6512.90616</v>
       </c>
     </row>
     <row r="40">
@@ -992,41 +992,41 @@
         <v>5642</v>
       </c>
       <c r="B40" t="n">
-        <v>8139.91165</v>
+        <v>8140.682150000001</v>
       </c>
       <c r="C40" t="n">
         <v>0</v>
       </c>
       <c r="D40" t="n">
-        <v>6511.92932</v>
+        <v>6512.545720000001</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="n">
-        <v>3559</v>
+        <v>2745</v>
       </c>
       <c r="B41" t="n">
-        <v>8135.288925000001</v>
+        <v>8135.00945</v>
       </c>
       <c r="C41" t="n">
         <v>0</v>
       </c>
       <c r="D41" t="n">
-        <v>6508.231140000001</v>
+        <v>6508.00756</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="n">
-        <v>2745</v>
+        <v>3559</v>
       </c>
       <c r="B42" t="n">
-        <v>8135.288925000001</v>
+        <v>8135.00945</v>
       </c>
       <c r="C42" t="n">
         <v>0</v>
       </c>
       <c r="D42" t="n">
-        <v>6508.231140000001</v>
+        <v>6508.00756</v>
       </c>
     </row>
     <row r="43">
@@ -1034,13 +1034,13 @@
         <v>6457</v>
       </c>
       <c r="B43" t="n">
-        <v>8134.8822</v>
+        <v>8134.602725</v>
       </c>
       <c r="C43" t="n">
         <v>0</v>
       </c>
       <c r="D43" t="n">
-        <v>6507.905760000001</v>
+        <v>6507.68218</v>
       </c>
     </row>
     <row r="44">
@@ -1048,13 +1048,13 @@
         <v>11722</v>
       </c>
       <c r="B44" t="n">
-        <v>8134.662824999999</v>
+        <v>8134.383375</v>
       </c>
       <c r="C44" t="n">
         <v>0</v>
       </c>
       <c r="D44" t="n">
-        <v>6507.73026</v>
+        <v>6507.506700000001</v>
       </c>
     </row>
     <row r="45">
@@ -1062,13 +1062,13 @@
         <v>481</v>
       </c>
       <c r="B45" t="n">
-        <v>8134.373525</v>
+        <v>8134.094075</v>
       </c>
       <c r="C45" t="n">
         <v>0</v>
       </c>
       <c r="D45" t="n">
-        <v>6507.498820000001</v>
+        <v>6507.27526</v>
       </c>
     </row>
     <row r="46">
@@ -1076,13 +1076,13 @@
         <v>21249</v>
       </c>
       <c r="B46" t="n">
-        <v>8134.291875</v>
+        <v>8134.0124</v>
       </c>
       <c r="C46" t="n">
         <v>0</v>
       </c>
       <c r="D46" t="n">
-        <v>6507.4335</v>
+        <v>6507.20992</v>
       </c>
     </row>
     <row r="47">
@@ -1090,13 +1090,13 @@
         <v>20630</v>
       </c>
       <c r="B47" t="n">
-        <v>8134.001</v>
+        <v>8133.721525000001</v>
       </c>
       <c r="C47" t="n">
         <v>0</v>
       </c>
       <c r="D47" t="n">
-        <v>6507.200800000001</v>
+        <v>6506.977220000001</v>
       </c>
     </row>
     <row r="48">
@@ -1104,13 +1104,13 @@
         <v>17724</v>
       </c>
       <c r="B48" t="n">
-        <v>8131.56395</v>
+        <v>8131.2845</v>
       </c>
       <c r="C48" t="n">
         <v>0</v>
       </c>
       <c r="D48" t="n">
-        <v>6505.25116</v>
+        <v>6505.0276</v>
       </c>
     </row>
     <row r="49">
@@ -1118,13 +1118,13 @@
         <v>865</v>
       </c>
       <c r="B49" t="n">
-        <v>8130.037075</v>
+        <v>8129.757599999999</v>
       </c>
       <c r="C49" t="n">
         <v>0</v>
       </c>
       <c r="D49" t="n">
-        <v>6504.02966</v>
+        <v>6503.806079999999</v>
       </c>
     </row>
     <row r="50">
@@ -1132,13 +1132,13 @@
         <v>17762</v>
       </c>
       <c r="B50" t="n">
-        <v>8127.758975000001</v>
+        <v>8127.479499999999</v>
       </c>
       <c r="C50" t="n">
         <v>0</v>
       </c>
       <c r="D50" t="n">
-        <v>6502.207180000001</v>
+        <v>6501.9836</v>
       </c>
     </row>
     <row r="51">
@@ -1146,713 +1146,13 @@
         <v>20315</v>
       </c>
       <c r="B51" t="n">
-        <v>8126.9168</v>
+        <v>8126.637325</v>
       </c>
       <c r="C51" t="n">
         <v>0</v>
       </c>
       <c r="D51" t="n">
-        <v>6501.53344</v>
-      </c>
-    </row>
-    <row r="52">
-      <c r="A52" t="n">
-        <v>30688</v>
-      </c>
-      <c r="B52" t="n">
-        <v>0</v>
-      </c>
-      <c r="C52" t="n">
-        <v>0.9079063236713409</v>
-      </c>
-      <c r="D52" t="n">
-        <v>0.1048269495826947</v>
-      </c>
-    </row>
-    <row r="53">
-      <c r="A53" t="n">
-        <v>30684</v>
-      </c>
-      <c r="B53" t="n">
-        <v>0</v>
-      </c>
-      <c r="C53" t="n">
-        <v>0.9088308215141296</v>
-      </c>
-      <c r="D53" t="n">
-        <v>0.1047761790860833</v>
-      </c>
-    </row>
-    <row r="54">
-      <c r="A54" t="n">
-        <v>30569</v>
-      </c>
-      <c r="B54" t="n">
-        <v>0</v>
-      </c>
-      <c r="C54" t="n">
-        <v>0.9088698029518127</v>
-      </c>
-      <c r="D54" t="n">
-        <v>0.1047740394293663</v>
-      </c>
-    </row>
-    <row r="55">
-      <c r="A55" t="n">
-        <v>30576</v>
-      </c>
-      <c r="B55" t="n">
-        <v>0</v>
-      </c>
-      <c r="C55" t="n">
-        <v>0.9090279142061869</v>
-      </c>
-      <c r="D55" t="n">
-        <v>0.1047653617381305</v>
-      </c>
-    </row>
-    <row r="56">
-      <c r="A56" t="n">
-        <v>30585</v>
-      </c>
-      <c r="B56" t="n">
-        <v>0</v>
-      </c>
-      <c r="C56" t="n">
-        <v>0.9092231591542562</v>
-      </c>
-      <c r="D56" t="n">
-        <v>0.1047546480048962</v>
-      </c>
-    </row>
-    <row r="57">
-      <c r="A57" t="n">
-        <v>30646</v>
-      </c>
-      <c r="B57" t="n">
-        <v>0</v>
-      </c>
-      <c r="C57" t="n">
-        <v>0.9094085693359375</v>
-      </c>
-      <c r="D57" t="n">
-        <v>0.1047444759659568</v>
-      </c>
-    </row>
-    <row r="58">
-      <c r="A58" t="n">
-        <v>30598</v>
-      </c>
-      <c r="B58" t="n">
-        <v>0</v>
-      </c>
-      <c r="C58" t="n">
-        <v>0.9095043937365214</v>
-      </c>
-      <c r="D58" t="n">
-        <v>0.1047392195880941</v>
-      </c>
-    </row>
-    <row r="59">
-      <c r="A59" t="n">
-        <v>30679</v>
-      </c>
-      <c r="B59" t="n">
-        <v>0</v>
-      </c>
-      <c r="C59" t="n">
-        <v>0.9095242420832316</v>
-      </c>
-      <c r="D59" t="n">
-        <v>0.1047381308874122</v>
-      </c>
-    </row>
-    <row r="60">
-      <c r="A60" t="n">
-        <v>30573</v>
-      </c>
-      <c r="B60" t="n">
-        <v>0</v>
-      </c>
-      <c r="C60" t="n">
-        <v>0.9096662998199463</v>
-      </c>
-      <c r="D60" t="n">
-        <v>0.104730339546159</v>
-      </c>
-    </row>
-    <row r="61">
-      <c r="A61" t="n">
-        <v>30685</v>
-      </c>
-      <c r="B61" t="n">
-        <v>0</v>
-      </c>
-      <c r="C61" t="n">
-        <v>0.9101585745811462</v>
-      </c>
-      <c r="D61" t="n">
-        <v>0.1047033490629726</v>
-      </c>
-    </row>
-    <row r="62">
-      <c r="A62" t="n">
-        <v>30640</v>
-      </c>
-      <c r="B62" t="n">
-        <v>0</v>
-      </c>
-      <c r="C62" t="n">
-        <v>0.9102955857912699</v>
-      </c>
-      <c r="D62" t="n">
-        <v>0.1046958394751027</v>
-      </c>
-    </row>
-    <row r="63">
-      <c r="A63" t="n">
-        <v>30618</v>
-      </c>
-      <c r="B63" t="n">
-        <v>0</v>
-      </c>
-      <c r="C63" t="n">
-        <v>0.9103342493375143</v>
-      </c>
-      <c r="D63" t="n">
-        <v>0.1046937205200389</v>
-      </c>
-    </row>
-    <row r="64">
-      <c r="A64" t="n">
-        <v>30631</v>
-      </c>
-      <c r="B64" t="n">
-        <v>0</v>
-      </c>
-      <c r="C64" t="n">
-        <v>0.9108180105686188</v>
-      </c>
-      <c r="D64" t="n">
-        <v>0.104667215241751</v>
-      </c>
-    </row>
-    <row r="65">
-      <c r="A65" t="n">
-        <v>30620</v>
-      </c>
-      <c r="B65" t="n">
-        <v>0</v>
-      </c>
-      <c r="C65" t="n">
-        <v>0.9108424584070841</v>
-      </c>
-      <c r="D65" t="n">
-        <v>0.1046658761009131</v>
-      </c>
-    </row>
-    <row r="66">
-      <c r="A66" t="n">
-        <v>30648</v>
-      </c>
-      <c r="B66" t="n">
-        <v>0</v>
-      </c>
-      <c r="C66" t="n">
-        <v>0.9116328756014506</v>
-      </c>
-      <c r="D66" t="n">
-        <v>0.1046225991154681</v>
-      </c>
-    </row>
-    <row r="67">
-      <c r="A67" t="n">
-        <v>30604</v>
-      </c>
-      <c r="B67" t="n">
-        <v>0</v>
-      </c>
-      <c r="C67" t="n">
-        <v>0.9124908298254013</v>
-      </c>
-      <c r="D67" t="n">
-        <v>0.1045756648246302</v>
-      </c>
-    </row>
-    <row r="68">
-      <c r="A68" t="n">
-        <v>30664</v>
-      </c>
-      <c r="B68" t="n">
-        <v>0</v>
-      </c>
-      <c r="C68" t="n">
-        <v>0.9127305895090103</v>
-      </c>
-      <c r="D68" t="n">
-        <v>0.1045625563249549</v>
-      </c>
-    </row>
-    <row r="69">
-      <c r="A69" t="n">
-        <v>30584</v>
-      </c>
-      <c r="B69" t="n">
-        <v>0</v>
-      </c>
-      <c r="C69" t="n">
-        <v>0.9127864092588425</v>
-      </c>
-      <c r="D69" t="n">
-        <v>0.1045595049357838</v>
-      </c>
-    </row>
-    <row r="70">
-      <c r="A70" t="n">
-        <v>30601</v>
-      </c>
-      <c r="B70" t="n">
-        <v>0</v>
-      </c>
-      <c r="C70" t="n">
-        <v>0.9129545241594315</v>
-      </c>
-      <c r="D70" t="n">
-        <v>0.1045503160028761</v>
-      </c>
-    </row>
-    <row r="71">
-      <c r="A71" t="n">
-        <v>30614</v>
-      </c>
-      <c r="B71" t="n">
-        <v>0</v>
-      </c>
-      <c r="C71" t="n">
-        <v>0.913024365901947</v>
-      </c>
-      <c r="D71" t="n">
-        <v>0.1045464990226116</v>
-      </c>
-    </row>
-    <row r="72">
-      <c r="A72" t="n">
-        <v>30691</v>
-      </c>
-      <c r="B72" t="n">
-        <v>0</v>
-      </c>
-      <c r="C72" t="n">
-        <v>0.9130336493253708</v>
-      </c>
-      <c r="D72" t="n">
-        <v>0.1045459916873547</v>
-      </c>
-    </row>
-    <row r="73">
-      <c r="A73" t="n">
-        <v>30668</v>
-      </c>
-      <c r="B73" t="n">
-        <v>0</v>
-      </c>
-      <c r="C73" t="n">
-        <v>0.9131515324115753</v>
-      </c>
-      <c r="D73" t="n">
-        <v>0.1045395498535837</v>
-      </c>
-    </row>
-    <row r="74">
-      <c r="A74" t="n">
-        <v>30591</v>
-      </c>
-      <c r="B74" t="n">
-        <v>0</v>
-      </c>
-      <c r="C74" t="n">
-        <v>0.9132043719291687</v>
-      </c>
-      <c r="D74" t="n">
-        <v>0.1045366626453666</v>
-      </c>
-    </row>
-    <row r="75">
-      <c r="A75" t="n">
-        <v>30607</v>
-      </c>
-      <c r="B75" t="n">
-        <v>0</v>
-      </c>
-      <c r="C75" t="n">
-        <v>0.9132615774869919</v>
-      </c>
-      <c r="D75" t="n">
-        <v>0.1045335370517886</v>
-      </c>
-    </row>
-    <row r="76">
-      <c r="A76" t="n">
-        <v>30687</v>
-      </c>
-      <c r="B76" t="n">
-        <v>0</v>
-      </c>
-      <c r="C76" t="n">
-        <v>0.9133206158876419</v>
-      </c>
-      <c r="D76" t="n">
-        <v>0.1045303115114424</v>
-      </c>
-    </row>
-    <row r="77">
-      <c r="A77" t="n">
-        <v>32520</v>
-      </c>
-      <c r="B77" t="n">
-        <v>0</v>
-      </c>
-      <c r="C77" t="n">
-        <v>0.9133719603220621</v>
-      </c>
-      <c r="D77" t="n">
-        <v>0.1045275064898179</v>
-      </c>
-    </row>
-    <row r="78">
-      <c r="A78" t="n">
-        <v>32872</v>
-      </c>
-      <c r="B78" t="n">
-        <v>0</v>
-      </c>
-      <c r="C78" t="n">
-        <v>0.9134237468242645</v>
-      </c>
-      <c r="D78" t="n">
-        <v>0.1045246774698719</v>
-      </c>
-    </row>
-    <row r="79">
-      <c r="A79" t="n">
-        <v>32860</v>
-      </c>
-      <c r="B79" t="n">
-        <v>0</v>
-      </c>
-      <c r="C79" t="n">
-        <v>0.9134385784467062</v>
-      </c>
-      <c r="D79" t="n">
-        <v>0.1045238672685048</v>
-      </c>
-    </row>
-    <row r="80">
-      <c r="A80" t="n">
-        <v>30649</v>
-      </c>
-      <c r="B80" t="n">
-        <v>0</v>
-      </c>
-      <c r="C80" t="n">
-        <v>0.9137069284915924</v>
-      </c>
-      <c r="D80" t="n">
-        <v>0.1045092103824082</v>
-      </c>
-    </row>
-    <row r="81">
-      <c r="A81" t="n">
-        <v>30645</v>
-      </c>
-      <c r="B81" t="n">
-        <v>0</v>
-      </c>
-      <c r="C81" t="n">
-        <v>0.9146003872156143</v>
-      </c>
-      <c r="D81" t="n">
-        <v>0.1044604405887843</v>
-      </c>
-    </row>
-    <row r="82">
-      <c r="A82" t="n">
-        <v>30639</v>
-      </c>
-      <c r="B82" t="n">
-        <v>0</v>
-      </c>
-      <c r="C82" t="n">
-        <v>0.9146513938903809</v>
-      </c>
-      <c r="D82" t="n">
-        <v>0.1044576577429168</v>
-      </c>
-    </row>
-    <row r="83">
-      <c r="A83" t="n">
-        <v>30638</v>
-      </c>
-      <c r="B83" t="n">
-        <v>0</v>
-      </c>
-      <c r="C83" t="n">
-        <v>0.9146600514650345</v>
-      </c>
-      <c r="D83" t="n">
-        <v>0.1044571854136543</v>
-      </c>
-    </row>
-    <row r="84">
-      <c r="A84" t="n">
-        <v>31864</v>
-      </c>
-      <c r="B84" t="n">
-        <v>0</v>
-      </c>
-      <c r="C84" t="n">
-        <v>0.9147107005119324</v>
-      </c>
-      <c r="D84" t="n">
-        <v>0.1044544222511142</v>
-      </c>
-    </row>
-    <row r="85">
-      <c r="A85" t="n">
-        <v>30610</v>
-      </c>
-      <c r="B85" t="n">
-        <v>0</v>
-      </c>
-      <c r="C85" t="n">
-        <v>0.9147670269012451</v>
-      </c>
-      <c r="D85" t="n">
-        <v>0.1044513495324124</v>
-      </c>
-    </row>
-    <row r="86">
-      <c r="A86" t="n">
-        <v>30647</v>
-      </c>
-      <c r="B86" t="n">
-        <v>0</v>
-      </c>
-      <c r="C86" t="n">
-        <v>0.9148766547441483</v>
-      </c>
-      <c r="D86" t="n">
-        <v>0.1044453696296812</v>
-      </c>
-    </row>
-    <row r="87">
-      <c r="A87" t="n">
-        <v>32863</v>
-      </c>
-      <c r="B87" t="n">
-        <v>0</v>
-      </c>
-      <c r="C87" t="n">
-        <v>0.9150209426879883</v>
-      </c>
-      <c r="D87" t="n">
-        <v>0.104437500155624</v>
-      </c>
-    </row>
-    <row r="88">
-      <c r="A88" t="n">
-        <v>32725</v>
-      </c>
-      <c r="B88" t="n">
-        <v>0</v>
-      </c>
-      <c r="C88" t="n">
-        <v>0.9153400957584381</v>
-      </c>
-      <c r="D88" t="n">
-        <v>0.1044200977376834</v>
-      </c>
-    </row>
-    <row r="89">
-      <c r="A89" t="n">
-        <v>30656</v>
-      </c>
-      <c r="B89" t="n">
-        <v>0</v>
-      </c>
-      <c r="C89" t="n">
-        <v>0.9158814698457718</v>
-      </c>
-      <c r="D89" t="n">
-        <v>0.1043905915620657</v>
-      </c>
-    </row>
-    <row r="90">
-      <c r="A90" t="n">
-        <v>31745</v>
-      </c>
-      <c r="B90" t="n">
-        <v>0</v>
-      </c>
-      <c r="C90" t="n">
-        <v>0.9160196185112</v>
-      </c>
-      <c r="D90" t="n">
-        <v>0.1043830648015001</v>
-      </c>
-    </row>
-    <row r="91">
-      <c r="A91" t="n">
-        <v>32965</v>
-      </c>
-      <c r="B91" t="n">
-        <v>0</v>
-      </c>
-      <c r="C91" t="n">
-        <v>0.9161312580108643</v>
-      </c>
-      <c r="D91" t="n">
-        <v>0.1043769831340364</v>
-      </c>
-    </row>
-    <row r="92">
-      <c r="A92" t="n">
-        <v>32057</v>
-      </c>
-      <c r="B92" t="n">
-        <v>0</v>
-      </c>
-      <c r="C92" t="n">
-        <v>0.9161312580108643</v>
-      </c>
-      <c r="D92" t="n">
-        <v>0.1043769831340364</v>
-      </c>
-    </row>
-    <row r="93">
-      <c r="A93" t="n">
-        <v>30617</v>
-      </c>
-      <c r="B93" t="n">
-        <v>0</v>
-      </c>
-      <c r="C93" t="n">
-        <v>0.9163000583648682</v>
-      </c>
-      <c r="D93" t="n">
-        <v>0.1043677889206219</v>
-      </c>
-    </row>
-    <row r="94">
-      <c r="A94" t="n">
-        <v>30983</v>
-      </c>
-      <c r="B94" t="n">
-        <v>0</v>
-      </c>
-      <c r="C94" t="n">
-        <v>0.9165835976600647</v>
-      </c>
-      <c r="D94" t="n">
-        <v>0.1043523487544075</v>
-      </c>
-    </row>
-    <row r="95">
-      <c r="A95" t="n">
-        <v>32862</v>
-      </c>
-      <c r="B95" t="n">
-        <v>0</v>
-      </c>
-      <c r="C95" t="n">
-        <v>0.9167401790618896</v>
-      </c>
-      <c r="D95" t="n">
-        <v>0.1043438240533394</v>
-      </c>
-    </row>
-    <row r="96">
-      <c r="A96" t="n">
-        <v>30634</v>
-      </c>
-      <c r="B96" t="n">
-        <v>0</v>
-      </c>
-      <c r="C96" t="n">
-        <v>0.9169472008943558</v>
-      </c>
-      <c r="D96" t="n">
-        <v>0.1043325553811235</v>
-      </c>
-    </row>
-    <row r="97">
-      <c r="A97" t="n">
-        <v>30663</v>
-      </c>
-      <c r="B97" t="n">
-        <v>0</v>
-      </c>
-      <c r="C97" t="n">
-        <v>0.9169632196426392</v>
-      </c>
-      <c r="D97" t="n">
-        <v>0.1043316835454381</v>
-      </c>
-    </row>
-    <row r="98">
-      <c r="A98" t="n">
-        <v>30612</v>
-      </c>
-      <c r="B98" t="n">
-        <v>0</v>
-      </c>
-      <c r="C98" t="n">
-        <v>0.9171411991119385</v>
-      </c>
-      <c r="D98" t="n">
-        <v>0.1043219978229274</v>
-      </c>
-    </row>
-    <row r="99">
-      <c r="A99" t="n">
-        <v>30654</v>
-      </c>
-      <c r="B99" t="n">
-        <v>0</v>
-      </c>
-      <c r="C99" t="n">
-        <v>0.9172030538320541</v>
-      </c>
-      <c r="D99" t="n">
-        <v>0.104318632082421</v>
-      </c>
-    </row>
-    <row r="100">
-      <c r="A100" t="n">
-        <v>30661</v>
-      </c>
-      <c r="B100" t="n">
-        <v>0</v>
-      </c>
-      <c r="C100" t="n">
-        <v>0.9177192896604538</v>
-      </c>
-      <c r="D100" t="n">
-        <v>0.1042905502793433</v>
-      </c>
-    </row>
-    <row r="101">
-      <c r="A101" t="n">
-        <v>31281</v>
-      </c>
-      <c r="B101" t="n">
-        <v>0</v>
-      </c>
-      <c r="C101" t="n">
-        <v>0.9177635312080383</v>
-      </c>
-      <c r="D101" t="n">
-        <v>0.10428814436471</v>
+        <v>6501.30986</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added run_all_files with --FLAG where you can select the configuration
</commit_message>
<xml_diff>
--- a/output/scores.xlsx
+++ b/output/scores.xlsx
@@ -457,702 +457,702 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>21475</v>
+        <v>7921</v>
       </c>
       <c r="B2" t="n">
-        <v>8244.1301</v>
+        <v>610.1947</v>
       </c>
       <c r="C2" t="n">
         <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>6595.304080000001</v>
+        <v>488.15576</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>20753</v>
+        <v>14073</v>
       </c>
       <c r="B3" t="n">
-        <v>8236.766274999998</v>
+        <v>608.8172</v>
       </c>
       <c r="C3" t="n">
         <v>0</v>
       </c>
       <c r="D3" t="n">
-        <v>6589.413019999999</v>
+        <v>487.05376</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>10216</v>
+        <v>6605</v>
       </c>
       <c r="B4" t="n">
-        <v>8227.9354</v>
+        <v>608.8172</v>
       </c>
       <c r="C4" t="n">
         <v>0</v>
       </c>
       <c r="D4" t="n">
-        <v>6582.348320000001</v>
+        <v>487.05376</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>19359</v>
+        <v>2780</v>
       </c>
       <c r="B5" t="n">
-        <v>8219.466375</v>
+        <v>606.3536</v>
       </c>
       <c r="C5" t="n">
         <v>0</v>
       </c>
       <c r="D5" t="n">
-        <v>6575.573100000001</v>
+        <v>485.08288</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>27008</v>
+        <v>1279</v>
       </c>
       <c r="B6" t="n">
-        <v>8209.4872</v>
+        <v>524.57925</v>
       </c>
       <c r="C6" t="n">
         <v>0</v>
       </c>
       <c r="D6" t="n">
-        <v>6567.58976</v>
+        <v>419.6634</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>27734</v>
+        <v>6059</v>
       </c>
       <c r="B7" t="n">
-        <v>8203.661599999999</v>
+        <v>512.1137</v>
       </c>
       <c r="C7" t="n">
         <v>0</v>
       </c>
       <c r="D7" t="n">
-        <v>6562.92928</v>
+        <v>409.69096</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>21625</v>
+        <v>15097</v>
       </c>
       <c r="B8" t="n">
-        <v>8193.7513</v>
+        <v>511.92305</v>
       </c>
       <c r="C8" t="n">
         <v>0</v>
       </c>
       <c r="D8" t="n">
-        <v>6555.00104</v>
+        <v>409.53844</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>957</v>
+        <v>12717</v>
       </c>
       <c r="B9" t="n">
-        <v>8190.737375</v>
+        <v>507.4982</v>
       </c>
       <c r="C9" t="n">
         <v>0</v>
       </c>
       <c r="D9" t="n">
-        <v>6552.5899</v>
+        <v>405.99856</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>9075</v>
+        <v>5571</v>
       </c>
       <c r="B10" t="n">
-        <v>8184.391075</v>
+        <v>505.466975</v>
       </c>
       <c r="C10" t="n">
         <v>0</v>
       </c>
       <c r="D10" t="n">
-        <v>6547.51286</v>
+        <v>404.37358</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>12511</v>
+        <v>16328</v>
       </c>
       <c r="B11" t="n">
-        <v>8180.90375</v>
+        <v>503.2411</v>
       </c>
       <c r="C11" t="n">
         <v>0</v>
       </c>
       <c r="D11" t="n">
-        <v>6544.723000000001</v>
+        <v>402.59288</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>5329</v>
+        <v>1791</v>
       </c>
       <c r="B12" t="n">
-        <v>8173.2597</v>
+        <v>502.386775</v>
       </c>
       <c r="C12" t="n">
         <v>0</v>
       </c>
       <c r="D12" t="n">
-        <v>6538.60776</v>
+        <v>401.90942</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>3045</v>
+        <v>5799</v>
       </c>
       <c r="B13" t="n">
-        <v>8170.563599999999</v>
+        <v>499.1681</v>
       </c>
       <c r="C13" t="n">
         <v>0</v>
       </c>
       <c r="D13" t="n">
-        <v>6536.45088</v>
+        <v>399.33448</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>8057</v>
+        <v>15557</v>
       </c>
       <c r="B14" t="n">
-        <v>8169.128075</v>
+        <v>498.798</v>
       </c>
       <c r="C14" t="n">
         <v>0</v>
       </c>
       <c r="D14" t="n">
-        <v>6535.30246</v>
+        <v>399.0384</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>2469</v>
+        <v>9681</v>
       </c>
       <c r="B15" t="n">
-        <v>8167.481125</v>
+        <v>498.47285</v>
       </c>
       <c r="C15" t="n">
         <v>0</v>
       </c>
       <c r="D15" t="n">
-        <v>6533.9849</v>
+        <v>398.77828</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>7197</v>
+        <v>6374</v>
       </c>
       <c r="B16" t="n">
-        <v>8167.220275</v>
+        <v>497.546725</v>
       </c>
       <c r="C16" t="n">
         <v>0</v>
       </c>
       <c r="D16" t="n">
-        <v>6533.77622</v>
+        <v>398.03738</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>9205</v>
+        <v>20033</v>
       </c>
       <c r="B17" t="n">
-        <v>8166.3553</v>
+        <v>497.1067</v>
       </c>
       <c r="C17" t="n">
         <v>0</v>
       </c>
       <c r="D17" t="n">
-        <v>6533.08424</v>
+        <v>397.68536</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>24463</v>
+        <v>805</v>
       </c>
       <c r="B18" t="n">
-        <v>8166.065399999999</v>
+        <v>496.7993750000001</v>
       </c>
       <c r="C18" t="n">
         <v>0</v>
       </c>
       <c r="D18" t="n">
-        <v>6532.85232</v>
+        <v>397.4395000000001</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>7553</v>
+        <v>2733</v>
       </c>
       <c r="B19" t="n">
-        <v>8163.0496</v>
+        <v>494.807625</v>
       </c>
       <c r="C19" t="n">
         <v>0</v>
       </c>
       <c r="D19" t="n">
-        <v>6530.43968</v>
+        <v>395.8461</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>1770</v>
+        <v>3092</v>
       </c>
       <c r="B20" t="n">
-        <v>8161.907799999999</v>
+        <v>494.807625</v>
       </c>
       <c r="C20" t="n">
         <v>0</v>
       </c>
       <c r="D20" t="n">
-        <v>6529.526239999999</v>
+        <v>395.8461</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>29143</v>
+        <v>8290</v>
       </c>
       <c r="B21" t="n">
-        <v>8161.6783</v>
+        <v>494.807625</v>
       </c>
       <c r="C21" t="n">
         <v>0</v>
       </c>
       <c r="D21" t="n">
-        <v>6529.34264</v>
+        <v>395.8461</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>30543</v>
+        <v>8903</v>
       </c>
       <c r="B22" t="n">
-        <v>8161.6783</v>
+        <v>494.807625</v>
       </c>
       <c r="C22" t="n">
         <v>0</v>
       </c>
       <c r="D22" t="n">
-        <v>6529.34264</v>
+        <v>395.8461</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>12264</v>
+        <v>8980</v>
       </c>
       <c r="B23" t="n">
-        <v>8158.907825</v>
+        <v>493.585275</v>
       </c>
       <c r="C23" t="n">
         <v>0</v>
       </c>
       <c r="D23" t="n">
-        <v>6527.126260000001</v>
+        <v>394.8682200000001</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>11990</v>
+        <v>2787</v>
       </c>
       <c r="B24" t="n">
-        <v>8156.779025000001</v>
+        <v>493.339975</v>
       </c>
       <c r="C24" t="n">
         <v>0</v>
       </c>
       <c r="D24" t="n">
-        <v>6525.423220000001</v>
+        <v>394.67198</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>4340</v>
+        <v>8528</v>
       </c>
       <c r="B25" t="n">
-        <v>8156.149649999999</v>
+        <v>493.339975</v>
       </c>
       <c r="C25" t="n">
         <v>0</v>
       </c>
       <c r="D25" t="n">
-        <v>6524.91972</v>
+        <v>394.67198</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>9208</v>
+        <v>11624</v>
       </c>
       <c r="B26" t="n">
-        <v>8155.944750000001</v>
+        <v>493.339975</v>
       </c>
       <c r="C26" t="n">
         <v>0</v>
       </c>
       <c r="D26" t="n">
-        <v>6524.755800000001</v>
+        <v>394.67198</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>12696</v>
+        <v>21454</v>
       </c>
       <c r="B27" t="n">
-        <v>8155.125</v>
+        <v>493.339975</v>
       </c>
       <c r="C27" t="n">
         <v>0</v>
       </c>
       <c r="D27" t="n">
-        <v>6524.1</v>
+        <v>394.67198</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>7535</v>
+        <v>2889</v>
       </c>
       <c r="B28" t="n">
-        <v>8153.789699999999</v>
+        <v>493.339975</v>
       </c>
       <c r="C28" t="n">
         <v>0</v>
       </c>
       <c r="D28" t="n">
-        <v>6523.03176</v>
+        <v>394.67198</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>25668</v>
+        <v>1740</v>
       </c>
       <c r="B29" t="n">
-        <v>8148.133124999999</v>
+        <v>493.339975</v>
       </c>
       <c r="C29" t="n">
         <v>0</v>
       </c>
       <c r="D29" t="n">
-        <v>6518.5065</v>
+        <v>394.67198</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>29063</v>
+        <v>4376</v>
       </c>
       <c r="B30" t="n">
-        <v>8147.39975</v>
+        <v>493.339975</v>
       </c>
       <c r="C30" t="n">
         <v>0</v>
       </c>
       <c r="D30" t="n">
-        <v>6517.919800000001</v>
+        <v>394.67198</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>13548</v>
+        <v>12837</v>
       </c>
       <c r="B31" t="n">
-        <v>8145.776599999999</v>
+        <v>493.339975</v>
       </c>
       <c r="C31" t="n">
         <v>0</v>
       </c>
       <c r="D31" t="n">
-        <v>6516.621279999999</v>
+        <v>394.67198</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>13554</v>
+        <v>14461</v>
       </c>
       <c r="B32" t="n">
-        <v>8143.872975</v>
+        <v>493.339975</v>
       </c>
       <c r="C32" t="n">
         <v>0</v>
       </c>
       <c r="D32" t="n">
-        <v>6515.09838</v>
+        <v>394.67198</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>15319</v>
+        <v>247</v>
       </c>
       <c r="B33" t="n">
-        <v>8143.832975</v>
+        <v>493.339975</v>
       </c>
       <c r="C33" t="n">
         <v>0</v>
       </c>
       <c r="D33" t="n">
-        <v>6515.06638</v>
+        <v>394.67198</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>16823</v>
+        <v>10079</v>
       </c>
       <c r="B34" t="n">
-        <v>8143.0065</v>
+        <v>493.339975</v>
       </c>
       <c r="C34" t="n">
         <v>0</v>
       </c>
       <c r="D34" t="n">
-        <v>6514.405200000001</v>
+        <v>394.67198</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>14382</v>
+        <v>5825</v>
       </c>
       <c r="B35" t="n">
-        <v>8142.856974999999</v>
+        <v>493.339975</v>
       </c>
       <c r="C35" t="n">
         <v>0</v>
       </c>
       <c r="D35" t="n">
-        <v>6514.28558</v>
+        <v>394.67198</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>17542</v>
+        <v>4922</v>
       </c>
       <c r="B36" t="n">
-        <v>8142.713675000001</v>
+        <v>493.339975</v>
       </c>
       <c r="C36" t="n">
         <v>0</v>
       </c>
       <c r="D36" t="n">
-        <v>6514.170940000001</v>
+        <v>394.67198</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>13703</v>
+        <v>12983</v>
       </c>
       <c r="B37" t="n">
-        <v>8142.7061</v>
+        <v>493.339975</v>
       </c>
       <c r="C37" t="n">
         <v>0</v>
       </c>
       <c r="D37" t="n">
-        <v>6514.16488</v>
+        <v>394.67198</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>9010</v>
+        <v>6097</v>
       </c>
       <c r="B38" t="n">
-        <v>8142.095574999999</v>
+        <v>483.473575</v>
       </c>
       <c r="C38" t="n">
         <v>0</v>
       </c>
       <c r="D38" t="n">
-        <v>6513.67646</v>
+        <v>386.77886</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="n">
-        <v>7897</v>
+        <v>10333</v>
       </c>
       <c r="B39" t="n">
-        <v>8141.1327</v>
+        <v>483.119375</v>
       </c>
       <c r="C39" t="n">
         <v>0</v>
       </c>
       <c r="D39" t="n">
-        <v>6512.90616</v>
+        <v>386.4955</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="n">
-        <v>5642</v>
+        <v>1920</v>
       </c>
       <c r="B40" t="n">
-        <v>8140.682150000001</v>
+        <v>480.058375</v>
       </c>
       <c r="C40" t="n">
         <v>0</v>
       </c>
       <c r="D40" t="n">
-        <v>6512.545720000001</v>
+        <v>384.0467</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="n">
-        <v>2745</v>
+        <v>18516</v>
       </c>
       <c r="B41" t="n">
-        <v>8135.00945</v>
+        <v>480.058375</v>
       </c>
       <c r="C41" t="n">
         <v>0</v>
       </c>
       <c r="D41" t="n">
-        <v>6508.00756</v>
+        <v>384.0467</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="n">
-        <v>3559</v>
+        <v>13597</v>
       </c>
       <c r="B42" t="n">
-        <v>8135.00945</v>
+        <v>480.058375</v>
       </c>
       <c r="C42" t="n">
         <v>0</v>
       </c>
       <c r="D42" t="n">
-        <v>6508.00756</v>
+        <v>384.0467</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="n">
-        <v>6457</v>
+        <v>5836</v>
       </c>
       <c r="B43" t="n">
-        <v>8134.602725</v>
+        <v>479.588875</v>
       </c>
       <c r="C43" t="n">
         <v>0</v>
       </c>
       <c r="D43" t="n">
-        <v>6507.68218</v>
+        <v>383.6711</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="n">
-        <v>11722</v>
+        <v>7750</v>
       </c>
       <c r="B44" t="n">
-        <v>8134.383375</v>
+        <v>478.9514</v>
       </c>
       <c r="C44" t="n">
         <v>0</v>
       </c>
       <c r="D44" t="n">
-        <v>6507.506700000001</v>
+        <v>383.16112</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="n">
-        <v>481</v>
+        <v>3547</v>
       </c>
       <c r="B45" t="n">
-        <v>8134.094075</v>
+        <v>478.728175</v>
       </c>
       <c r="C45" t="n">
         <v>0</v>
       </c>
       <c r="D45" t="n">
-        <v>6507.27526</v>
+        <v>382.98254</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="n">
-        <v>21249</v>
+        <v>13538</v>
       </c>
       <c r="B46" t="n">
-        <v>8134.0124</v>
+        <v>477.2023</v>
       </c>
       <c r="C46" t="n">
         <v>0</v>
       </c>
       <c r="D46" t="n">
-        <v>6507.20992</v>
+        <v>381.7618400000001</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="n">
-        <v>20630</v>
+        <v>9518</v>
       </c>
       <c r="B47" t="n">
-        <v>8133.721525000001</v>
+        <v>476.428975</v>
       </c>
       <c r="C47" t="n">
         <v>0</v>
       </c>
       <c r="D47" t="n">
-        <v>6506.977220000001</v>
+        <v>381.14318</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="n">
-        <v>17724</v>
+        <v>5739</v>
       </c>
       <c r="B48" t="n">
-        <v>8131.2845</v>
+        <v>475.668575</v>
       </c>
       <c r="C48" t="n">
         <v>0</v>
       </c>
       <c r="D48" t="n">
-        <v>6505.0276</v>
+        <v>380.53486</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="n">
-        <v>865</v>
+        <v>2138</v>
       </c>
       <c r="B49" t="n">
-        <v>8129.757599999999</v>
+        <v>475.214225</v>
       </c>
       <c r="C49" t="n">
         <v>0</v>
       </c>
       <c r="D49" t="n">
-        <v>6503.806079999999</v>
+        <v>380.17138</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="n">
-        <v>17762</v>
+        <v>11720</v>
       </c>
       <c r="B50" t="n">
-        <v>8127.479499999999</v>
+        <v>475.212475</v>
       </c>
       <c r="C50" t="n">
         <v>0</v>
       </c>
       <c r="D50" t="n">
-        <v>6501.9836</v>
+        <v>380.16998</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="n">
-        <v>20315</v>
+        <v>14221</v>
       </c>
       <c r="B51" t="n">
-        <v>8126.637325</v>
+        <v>474.736775</v>
       </c>
       <c r="C51" t="n">
         <v>0</v>
       </c>
       <c r="D51" t="n">
-        <v>6501.30986</v>
+        <v>379.78942</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added functionality that looks up the genes from the pathways to see whether they should belong there, the code is working, the system instruction is not
</commit_message>
<xml_diff>
--- a/output/scores.xlsx
+++ b/output/scores.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D51"/>
+  <dimension ref="A1:D101"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -457,702 +457,1402 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>7921</v>
+        <v>20753</v>
       </c>
       <c r="B2" t="n">
-        <v>610.1947</v>
+        <v>8245.554699999999</v>
       </c>
       <c r="C2" t="n">
         <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>488.15576</v>
+        <v>6596.443759999999</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>14073</v>
+        <v>10216</v>
       </c>
       <c r="B3" t="n">
-        <v>608.8172</v>
+        <v>8237.858450000002</v>
       </c>
       <c r="C3" t="n">
         <v>0</v>
       </c>
       <c r="D3" t="n">
-        <v>487.05376</v>
+        <v>6590.286760000002</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>6605</v>
+        <v>27008</v>
       </c>
       <c r="B4" t="n">
-        <v>608.8172</v>
+        <v>8224.482</v>
       </c>
       <c r="C4" t="n">
         <v>0</v>
       </c>
       <c r="D4" t="n">
-        <v>487.05376</v>
+        <v>6579.5856</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>2780</v>
+        <v>27734</v>
       </c>
       <c r="B5" t="n">
-        <v>606.3536</v>
+        <v>8216.1823</v>
       </c>
       <c r="C5" t="n">
         <v>0</v>
       </c>
       <c r="D5" t="n">
-        <v>485.08288</v>
+        <v>6572.94584</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>1279</v>
+        <v>19359</v>
       </c>
       <c r="B6" t="n">
-        <v>524.57925</v>
+        <v>8215.506649999999</v>
       </c>
       <c r="C6" t="n">
         <v>0</v>
       </c>
       <c r="D6" t="n">
-        <v>419.6634</v>
+        <v>6572.40532</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>6059</v>
+        <v>21625</v>
       </c>
       <c r="B7" t="n">
-        <v>512.1137</v>
+        <v>8205.744650000001</v>
       </c>
       <c r="C7" t="n">
         <v>0</v>
       </c>
       <c r="D7" t="n">
-        <v>409.69096</v>
+        <v>6564.595720000001</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>15097</v>
+        <v>9075</v>
       </c>
       <c r="B8" t="n">
-        <v>511.92305</v>
+        <v>8183.968699999999</v>
       </c>
       <c r="C8" t="n">
         <v>0</v>
       </c>
       <c r="D8" t="n">
-        <v>409.53844</v>
+        <v>6547.17496</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>12717</v>
+        <v>957</v>
       </c>
       <c r="B9" t="n">
-        <v>507.4982</v>
+        <v>8180.4181</v>
       </c>
       <c r="C9" t="n">
         <v>0</v>
       </c>
       <c r="D9" t="n">
-        <v>405.99856</v>
+        <v>6544.33448</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>5571</v>
+        <v>12511</v>
       </c>
       <c r="B10" t="n">
-        <v>505.466975</v>
+        <v>8169.125675</v>
       </c>
       <c r="C10" t="n">
         <v>0</v>
       </c>
       <c r="D10" t="n">
-        <v>404.37358</v>
+        <v>6535.30054</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>16328</v>
+        <v>9205</v>
       </c>
       <c r="B11" t="n">
-        <v>503.2411</v>
+        <v>8161.8241</v>
       </c>
       <c r="C11" t="n">
         <v>0</v>
       </c>
       <c r="D11" t="n">
-        <v>402.59288</v>
+        <v>6529.45928</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>1791</v>
+        <v>5329</v>
       </c>
       <c r="B12" t="n">
-        <v>502.386775</v>
+        <v>8161.721875000001</v>
       </c>
       <c r="C12" t="n">
         <v>0</v>
       </c>
       <c r="D12" t="n">
-        <v>401.90942</v>
+        <v>6529.377500000001</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>5799</v>
+        <v>2469</v>
       </c>
       <c r="B13" t="n">
-        <v>499.1681</v>
+        <v>8160.27445</v>
       </c>
       <c r="C13" t="n">
         <v>0</v>
       </c>
       <c r="D13" t="n">
-        <v>399.33448</v>
+        <v>6528.21956</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>15557</v>
+        <v>7553</v>
       </c>
       <c r="B14" t="n">
-        <v>498.798</v>
+        <v>8156.1865</v>
       </c>
       <c r="C14" t="n">
         <v>0</v>
       </c>
       <c r="D14" t="n">
-        <v>399.0384</v>
+        <v>6524.9492</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>9681</v>
+        <v>1577</v>
       </c>
       <c r="B15" t="n">
-        <v>498.47285</v>
+        <v>8155.634050000001</v>
       </c>
       <c r="C15" t="n">
         <v>0</v>
       </c>
       <c r="D15" t="n">
-        <v>398.77828</v>
+        <v>6524.507240000001</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>6374</v>
+        <v>29143</v>
       </c>
       <c r="B16" t="n">
-        <v>497.546725</v>
+        <v>8155.2673</v>
       </c>
       <c r="C16" t="n">
         <v>0</v>
       </c>
       <c r="D16" t="n">
-        <v>398.03738</v>
+        <v>6524.21384</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>20033</v>
+        <v>30543</v>
       </c>
       <c r="B17" t="n">
-        <v>497.1067</v>
+        <v>8155.2673</v>
       </c>
       <c r="C17" t="n">
         <v>0</v>
       </c>
       <c r="D17" t="n">
-        <v>397.68536</v>
+        <v>6524.21384</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>805</v>
+        <v>24463</v>
       </c>
       <c r="B18" t="n">
-        <v>496.7993750000001</v>
+        <v>8154.727575</v>
       </c>
       <c r="C18" t="n">
         <v>0</v>
       </c>
       <c r="D18" t="n">
-        <v>397.4395000000001</v>
+        <v>6523.78206</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>2733</v>
+        <v>3045</v>
       </c>
       <c r="B19" t="n">
-        <v>494.807625</v>
+        <v>8149.7101</v>
       </c>
       <c r="C19" t="n">
         <v>0</v>
       </c>
       <c r="D19" t="n">
-        <v>395.8461</v>
+        <v>6519.768080000001</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>3092</v>
+        <v>12696</v>
       </c>
       <c r="B20" t="n">
-        <v>494.807625</v>
+        <v>8147.584275</v>
       </c>
       <c r="C20" t="n">
         <v>0</v>
       </c>
       <c r="D20" t="n">
-        <v>395.8461</v>
+        <v>6518.06742</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>8290</v>
+        <v>8057</v>
       </c>
       <c r="B21" t="n">
-        <v>494.807625</v>
+        <v>8146.9408</v>
       </c>
       <c r="C21" t="n">
         <v>0</v>
       </c>
       <c r="D21" t="n">
-        <v>395.8461</v>
+        <v>6517.552640000001</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>8903</v>
+        <v>4340</v>
       </c>
       <c r="B22" t="n">
-        <v>494.807625</v>
+        <v>8146.308349999999</v>
       </c>
       <c r="C22" t="n">
         <v>0</v>
       </c>
       <c r="D22" t="n">
-        <v>395.8461</v>
+        <v>6517.046679999999</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>8980</v>
+        <v>7197</v>
       </c>
       <c r="B23" t="n">
-        <v>493.585275</v>
+        <v>8143.2355</v>
       </c>
       <c r="C23" t="n">
         <v>0</v>
       </c>
       <c r="D23" t="n">
-        <v>394.8682200000001</v>
+        <v>6514.588400000001</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>2787</v>
+        <v>1770</v>
       </c>
       <c r="B24" t="n">
-        <v>493.339975</v>
+        <v>8140.2019</v>
       </c>
       <c r="C24" t="n">
         <v>0</v>
       </c>
       <c r="D24" t="n">
-        <v>394.67198</v>
+        <v>6512.161520000001</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>8528</v>
+        <v>11990</v>
       </c>
       <c r="B25" t="n">
-        <v>493.339975</v>
+        <v>8139.952325</v>
       </c>
       <c r="C25" t="n">
         <v>0</v>
       </c>
       <c r="D25" t="n">
-        <v>394.67198</v>
+        <v>6511.96186</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>11624</v>
+        <v>7535</v>
       </c>
       <c r="B26" t="n">
-        <v>493.339975</v>
+        <v>8139.214475000001</v>
       </c>
       <c r="C26" t="n">
         <v>0</v>
       </c>
       <c r="D26" t="n">
-        <v>394.67198</v>
+        <v>6511.371580000001</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>21454</v>
+        <v>25668</v>
       </c>
       <c r="B27" t="n">
-        <v>493.339975</v>
+        <v>8138.717275000001</v>
       </c>
       <c r="C27" t="n">
         <v>0</v>
       </c>
       <c r="D27" t="n">
-        <v>394.67198</v>
+        <v>6510.973820000001</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>2889</v>
+        <v>12264</v>
       </c>
       <c r="B28" t="n">
-        <v>493.339975</v>
+        <v>8136.2654</v>
       </c>
       <c r="C28" t="n">
         <v>0</v>
       </c>
       <c r="D28" t="n">
-        <v>394.67198</v>
+        <v>6509.012320000001</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>1740</v>
+        <v>9208</v>
       </c>
       <c r="B29" t="n">
-        <v>493.339975</v>
+        <v>8136.1844</v>
       </c>
       <c r="C29" t="n">
         <v>0</v>
       </c>
       <c r="D29" t="n">
-        <v>394.67198</v>
+        <v>6508.947520000001</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>4376</v>
+        <v>16823</v>
       </c>
       <c r="B30" t="n">
-        <v>493.339975</v>
+        <v>8134.7607</v>
       </c>
       <c r="C30" t="n">
         <v>0</v>
       </c>
       <c r="D30" t="n">
-        <v>394.67198</v>
+        <v>6507.80856</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>12837</v>
+        <v>17724</v>
       </c>
       <c r="B31" t="n">
-        <v>493.339975</v>
+        <v>8134.0388</v>
       </c>
       <c r="C31" t="n">
         <v>0</v>
       </c>
       <c r="D31" t="n">
-        <v>394.67198</v>
+        <v>6507.231040000001</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>14461</v>
+        <v>31569</v>
       </c>
       <c r="B32" t="n">
-        <v>493.339975</v>
+        <v>8133.954450000001</v>
       </c>
       <c r="C32" t="n">
         <v>0</v>
       </c>
       <c r="D32" t="n">
-        <v>394.67198</v>
+        <v>6507.163560000001</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>247</v>
+        <v>34240</v>
       </c>
       <c r="B33" t="n">
-        <v>493.339975</v>
+        <v>8133.954450000001</v>
       </c>
       <c r="C33" t="n">
         <v>0</v>
       </c>
       <c r="D33" t="n">
-        <v>394.67198</v>
+        <v>6507.163560000001</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>10079</v>
+        <v>7897</v>
       </c>
       <c r="B34" t="n">
-        <v>493.339975</v>
+        <v>8131.755300000001</v>
       </c>
       <c r="C34" t="n">
         <v>0</v>
       </c>
       <c r="D34" t="n">
-        <v>394.67198</v>
+        <v>6505.404240000001</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>5825</v>
+        <v>35942</v>
       </c>
       <c r="B35" t="n">
-        <v>493.339975</v>
+        <v>8129.244975000001</v>
       </c>
       <c r="C35" t="n">
         <v>0</v>
       </c>
       <c r="D35" t="n">
-        <v>394.67198</v>
+        <v>6503.395980000001</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>4922</v>
+        <v>33271</v>
       </c>
       <c r="B36" t="n">
-        <v>493.339975</v>
+        <v>8129.244975000001</v>
       </c>
       <c r="C36" t="n">
         <v>0</v>
       </c>
       <c r="D36" t="n">
-        <v>394.67198</v>
+        <v>6503.395980000001</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>12983</v>
+        <v>21249</v>
       </c>
       <c r="B37" t="n">
-        <v>493.339975</v>
+        <v>8126.701650000001</v>
       </c>
       <c r="C37" t="n">
         <v>0</v>
       </c>
       <c r="D37" t="n">
-        <v>394.67198</v>
+        <v>6501.361320000001</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>6097</v>
+        <v>13548</v>
       </c>
       <c r="B38" t="n">
-        <v>483.473575</v>
+        <v>8126.08865</v>
       </c>
       <c r="C38" t="n">
         <v>0</v>
       </c>
       <c r="D38" t="n">
-        <v>386.77886</v>
+        <v>6500.87092</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="n">
-        <v>10333</v>
+        <v>34491</v>
       </c>
       <c r="B39" t="n">
-        <v>483.119375</v>
+        <v>8125.830975</v>
       </c>
       <c r="C39" t="n">
         <v>0</v>
       </c>
       <c r="D39" t="n">
-        <v>386.4955</v>
+        <v>6500.66478</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="n">
-        <v>1920</v>
+        <v>31820</v>
       </c>
       <c r="B40" t="n">
-        <v>480.058375</v>
+        <v>8125.830975</v>
       </c>
       <c r="C40" t="n">
         <v>0</v>
       </c>
       <c r="D40" t="n">
-        <v>384.0467</v>
+        <v>6500.66478</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="n">
-        <v>18516</v>
+        <v>14382</v>
       </c>
       <c r="B41" t="n">
-        <v>480.058375</v>
+        <v>8124.463</v>
       </c>
       <c r="C41" t="n">
         <v>0</v>
       </c>
       <c r="D41" t="n">
-        <v>384.0467</v>
+        <v>6499.570400000001</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="n">
-        <v>13597</v>
+        <v>5642</v>
       </c>
       <c r="B42" t="n">
-        <v>480.058375</v>
+        <v>8123.6559</v>
       </c>
       <c r="C42" t="n">
         <v>0</v>
       </c>
       <c r="D42" t="n">
-        <v>384.0467</v>
+        <v>6498.92472</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="n">
-        <v>5836</v>
+        <v>17542</v>
       </c>
       <c r="B43" t="n">
-        <v>479.588875</v>
+        <v>8123.321099999999</v>
       </c>
       <c r="C43" t="n">
         <v>0</v>
       </c>
       <c r="D43" t="n">
-        <v>383.6711</v>
+        <v>6498.65688</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="n">
-        <v>7750</v>
+        <v>9010</v>
       </c>
       <c r="B44" t="n">
-        <v>478.9514</v>
+        <v>8122.423574999999</v>
       </c>
       <c r="C44" t="n">
         <v>0</v>
       </c>
       <c r="D44" t="n">
-        <v>383.16112</v>
+        <v>6497.938859999999</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="n">
-        <v>3547</v>
+        <v>29063</v>
       </c>
       <c r="B45" t="n">
-        <v>478.728175</v>
+        <v>8121.7375</v>
       </c>
       <c r="C45" t="n">
         <v>0</v>
       </c>
       <c r="D45" t="n">
-        <v>382.98254</v>
+        <v>6497.39</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="n">
-        <v>13538</v>
+        <v>11722</v>
       </c>
       <c r="B46" t="n">
-        <v>477.2023</v>
+        <v>8121.719475</v>
       </c>
       <c r="C46" t="n">
         <v>0</v>
       </c>
       <c r="D46" t="n">
-        <v>381.7618400000001</v>
+        <v>6497.37558</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="n">
-        <v>9518</v>
+        <v>13554</v>
       </c>
       <c r="B47" t="n">
-        <v>476.428975</v>
+        <v>8121.304099999999</v>
       </c>
       <c r="C47" t="n">
         <v>0</v>
       </c>
       <c r="D47" t="n">
-        <v>381.14318</v>
+        <v>6497.04328</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="n">
-        <v>5739</v>
+        <v>15319</v>
       </c>
       <c r="B48" t="n">
-        <v>475.668575</v>
+        <v>8118.2064</v>
       </c>
       <c r="C48" t="n">
         <v>0</v>
       </c>
       <c r="D48" t="n">
-        <v>380.53486</v>
+        <v>6494.56512</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="n">
-        <v>2138</v>
+        <v>6457</v>
       </c>
       <c r="B49" t="n">
-        <v>475.214225</v>
+        <v>8116.238775</v>
       </c>
       <c r="C49" t="n">
         <v>0</v>
       </c>
       <c r="D49" t="n">
-        <v>380.17138</v>
+        <v>6492.99102</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="n">
-        <v>11720</v>
+        <v>481</v>
       </c>
       <c r="B50" t="n">
-        <v>475.212475</v>
+        <v>8115.0572</v>
       </c>
       <c r="C50" t="n">
         <v>0</v>
       </c>
       <c r="D50" t="n">
-        <v>380.16998</v>
+        <v>6492.045760000001</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="n">
-        <v>14221</v>
+        <v>13703</v>
       </c>
       <c r="B51" t="n">
-        <v>474.736775</v>
+        <v>8114.830225</v>
       </c>
       <c r="C51" t="n">
         <v>0</v>
       </c>
       <c r="D51" t="n">
-        <v>379.78942</v>
+        <v>6491.86418</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="n">
+        <v>33947</v>
+      </c>
+      <c r="B52" t="n">
+        <v>0</v>
+      </c>
+      <c r="C52" t="n">
+        <v>0.8968429565429688</v>
+      </c>
+      <c r="D52" t="n">
+        <v>0.1054383544563456</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="n">
+        <v>35536</v>
+      </c>
+      <c r="B53" t="n">
+        <v>0</v>
+      </c>
+      <c r="C53" t="n">
+        <v>0.897493322690328</v>
+      </c>
+      <c r="D53" t="n">
+        <v>0.1054022154430738</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="n">
+        <v>33653</v>
+      </c>
+      <c r="B54" t="n">
+        <v>0</v>
+      </c>
+      <c r="C54" t="n">
+        <v>0.8976641893386841</v>
+      </c>
+      <c r="D54" t="n">
+        <v>0.1053927249740102</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="n">
+        <v>35002</v>
+      </c>
+      <c r="B55" t="n">
+        <v>0</v>
+      </c>
+      <c r="C55" t="n">
+        <v>0.8976899385452271</v>
+      </c>
+      <c r="D55" t="n">
+        <v>0.1053912949305725</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="n">
+        <v>34381</v>
+      </c>
+      <c r="B56" t="n">
+        <v>0</v>
+      </c>
+      <c r="C56" t="n">
+        <v>0.8978914221127828</v>
+      </c>
+      <c r="D56" t="n">
+        <v>0.1053801064011105</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="n">
+        <v>33476</v>
+      </c>
+      <c r="B57" t="n">
+        <v>0</v>
+      </c>
+      <c r="C57" t="n">
+        <v>0.898270308971405</v>
+      </c>
+      <c r="D57" t="n">
+        <v>0.1053590729701566</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="n">
+        <v>33951</v>
+      </c>
+      <c r="B58" t="n">
+        <v>0</v>
+      </c>
+      <c r="C58" t="n">
+        <v>0.8983739217122396</v>
+      </c>
+      <c r="D58" t="n">
+        <v>0.1053533225001373</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="n">
+        <v>35952</v>
+      </c>
+      <c r="B59" t="n">
+        <v>0</v>
+      </c>
+      <c r="C59" t="n">
+        <v>0.8984845578670502</v>
+      </c>
+      <c r="D59" t="n">
+        <v>0.105347182926102</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="n">
+        <v>33669</v>
+      </c>
+      <c r="B60" t="n">
+        <v>0</v>
+      </c>
+      <c r="C60" t="n">
+        <v>0.89869624376297</v>
+      </c>
+      <c r="D60" t="n">
+        <v>0.1053354377547121</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="n">
+        <v>34393</v>
+      </c>
+      <c r="B61" t="n">
+        <v>0</v>
+      </c>
+      <c r="C61" t="n">
+        <v>0.8989661534627279</v>
+      </c>
+      <c r="D61" t="n">
+        <v>0.105320465894194</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="n">
+        <v>35977</v>
+      </c>
+      <c r="B62" t="n">
+        <v>0</v>
+      </c>
+      <c r="C62" t="n">
+        <v>0.8992423713207245</v>
+      </c>
+      <c r="D62" t="n">
+        <v>0.1053051485266311</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="n">
+        <v>33370</v>
+      </c>
+      <c r="B63" t="n">
+        <v>0</v>
+      </c>
+      <c r="C63" t="n">
+        <v>0.8993287483851115</v>
+      </c>
+      <c r="D63" t="n">
+        <v>0.10530035949282</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="n">
+        <v>34991</v>
+      </c>
+      <c r="B64" t="n">
+        <v>0</v>
+      </c>
+      <c r="C64" t="n">
+        <v>0.9000890254974365</v>
+      </c>
+      <c r="D64" t="n">
+        <v>0.1052582259653022</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="n">
+        <v>35963</v>
+      </c>
+      <c r="B65" t="n">
+        <v>0</v>
+      </c>
+      <c r="C65" t="n">
+        <v>0.900578498840332</v>
+      </c>
+      <c r="D65" t="n">
+        <v>0.1052311178528186</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="n">
+        <v>34476</v>
+      </c>
+      <c r="B66" t="n">
+        <v>0</v>
+      </c>
+      <c r="C66" t="n">
+        <v>0.9015579521656036</v>
+      </c>
+      <c r="D66" t="n">
+        <v>0.1051769154719837</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="n">
+        <v>33955</v>
+      </c>
+      <c r="B67" t="n">
+        <v>0</v>
+      </c>
+      <c r="C67" t="n">
+        <v>0.9027023911476135</v>
+      </c>
+      <c r="D67" t="n">
+        <v>0.1051136535753078</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="n">
+        <v>34333</v>
+      </c>
+      <c r="B68" t="n">
+        <v>0</v>
+      </c>
+      <c r="C68" t="n">
+        <v>0.9027253190676371</v>
+      </c>
+      <c r="D68" t="n">
+        <v>0.1051123869513667</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="n">
+        <v>35475</v>
+      </c>
+      <c r="B69" t="n">
+        <v>0</v>
+      </c>
+      <c r="C69" t="n">
+        <v>0.902880847454071</v>
+      </c>
+      <c r="D69" t="n">
+        <v>0.1051037957881529</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="n">
+        <v>35537</v>
+      </c>
+      <c r="B70" t="n">
+        <v>0</v>
+      </c>
+      <c r="C70" t="n">
+        <v>0.9030412137508392</v>
+      </c>
+      <c r="D70" t="n">
+        <v>0.1050949388562142</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="n">
+        <v>35784</v>
+      </c>
+      <c r="B71" t="n">
+        <v>0</v>
+      </c>
+      <c r="C71" t="n">
+        <v>0.9032787084579468</v>
+      </c>
+      <c r="D71" t="n">
+        <v>0.105081824911519</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="n">
+        <v>33496</v>
+      </c>
+      <c r="B72" t="n">
+        <v>0</v>
+      </c>
+      <c r="C72" t="n">
+        <v>0.9033027688662211</v>
+      </c>
+      <c r="D72" t="n">
+        <v>0.1050804965303224</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="n">
+        <v>35540</v>
+      </c>
+      <c r="B73" t="n">
+        <v>0</v>
+      </c>
+      <c r="C73" t="n">
+        <v>0.9035961329936981</v>
+      </c>
+      <c r="D73" t="n">
+        <v>0.1050643025238075</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="n">
+        <v>34357</v>
+      </c>
+      <c r="B74" t="n">
+        <v>0</v>
+      </c>
+      <c r="C74" t="n">
+        <v>0.9041078090667725</v>
+      </c>
+      <c r="D74" t="n">
+        <v>0.1050360694114387</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="n">
+        <v>35535</v>
+      </c>
+      <c r="B75" t="n">
+        <v>0</v>
+      </c>
+      <c r="C75" t="n">
+        <v>0.904373899102211</v>
+      </c>
+      <c r="D75" t="n">
+        <v>0.1050213931698429</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="n">
+        <v>34471</v>
+      </c>
+      <c r="B76" t="n">
+        <v>0</v>
+      </c>
+      <c r="C76" t="n">
+        <v>0.9044817984104156</v>
+      </c>
+      <c r="D76" t="n">
+        <v>0.1050154431336287</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="n">
+        <v>35474</v>
+      </c>
+      <c r="B77" t="n">
+        <v>0</v>
+      </c>
+      <c r="C77" t="n">
+        <v>0.9045203328132629</v>
+      </c>
+      <c r="D77" t="n">
+        <v>0.1050133183427713</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="n">
+        <v>34383</v>
+      </c>
+      <c r="B78" t="n">
+        <v>0</v>
+      </c>
+      <c r="C78" t="n">
+        <v>0.9046141058206558</v>
+      </c>
+      <c r="D78" t="n">
+        <v>0.1050081480488797</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="n">
+        <v>35636</v>
+      </c>
+      <c r="B79" t="n">
+        <v>0</v>
+      </c>
+      <c r="C79" t="n">
+        <v>0.9047234803438187</v>
+      </c>
+      <c r="D79" t="n">
+        <v>0.1050021181887768</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="n">
+        <v>34728</v>
+      </c>
+      <c r="B80" t="n">
+        <v>0</v>
+      </c>
+      <c r="C80" t="n">
+        <v>0.9047234803438187</v>
+      </c>
+      <c r="D80" t="n">
+        <v>0.1050021181887768</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="n">
+        <v>35211</v>
+      </c>
+      <c r="B81" t="n">
+        <v>0</v>
+      </c>
+      <c r="C81" t="n">
+        <v>0.9047258893648783</v>
+      </c>
+      <c r="D81" t="n">
+        <v>0.105001985386301</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="n">
+        <v>33656</v>
+      </c>
+      <c r="B82" t="n">
+        <v>0</v>
+      </c>
+      <c r="C82" t="n">
+        <v>0.9047581106424332</v>
+      </c>
+      <c r="D82" t="n">
+        <v>0.1050002091512525</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="n">
+        <v>33652</v>
+      </c>
+      <c r="B83" t="n">
+        <v>0</v>
+      </c>
+      <c r="C83" t="n">
+        <v>0.9050462245941162</v>
+      </c>
+      <c r="D83" t="n">
+        <v>0.1049843292083957</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="n">
+        <v>35781</v>
+      </c>
+      <c r="B84" t="n">
+        <v>0</v>
+      </c>
+      <c r="C84" t="n">
+        <v>0.905357301235199</v>
+      </c>
+      <c r="D84" t="n">
+        <v>0.1049671890255673</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="n">
+        <v>33372</v>
+      </c>
+      <c r="B85" t="n">
+        <v>0</v>
+      </c>
+      <c r="C85" t="n">
+        <v>0.9053683131933212</v>
+      </c>
+      <c r="D85" t="n">
+        <v>0.1049665823742015</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="n">
+        <v>35532</v>
+      </c>
+      <c r="B86" t="n">
+        <v>0</v>
+      </c>
+      <c r="C86" t="n">
+        <v>0.9057461619377136</v>
+      </c>
+      <c r="D86" t="n">
+        <v>0.1049457708452867</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="n">
+        <v>35541</v>
+      </c>
+      <c r="B87" t="n">
+        <v>0</v>
+      </c>
+      <c r="C87" t="n">
+        <v>0.9061278700828552</v>
+      </c>
+      <c r="D87" t="n">
+        <v>0.1049247551221768</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="n">
+        <v>35470</v>
+      </c>
+      <c r="B88" t="n">
+        <v>0</v>
+      </c>
+      <c r="C88" t="n">
+        <v>0.906619518995285</v>
+      </c>
+      <c r="D88" t="n">
+        <v>0.1048976987843869</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="n">
+        <v>33952</v>
+      </c>
+      <c r="B89" t="n">
+        <v>0</v>
+      </c>
+      <c r="C89" t="n">
+        <v>0.9071236550807953</v>
+      </c>
+      <c r="D89" t="n">
+        <v>0.1048699697406496</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="n">
+        <v>33654</v>
+      </c>
+      <c r="B90" t="n">
+        <v>0</v>
+      </c>
+      <c r="C90" t="n">
+        <v>0.90763820707798</v>
+      </c>
+      <c r="D90" t="n">
+        <v>0.1048416829029387</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="n">
+        <v>35533</v>
+      </c>
+      <c r="B91" t="n">
+        <v>0</v>
+      </c>
+      <c r="C91" t="n">
+        <v>0.9079031497240067</v>
+      </c>
+      <c r="D91" t="n">
+        <v>0.1048271239705913</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="n">
+        <v>34416</v>
+      </c>
+      <c r="B92" t="n">
+        <v>0</v>
+      </c>
+      <c r="C92" t="n">
+        <v>0.9082106351852417</v>
+      </c>
+      <c r="D92" t="n">
+        <v>0.1048102323256283</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="n">
+        <v>33641</v>
+      </c>
+      <c r="B93" t="n">
+        <v>0</v>
+      </c>
+      <c r="C93" t="n">
+        <v>0.908934473991394</v>
+      </c>
+      <c r="D93" t="n">
+        <v>0.1047704898858156</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="n">
+        <v>34602</v>
+      </c>
+      <c r="B94" t="n">
+        <v>0</v>
+      </c>
+      <c r="C94" t="n">
+        <v>0.9090376794338226</v>
+      </c>
+      <c r="D94" t="n">
+        <v>0.1047648258358711</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="n">
+        <v>35425</v>
+      </c>
+      <c r="B95" t="n">
+        <v>0</v>
+      </c>
+      <c r="C95" t="n">
+        <v>0.9134311676025391</v>
+      </c>
+      <c r="D95" t="n">
+        <v>0.104524272096285</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="n">
+        <v>35531</v>
+      </c>
+      <c r="B96" t="n">
+        <v>0</v>
+      </c>
+      <c r="C96" t="n">
+        <v>0.9135860353708267</v>
+      </c>
+      <c r="D96" t="n">
+        <v>0.1045158128786421</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="n">
+        <v>35191</v>
+      </c>
+      <c r="B97" t="n">
+        <v>0</v>
+      </c>
+      <c r="C97" t="n">
+        <v>0.9137048870325089</v>
+      </c>
+      <c r="D97" t="n">
+        <v>0.1045093218683945</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="n">
+        <v>34938</v>
+      </c>
+      <c r="B98" t="n">
+        <v>0</v>
+      </c>
+      <c r="C98" t="n">
+        <v>0.9137140512466431</v>
+      </c>
+      <c r="D98" t="n">
+        <v>0.1045088214039683</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="n">
+        <v>34474</v>
+      </c>
+      <c r="B99" t="n">
+        <v>0</v>
+      </c>
+      <c r="C99" t="n">
+        <v>0.913762092590332</v>
+      </c>
+      <c r="D99" t="n">
+        <v>0.1045061979095292</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="n">
+        <v>35935</v>
+      </c>
+      <c r="B100" t="n">
+        <v>0</v>
+      </c>
+      <c r="C100" t="n">
+        <v>0.9142507314682007</v>
+      </c>
+      <c r="D100" t="n">
+        <v>0.1044795212624018</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="n">
+        <v>35216</v>
+      </c>
+      <c r="B101" t="n">
+        <v>0</v>
+      </c>
+      <c r="C101" t="n">
+        <v>0.9142822623252869</v>
+      </c>
+      <c r="D101" t="n">
+        <v>0.1044778003412408</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Validation of Papers, however regex not working propperly
</commit_message>
<xml_diff>
--- a/output/scores.xlsx
+++ b/output/scores.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -457,534 +457,534 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>2451</v>
+        <v>2450</v>
       </c>
       <c r="B2" t="n">
-        <v>179.7835</v>
+        <v>169.6026</v>
       </c>
       <c r="C2" t="n">
         <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>143.8268</v>
+        <v>135.68208</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>527</v>
+        <v>780</v>
       </c>
       <c r="B3" t="n">
-        <v>179.4564</v>
+        <v>168.4212</v>
       </c>
       <c r="C3" t="n">
         <v>0</v>
       </c>
       <c r="D3" t="n">
-        <v>143.56512</v>
+        <v>134.73696</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>2462</v>
+        <v>1689</v>
       </c>
       <c r="B4" t="n">
-        <v>175.1766</v>
+        <v>168.1452</v>
       </c>
       <c r="C4" t="n">
         <v>0</v>
       </c>
       <c r="D4" t="n">
-        <v>140.14128</v>
+        <v>134.51616</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>2551</v>
+        <v>1626</v>
       </c>
       <c r="B5" t="n">
-        <v>169.6164</v>
+        <v>167.9052</v>
       </c>
       <c r="C5" t="n">
         <v>0</v>
       </c>
       <c r="D5" t="n">
-        <v>135.69312</v>
+        <v>134.32416</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>2450</v>
+        <v>387</v>
       </c>
       <c r="B6" t="n">
-        <v>169.6026</v>
+        <v>166.499</v>
       </c>
       <c r="C6" t="n">
         <v>0</v>
       </c>
       <c r="D6" t="n">
-        <v>135.68208</v>
+        <v>133.1992</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>780</v>
+        <v>908</v>
       </c>
       <c r="B7" t="n">
-        <v>168.4212</v>
+        <v>166.4251</v>
       </c>
       <c r="C7" t="n">
         <v>0</v>
       </c>
       <c r="D7" t="n">
-        <v>134.73696</v>
+        <v>133.14008</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>1689</v>
+        <v>903</v>
       </c>
       <c r="B8" t="n">
-        <v>168.1452</v>
+        <v>165.0349</v>
       </c>
       <c r="C8" t="n">
         <v>0</v>
       </c>
       <c r="D8" t="n">
-        <v>134.51616</v>
+        <v>132.02792</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>1206</v>
+        <v>967</v>
       </c>
       <c r="B9" t="n">
-        <v>167.8389</v>
+        <v>164.6438</v>
       </c>
       <c r="C9" t="n">
         <v>0</v>
       </c>
       <c r="D9" t="n">
-        <v>134.27112</v>
+        <v>131.71504</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>908</v>
+        <v>509</v>
       </c>
       <c r="B10" t="n">
-        <v>166.4251</v>
+        <v>164.6222</v>
       </c>
       <c r="C10" t="n">
         <v>0</v>
       </c>
       <c r="D10" t="n">
-        <v>133.14008</v>
+        <v>131.69776</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>903</v>
+        <v>1469</v>
       </c>
       <c r="B11" t="n">
-        <v>165.0349</v>
+        <v>163.7061</v>
       </c>
       <c r="C11" t="n">
         <v>0</v>
       </c>
       <c r="D11" t="n">
-        <v>132.02792</v>
+        <v>130.96488</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>967</v>
+        <v>1580</v>
       </c>
       <c r="B12" t="n">
-        <v>164.6438</v>
+        <v>163.5039</v>
       </c>
       <c r="C12" t="n">
         <v>0</v>
       </c>
       <c r="D12" t="n">
-        <v>131.71504</v>
+        <v>130.80312</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>509</v>
+        <v>2328</v>
       </c>
       <c r="B13" t="n">
-        <v>164.6222</v>
+        <v>163.3697</v>
       </c>
       <c r="C13" t="n">
         <v>0</v>
       </c>
       <c r="D13" t="n">
-        <v>131.69776</v>
+        <v>130.69576</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>1548</v>
+        <v>259</v>
       </c>
       <c r="B14" t="n">
-        <v>164.2457</v>
+        <v>162.6408</v>
       </c>
       <c r="C14" t="n">
         <v>0</v>
       </c>
       <c r="D14" t="n">
-        <v>131.39656</v>
+        <v>130.11264</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>1586</v>
+        <v>527</v>
       </c>
       <c r="B15" t="n">
-        <v>163.8001</v>
+        <v>114.2424</v>
       </c>
       <c r="C15" t="n">
         <v>0</v>
       </c>
       <c r="D15" t="n">
-        <v>131.04008</v>
+        <v>91.39392000000001</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>1469</v>
+        <v>2451</v>
       </c>
       <c r="B16" t="n">
-        <v>163.7061</v>
+        <v>112.7039</v>
       </c>
       <c r="C16" t="n">
         <v>0</v>
       </c>
       <c r="D16" t="n">
-        <v>130.96488</v>
+        <v>90.16312000000001</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>1580</v>
+        <v>2551</v>
       </c>
       <c r="B17" t="n">
-        <v>163.5039</v>
+        <v>108.7985</v>
       </c>
       <c r="C17" t="n">
         <v>0</v>
       </c>
       <c r="D17" t="n">
-        <v>130.80312</v>
+        <v>87.03880000000001</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>287</v>
+        <v>2518</v>
       </c>
       <c r="B18" t="n">
-        <v>163.4785</v>
+        <v>108.5449</v>
       </c>
       <c r="C18" t="n">
         <v>0</v>
       </c>
       <c r="D18" t="n">
-        <v>130.7828</v>
+        <v>86.83592</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>2328</v>
+        <v>1207</v>
       </c>
       <c r="B19" t="n">
-        <v>163.3697</v>
+        <v>107.79585</v>
       </c>
       <c r="C19" t="n">
         <v>0</v>
       </c>
       <c r="D19" t="n">
-        <v>130.69576</v>
+        <v>86.23668000000001</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>259</v>
+        <v>2257</v>
       </c>
       <c r="B20" t="n">
-        <v>162.6408</v>
+        <v>107.35135</v>
       </c>
       <c r="C20" t="n">
         <v>0</v>
       </c>
       <c r="D20" t="n">
-        <v>130.11264</v>
+        <v>85.88108000000001</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>250</v>
+        <v>1349</v>
       </c>
       <c r="B21" t="n">
-        <v>111.6117</v>
+        <v>107.35135</v>
       </c>
       <c r="C21" t="n">
         <v>0</v>
       </c>
       <c r="D21" t="n">
-        <v>89.28936</v>
+        <v>85.88108000000001</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>1567</v>
+        <v>1206</v>
       </c>
       <c r="B22" t="n">
-        <v>110.23595</v>
+        <v>107.04275</v>
       </c>
       <c r="C22" t="n">
         <v>0</v>
       </c>
       <c r="D22" t="n">
-        <v>88.18876</v>
+        <v>85.63420000000001</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>1590</v>
+        <v>1548</v>
       </c>
       <c r="B23" t="n">
-        <v>109.47795</v>
+        <v>106.3023</v>
       </c>
       <c r="C23" t="n">
         <v>0</v>
       </c>
       <c r="D23" t="n">
-        <v>87.58235999999999</v>
+        <v>85.04184000000001</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>553</v>
+        <v>569</v>
       </c>
       <c r="B24" t="n">
-        <v>108.36245</v>
+        <v>105.9566</v>
       </c>
       <c r="C24" t="n">
         <v>0</v>
       </c>
       <c r="D24" t="n">
-        <v>86.68996</v>
+        <v>84.76528000000002</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>709</v>
+        <v>1616</v>
       </c>
       <c r="B25" t="n">
-        <v>108.0392</v>
+        <v>105.3634</v>
       </c>
       <c r="C25" t="n">
         <v>0</v>
       </c>
       <c r="D25" t="n">
-        <v>86.43136</v>
+        <v>84.29072000000002</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>547</v>
+        <v>1590</v>
       </c>
       <c r="B26" t="n">
-        <v>107.2905</v>
+        <v>105.35565</v>
       </c>
       <c r="C26" t="n">
         <v>0</v>
       </c>
       <c r="D26" t="n">
-        <v>85.83240000000001</v>
+        <v>84.28452</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>1128</v>
+        <v>243</v>
       </c>
       <c r="B27" t="n">
-        <v>105.63385</v>
+        <v>105.27315</v>
       </c>
       <c r="C27" t="n">
         <v>0</v>
       </c>
       <c r="D27" t="n">
-        <v>84.50708000000002</v>
+        <v>84.21852000000001</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>2526</v>
+        <v>1418</v>
       </c>
       <c r="B28" t="n">
-        <v>105.25075</v>
+        <v>104.9433</v>
       </c>
       <c r="C28" t="n">
         <v>0</v>
       </c>
       <c r="D28" t="n">
-        <v>84.20060000000001</v>
+        <v>83.95464</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>374</v>
+        <v>553</v>
       </c>
       <c r="B29" t="n">
-        <v>105.0517</v>
+        <v>104.24015</v>
       </c>
       <c r="C29" t="n">
         <v>0</v>
       </c>
       <c r="D29" t="n">
-        <v>84.04136000000001</v>
+        <v>83.39212000000001</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>1207</v>
+        <v>709</v>
       </c>
       <c r="B30" t="n">
-        <v>104.78845</v>
+        <v>103.9169</v>
       </c>
       <c r="C30" t="n">
         <v>0</v>
       </c>
       <c r="D30" t="n">
-        <v>83.83076</v>
+        <v>83.13352</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>2518</v>
+        <v>1586</v>
       </c>
       <c r="B31" t="n">
-        <v>104.27815</v>
+        <v>103.43295</v>
       </c>
       <c r="C31" t="n">
         <v>0</v>
       </c>
       <c r="D31" t="n">
-        <v>83.42252000000001</v>
+        <v>82.74636</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>243</v>
+        <v>547</v>
       </c>
       <c r="B32" t="n">
-        <v>104.259</v>
+        <v>103.1682</v>
       </c>
       <c r="C32" t="n">
         <v>0</v>
       </c>
       <c r="D32" t="n">
-        <v>83.4072</v>
+        <v>82.53456</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>2257</v>
+        <v>437</v>
       </c>
       <c r="B33" t="n">
-        <v>104.2335</v>
+        <v>103.1149</v>
       </c>
       <c r="C33" t="n">
         <v>0</v>
       </c>
       <c r="D33" t="n">
-        <v>83.38680000000001</v>
+        <v>82.49192000000001</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>1349</v>
+        <v>548</v>
       </c>
       <c r="B34" t="n">
-        <v>104.2335</v>
+        <v>102.8192</v>
       </c>
       <c r="C34" t="n">
         <v>0</v>
       </c>
       <c r="D34" t="n">
-        <v>83.38680000000001</v>
+        <v>82.25536000000001</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>387</v>
+        <v>521</v>
       </c>
       <c r="B35" t="n">
-        <v>102.65625</v>
+        <v>102.43275</v>
       </c>
       <c r="C35" t="n">
         <v>0</v>
       </c>
       <c r="D35" t="n">
-        <v>82.125</v>
+        <v>81.9462</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>1418</v>
+        <v>1141</v>
       </c>
       <c r="B36" t="n">
-        <v>102.5773</v>
+        <v>101.296</v>
       </c>
       <c r="C36" t="n">
         <v>0</v>
       </c>
       <c r="D36" t="n">
-        <v>82.06184000000002</v>
+        <v>81.0368</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>1616</v>
+        <v>2526</v>
       </c>
       <c r="B37" t="n">
-        <v>102.0652</v>
+        <v>101.1285</v>
       </c>
       <c r="C37" t="n">
         <v>0</v>
       </c>
       <c r="D37" t="n">
-        <v>81.65216000000001</v>
+        <v>80.90280000000001</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>1416</v>
+        <v>374</v>
       </c>
       <c r="B38" t="n">
-        <v>92.411</v>
+        <v>100.92945</v>
       </c>
       <c r="C38" t="n">
         <v>0</v>
       </c>
       <c r="D38" t="n">
-        <v>73.92880000000001</v>
+        <v>80.74356</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="n">
-        <v>1137</v>
+        <v>1567</v>
       </c>
       <c r="B39" t="n">
-        <v>89.16286666666667</v>
+        <v>88.06193333333333</v>
       </c>
       <c r="C39" t="n">
         <v>0</v>
       </c>
       <c r="D39" t="n">
-        <v>71.33029333333334</v>
+        <v>70.44954666666666</v>
       </c>
     </row>
     <row r="40">
@@ -992,41 +992,41 @@
         <v>486</v>
       </c>
       <c r="B40" t="n">
-        <v>88.39190000000001</v>
+        <v>87.16293333333333</v>
       </c>
       <c r="C40" t="n">
         <v>0</v>
       </c>
       <c r="D40" t="n">
-        <v>70.71352</v>
+        <v>69.73034666666666</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="n">
-        <v>1626</v>
+        <v>250</v>
       </c>
       <c r="B41" t="n">
-        <v>87.50266666666668</v>
+        <v>86.11486666666667</v>
       </c>
       <c r="C41" t="n">
         <v>0</v>
       </c>
       <c r="D41" t="n">
-        <v>70.00213333333335</v>
+        <v>68.89189333333334</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="n">
-        <v>449</v>
+        <v>2462</v>
       </c>
       <c r="B42" t="n">
-        <v>85.85239999999999</v>
+        <v>85.92726666666665</v>
       </c>
       <c r="C42" t="n">
         <v>0</v>
       </c>
       <c r="D42" t="n">
-        <v>68.68191999999999</v>
+        <v>68.74181333333333</v>
       </c>
     </row>
     <row r="43">
@@ -1034,41 +1034,41 @@
         <v>1623</v>
       </c>
       <c r="B43" t="n">
-        <v>85.64236666666666</v>
+        <v>84.36866666666667</v>
       </c>
       <c r="C43" t="n">
         <v>0</v>
       </c>
       <c r="D43" t="n">
-        <v>68.51389333333333</v>
+        <v>67.49493333333334</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="n">
-        <v>548</v>
+        <v>287</v>
       </c>
       <c r="B44" t="n">
-        <v>85.60743333333335</v>
+        <v>84.14733333333334</v>
       </c>
       <c r="C44" t="n">
         <v>0</v>
       </c>
       <c r="D44" t="n">
-        <v>68.48594666666668</v>
+        <v>67.31786666666667</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="n">
-        <v>437</v>
+        <v>1137</v>
       </c>
       <c r="B45" t="n">
-        <v>85.38226666666667</v>
+        <v>83.91686666666666</v>
       </c>
       <c r="C45" t="n">
         <v>0</v>
       </c>
       <c r="D45" t="n">
-        <v>68.30581333333333</v>
+        <v>67.13349333333333</v>
       </c>
     </row>
     <row r="46">
@@ -1076,783 +1076,783 @@
         <v>2543</v>
       </c>
       <c r="B46" t="n">
-        <v>84.06773333333332</v>
+        <v>82.80293333333333</v>
       </c>
       <c r="C46" t="n">
         <v>0</v>
       </c>
       <c r="D46" t="n">
-        <v>67.25418666666666</v>
+        <v>66.24234666666666</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="n">
-        <v>1141</v>
+        <v>1624</v>
       </c>
       <c r="B47" t="n">
-        <v>83.5256</v>
+        <v>82.52924999999999</v>
       </c>
       <c r="C47" t="n">
         <v>0</v>
       </c>
       <c r="D47" t="n">
-        <v>66.82048</v>
+        <v>66.0234</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="n">
-        <v>569</v>
+        <v>1416</v>
       </c>
       <c r="B48" t="n">
-        <v>83.26793333333335</v>
+        <v>78.2962</v>
       </c>
       <c r="C48" t="n">
         <v>0</v>
       </c>
       <c r="D48" t="n">
-        <v>66.61434666666668</v>
+        <v>62.63696</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="n">
-        <v>1624</v>
+        <v>710</v>
       </c>
       <c r="B49" t="n">
-        <v>81.49635000000001</v>
+        <v>75.87960000000001</v>
       </c>
       <c r="C49" t="n">
         <v>0</v>
       </c>
       <c r="D49" t="n">
-        <v>65.19708000000001</v>
+        <v>60.70368000000001</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="n">
-        <v>710</v>
+        <v>1128</v>
       </c>
       <c r="B50" t="n">
-        <v>75.459</v>
+        <v>75.50800000000001</v>
       </c>
       <c r="C50" t="n">
         <v>0</v>
       </c>
       <c r="D50" t="n">
-        <v>60.3672</v>
+        <v>60.40640000000001</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="n">
-        <v>521</v>
+        <v>449</v>
       </c>
       <c r="B51" t="n">
-        <v>73.844525</v>
+        <v>74.97212500000001</v>
       </c>
       <c r="C51" t="n">
         <v>0</v>
       </c>
       <c r="D51" t="n">
-        <v>59.07562000000001</v>
+        <v>59.97770000000001</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="n">
-        <v>2365</v>
+        <v>34273</v>
       </c>
       <c r="B52" t="n">
         <v>0</v>
       </c>
       <c r="C52" t="n">
-        <v>0.7919843196868896</v>
+        <v>0.7947285175323486</v>
       </c>
       <c r="D52" t="n">
-        <v>0.111608119447689</v>
+        <v>0.1114374670298262</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="n">
-        <v>2028</v>
+        <v>35689</v>
       </c>
       <c r="B53" t="n">
         <v>0</v>
       </c>
       <c r="C53" t="n">
-        <v>0.7929881811141968</v>
+        <v>0.7948347330093384</v>
       </c>
       <c r="D53" t="n">
-        <v>0.1115456320943043</v>
+        <v>0.1114308723370128</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="n">
-        <v>154</v>
+        <v>35727</v>
       </c>
       <c r="B54" t="n">
         <v>0</v>
       </c>
       <c r="C54" t="n">
-        <v>0.7935357093811035</v>
+        <v>0.7954474091529846</v>
       </c>
       <c r="D54" t="n">
-        <v>0.1115115795876817</v>
+        <v>0.111392847810759</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="n">
-        <v>173</v>
+        <v>35183</v>
       </c>
       <c r="B55" t="n">
         <v>0</v>
       </c>
       <c r="C55" t="n">
-        <v>0.7946640253067017</v>
+        <v>0.7967748045921326</v>
       </c>
       <c r="D55" t="n">
-        <v>0.1114414715956769</v>
+        <v>0.1113105546053112</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="n">
-        <v>134</v>
+        <v>34284</v>
       </c>
       <c r="B56" t="n">
         <v>0</v>
       </c>
       <c r="C56" t="n">
-        <v>0.7952176332473755</v>
+        <v>0.7980194687843323</v>
       </c>
       <c r="D56" t="n">
-        <v>0.1114071053536942</v>
+        <v>0.1112335007891894</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="n">
-        <v>30</v>
+        <v>35390</v>
       </c>
       <c r="B57" t="n">
         <v>0</v>
       </c>
       <c r="C57" t="n">
-        <v>0.801016628742218</v>
+        <v>0.7995876669883728</v>
       </c>
       <c r="D57" t="n">
-        <v>0.1110483916740262</v>
+        <v>0.1111365695980246</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="n">
-        <v>2193</v>
+        <v>35894</v>
       </c>
       <c r="B58" t="n">
         <v>0</v>
       </c>
       <c r="C58" t="n">
-        <v>0.8016068041324615</v>
+        <v>0.7999286651611328</v>
       </c>
       <c r="D58" t="n">
-        <v>0.1110120141316336</v>
+        <v>0.1111155146707415</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="n">
-        <v>1</v>
+        <v>33453</v>
       </c>
       <c r="B59" t="n">
         <v>0</v>
       </c>
       <c r="C59" t="n">
-        <v>0.8025662899017334</v>
+        <v>0.8051826953887939</v>
       </c>
       <c r="D59" t="n">
-        <v>0.1109529236846557</v>
+        <v>0.1107921101342735</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="n">
-        <v>2027</v>
+        <v>34601</v>
       </c>
       <c r="B60" t="n">
         <v>0</v>
       </c>
       <c r="C60" t="n">
-        <v>0.8076810836791992</v>
+        <v>0.806787371635437</v>
       </c>
       <c r="D60" t="n">
-        <v>0.1106389848329536</v>
+        <v>0.110693711468089</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="n">
-        <v>922</v>
+        <v>35971</v>
       </c>
       <c r="B61" t="n">
         <v>0</v>
       </c>
       <c r="C61" t="n">
-        <v>0.8079972565174103</v>
+        <v>0.8079086542129517</v>
       </c>
       <c r="D61" t="n">
-        <v>0.1106196368822168</v>
+        <v>0.1106250581487853</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="n">
-        <v>2609</v>
+        <v>35389</v>
       </c>
       <c r="B62" t="n">
         <v>0</v>
       </c>
       <c r="C62" t="n">
-        <v>0.8097895681858063</v>
+        <v>0.8087045550346375</v>
       </c>
       <c r="D62" t="n">
-        <v>0.1105100855457393</v>
+        <v>0.1105763787918198</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="n">
-        <v>1845</v>
+        <v>34491</v>
       </c>
       <c r="B63" t="n">
         <v>0</v>
       </c>
       <c r="C63" t="n">
-        <v>0.8100429177284241</v>
+        <v>0.8089724779129028</v>
       </c>
       <c r="D63" t="n">
-        <v>0.1104946175812212</v>
+        <v>0.1105600015710297</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="n">
-        <v>1051</v>
+        <v>34413</v>
       </c>
       <c r="B64" t="n">
         <v>0</v>
       </c>
       <c r="C64" t="n">
-        <v>0.8100535869598389</v>
+        <v>0.8095214366912842</v>
       </c>
       <c r="D64" t="n">
-        <v>0.1104939662786003</v>
+        <v>0.1105264607230631</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="n">
-        <v>568</v>
+        <v>34282</v>
       </c>
       <c r="B65" t="n">
         <v>0</v>
       </c>
       <c r="C65" t="n">
-        <v>0.8100799918174744</v>
+        <v>0.8104520440101624</v>
       </c>
       <c r="D65" t="n">
-        <v>0.1104923544285924</v>
+        <v>0.110469647987471</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="n">
-        <v>911</v>
+        <v>33568</v>
       </c>
       <c r="B66" t="n">
         <v>0</v>
       </c>
       <c r="C66" t="n">
-        <v>0.8102043271064758</v>
+        <v>0.8106575608253479</v>
       </c>
       <c r="D66" t="n">
-        <v>0.1104847651754818</v>
+        <v>0.110457109244243</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="n">
-        <v>1164</v>
+        <v>33672</v>
       </c>
       <c r="B67" t="n">
         <v>0</v>
       </c>
       <c r="C67" t="n">
-        <v>0.8107594847679138</v>
+        <v>0.811141312122345</v>
       </c>
       <c r="D67" t="n">
-        <v>0.110450891839804</v>
+        <v>0.1104276064277031</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="n">
-        <v>2153</v>
+        <v>35729</v>
       </c>
       <c r="B68" t="n">
         <v>0</v>
       </c>
       <c r="C68" t="n">
-        <v>0.8109683990478516</v>
+        <v>0.8117290735244751</v>
       </c>
       <c r="D68" t="n">
-        <v>0.1104381501660402</v>
+        <v>0.1103917814880163</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="n">
-        <v>2156</v>
+        <v>34958</v>
       </c>
       <c r="B69" t="n">
         <v>0</v>
       </c>
       <c r="C69" t="n">
-        <v>0.8109684189160665</v>
+        <v>0.8124069571495056</v>
       </c>
       <c r="D69" t="n">
-        <v>0.1104381489544183</v>
+        <v>0.1103504923168875</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="n">
-        <v>137</v>
+        <v>33930</v>
       </c>
       <c r="B70" t="n">
         <v>0</v>
       </c>
       <c r="C70" t="n">
-        <v>0.8110103805859884</v>
+        <v>0.812431663274765</v>
       </c>
       <c r="D70" t="n">
-        <v>0.1104355900683938</v>
+        <v>0.1103489880764017</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="n">
-        <v>91</v>
+        <v>35192</v>
       </c>
       <c r="B71" t="n">
         <v>0</v>
       </c>
       <c r="C71" t="n">
-        <v>0.8118703067302704</v>
+        <v>0.8136908411979675</v>
       </c>
       <c r="D71" t="n">
-        <v>0.1103831765756585</v>
+        <v>0.1102723768886087</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="n">
-        <v>2093</v>
+        <v>35607</v>
       </c>
       <c r="B72" t="n">
         <v>0</v>
       </c>
       <c r="C72" t="n">
-        <v>0.8120065927505493</v>
+        <v>0.8139218389987946</v>
       </c>
       <c r="D72" t="n">
-        <v>0.1103748743520897</v>
+        <v>0.1102583340142105</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="n">
-        <v>1135</v>
+        <v>34699</v>
       </c>
       <c r="B73" t="n">
         <v>0</v>
       </c>
       <c r="C73" t="n">
-        <v>0.8121118545532227</v>
+        <v>0.8139218389987946</v>
       </c>
       <c r="D73" t="n">
-        <v>0.1103684629055694</v>
+        <v>0.1102583340142105</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="n">
-        <v>1289</v>
+        <v>35524</v>
       </c>
       <c r="B74" t="n">
         <v>0</v>
       </c>
       <c r="C74" t="n">
-        <v>0.8122626344362894</v>
+        <v>0.8142833411693573</v>
       </c>
       <c r="D74" t="n">
-        <v>0.1103592802718745</v>
+        <v>0.1102363646634678</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="n">
-        <v>310</v>
+        <v>34581</v>
       </c>
       <c r="B75" t="n">
         <v>0</v>
       </c>
       <c r="C75" t="n">
-        <v>0.8126060565312704</v>
+        <v>0.8162015676498413</v>
       </c>
       <c r="D75" t="n">
-        <v>0.1103383712524573</v>
+        <v>0.1101199357837794</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="n">
-        <v>863</v>
+        <v>35521</v>
       </c>
       <c r="B76" t="n">
         <v>0</v>
       </c>
       <c r="C76" t="n">
-        <v>0.8128691911697388</v>
+        <v>0.8182508945465088</v>
       </c>
       <c r="D76" t="n">
-        <v>0.1103223558402202</v>
+        <v>0.1099958210387033</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="n">
-        <v>2367</v>
+        <v>34535</v>
       </c>
       <c r="B77" t="n">
         <v>0</v>
       </c>
       <c r="C77" t="n">
-        <v>0.8128746549288431</v>
+        <v>0.8182583451271057</v>
       </c>
       <c r="D77" t="n">
-        <v>0.1103220233435556</v>
+        <v>0.1099953703146727</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="n">
-        <v>2162</v>
+        <v>33499</v>
       </c>
       <c r="B78" t="n">
         <v>0</v>
       </c>
       <c r="C78" t="n">
-        <v>0.8143606384595236</v>
+        <v>0.8183606863021851</v>
       </c>
       <c r="D78" t="n">
-        <v>0.1102316682585273</v>
+        <v>0.1099891795432069</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="n">
-        <v>206</v>
+        <v>34522</v>
       </c>
       <c r="B79" t="n">
         <v>0</v>
       </c>
       <c r="C79" t="n">
-        <v>0.8154852390289307</v>
+        <v>0.8190566301345825</v>
       </c>
       <c r="D79" t="n">
-        <v>0.1101633853586032</v>
+        <v>0.109947099329834</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="n">
-        <v>1596</v>
+        <v>35518</v>
       </c>
       <c r="B80" t="n">
         <v>0</v>
       </c>
       <c r="C80" t="n">
-        <v>0.8158687353134155</v>
+        <v>0.8191812038421631</v>
       </c>
       <c r="D80" t="n">
-        <v>0.1101401197732943</v>
+        <v>0.1099395703834199</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="n">
-        <v>1059</v>
+        <v>34421</v>
       </c>
       <c r="B81" t="n">
         <v>0</v>
       </c>
       <c r="C81" t="n">
-        <v>0.8158804376920065</v>
+        <v>0.819238692522049</v>
       </c>
       <c r="D81" t="n">
-        <v>0.1101394099791069</v>
+        <v>0.1099360962484454</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="n">
-        <v>1160</v>
+        <v>34202</v>
       </c>
       <c r="B82" t="n">
         <v>0</v>
       </c>
       <c r="C82" t="n">
-        <v>0.8158887624740601</v>
+        <v>0.8196812272071838</v>
       </c>
       <c r="D82" t="n">
-        <v>0.110138905054685</v>
+        <v>0.1099093605020901</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="n">
-        <v>1092</v>
+        <v>34585</v>
       </c>
       <c r="B83" t="n">
         <v>0</v>
       </c>
       <c r="C83" t="n">
-        <v>0.8159446120262146</v>
+        <v>0.8210065364837646</v>
       </c>
       <c r="D83" t="n">
-        <v>0.1101355177220091</v>
+        <v>0.1098293696332282</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="n">
-        <v>1173</v>
+        <v>33378</v>
       </c>
       <c r="B84" t="n">
         <v>0</v>
       </c>
       <c r="C84" t="n">
-        <v>0.8173214197158813</v>
+        <v>0.8211919069290161</v>
       </c>
       <c r="D84" t="n">
-        <v>0.1100520787518522</v>
+        <v>0.109818190625089</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="n">
-        <v>1129</v>
+        <v>34497</v>
       </c>
       <c r="B85" t="n">
         <v>0</v>
       </c>
       <c r="C85" t="n">
-        <v>0.8178887665271759</v>
+        <v>0.821530818939209</v>
       </c>
       <c r="D85" t="n">
-        <v>0.1100177324831993</v>
+        <v>0.109797757973962</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="n">
-        <v>2165</v>
+        <v>33363</v>
       </c>
       <c r="B86" t="n">
         <v>0</v>
       </c>
       <c r="C86" t="n">
-        <v>0.818576455116272</v>
+        <v>0.8228433132171631</v>
       </c>
       <c r="D86" t="n">
-        <v>0.1099761296465332</v>
+        <v>0.109718700751639</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="n">
-        <v>2245</v>
+        <v>35893</v>
       </c>
       <c r="B87" t="n">
         <v>0</v>
       </c>
       <c r="C87" t="n">
-        <v>0.8187365531921387</v>
+        <v>0.8229777216911316</v>
       </c>
       <c r="D87" t="n">
-        <v>0.1099664487684991</v>
+        <v>0.1097106111721787</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="n">
-        <v>1337</v>
+        <v>34526</v>
       </c>
       <c r="B88" t="n">
         <v>0</v>
       </c>
       <c r="C88" t="n">
-        <v>0.8187365531921387</v>
+        <v>0.8232136964797974</v>
       </c>
       <c r="D88" t="n">
-        <v>0.1099664487684991</v>
+        <v>0.1096964115540343</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="n">
-        <v>840</v>
+        <v>34808</v>
       </c>
       <c r="B89" t="n">
         <v>0</v>
       </c>
       <c r="C89" t="n">
-        <v>0.819239616394043</v>
+        <v>0.823243111371994</v>
       </c>
       <c r="D89" t="n">
-        <v>0.1099360404191421</v>
+        <v>0.1096946417910772</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="n">
-        <v>1223</v>
+        <v>35892</v>
       </c>
       <c r="B90" t="n">
         <v>0</v>
       </c>
       <c r="C90" t="n">
-        <v>0.8193921049435934</v>
+        <v>0.8232634365558624</v>
       </c>
       <c r="D90" t="n">
-        <v>0.1099268263595112</v>
+        <v>0.1096934189487172</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="n">
-        <v>1446</v>
+        <v>34454</v>
       </c>
       <c r="B91" t="n">
         <v>0</v>
       </c>
       <c r="C91" t="n">
-        <v>0.8217453956604004</v>
+        <v>0.8237894177436829</v>
       </c>
       <c r="D91" t="n">
-        <v>0.1097848252979929</v>
+        <v>0.1096617833474611</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="n">
-        <v>575</v>
+        <v>34651</v>
       </c>
       <c r="B92" t="n">
         <v>0</v>
       </c>
       <c r="C92" t="n">
-        <v>0.8217646479606628</v>
+        <v>0.8246003389358521</v>
       </c>
       <c r="D92" t="n">
-        <v>0.1097836650984999</v>
+        <v>0.109613045515844</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="n">
-        <v>1239</v>
+        <v>34599</v>
       </c>
       <c r="B93" t="n">
         <v>0</v>
       </c>
       <c r="C93" t="n">
-        <v>0.8224078416824341</v>
+        <v>0.8247575759887695</v>
       </c>
       <c r="D93" t="n">
-        <v>0.1097449184675157</v>
+        <v>0.1096036002983176</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="n">
-        <v>2530</v>
+        <v>35550</v>
       </c>
       <c r="B94" t="n">
         <v>0</v>
       </c>
       <c r="C94" t="n">
-        <v>0.8226067622502645</v>
+        <v>0.8248059153556824</v>
       </c>
       <c r="D94" t="n">
-        <v>0.1097329408308964</v>
+        <v>0.1096006968834365</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="n">
-        <v>2202</v>
+        <v>33880</v>
       </c>
       <c r="B95" t="n">
         <v>0</v>
       </c>
       <c r="C95" t="n">
-        <v>0.8228475451469421</v>
+        <v>0.8248580098152161</v>
       </c>
       <c r="D95" t="n">
-        <v>0.1097184460282869</v>
+        <v>0.1095975680980527</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="n">
-        <v>2531</v>
+        <v>35824</v>
       </c>
       <c r="B96" t="n">
         <v>0</v>
       </c>
       <c r="C96" t="n">
-        <v>0.8230937719345093</v>
+        <v>0.825376033782959</v>
       </c>
       <c r="D96" t="n">
-        <v>0.1097036274704495</v>
+        <v>0.1095664653739945</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="n">
-        <v>920</v>
+        <v>35527</v>
       </c>
       <c r="B97" t="n">
         <v>0</v>
       </c>
       <c r="C97" t="n">
-        <v>0.8231211006641388</v>
+        <v>0.825574000676473</v>
       </c>
       <c r="D97" t="n">
-        <v>0.1097019830043888</v>
+        <v>0.1095545838875276</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="n">
-        <v>1219</v>
+        <v>33937</v>
       </c>
       <c r="B98" t="n">
         <v>0</v>
       </c>
       <c r="C98" t="n">
-        <v>0.8234641551971436</v>
+        <v>0.8258347809314728</v>
       </c>
       <c r="D98" t="n">
-        <v>0.1096813443960334</v>
+        <v>0.1095389364299257</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="n">
-        <v>2196</v>
+        <v>35619</v>
       </c>
       <c r="B99" t="n">
         <v>0</v>
       </c>
       <c r="C99" t="n">
-        <v>0.8266289234161377</v>
+        <v>0.8260629177093506</v>
       </c>
       <c r="D99" t="n">
-        <v>0.1094913134442011</v>
+        <v>0.1095252513264351</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="n">
-        <v>2026</v>
+        <v>34711</v>
       </c>
       <c r="B100" t="n">
         <v>0</v>
       </c>
       <c r="C100" t="n">
-        <v>0.8273717959721884</v>
+        <v>0.8260629177093506</v>
       </c>
       <c r="D100" t="n">
-        <v>0.1094468024738212</v>
+        <v>0.1095252513264351</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="n">
-        <v>1216</v>
+        <v>35558</v>
       </c>
       <c r="B101" t="n">
         <v>0</v>
       </c>
       <c r="C101" t="n">
-        <v>0.8353588779767355</v>
+        <v>0.8262338638305664</v>
       </c>
       <c r="D101" t="n">
-        <v>0.1089705138324098</v>
+        <v>0.1095149991253013</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Intergrated DeepSeek/Grok --> testing
DeepSeek hallucinated still too much, however, they use a larger amount of genes. --> what to do? Also should intergrate the hallucination calculation into the workflow
</commit_message>
<xml_diff>
--- a/output/scores.xlsx
+++ b/output/scores.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D100"/>
+  <dimension ref="A1:D101"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -457,548 +457,548 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>2551</v>
+        <v>2450</v>
       </c>
       <c r="B2" t="n">
-        <v>169.6164</v>
+        <v>169.6026</v>
       </c>
       <c r="C2" t="n">
         <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>118.73148</v>
+        <v>118.72182</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>2450</v>
+        <v>1689</v>
       </c>
       <c r="B3" t="n">
-        <v>169.6026</v>
+        <v>168.1452</v>
       </c>
       <c r="C3" t="n">
         <v>0</v>
       </c>
       <c r="D3" t="n">
-        <v>118.72182</v>
+        <v>117.70164</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>1207</v>
+        <v>908</v>
       </c>
       <c r="B4" t="n">
-        <v>167.9877</v>
+        <v>166.4251</v>
       </c>
       <c r="C4" t="n">
         <v>0</v>
       </c>
       <c r="D4" t="n">
-        <v>117.59139</v>
+        <v>116.49757</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>1206</v>
+        <v>243</v>
       </c>
       <c r="B5" t="n">
-        <v>167.8389</v>
+        <v>165.8187</v>
       </c>
       <c r="C5" t="n">
         <v>0</v>
       </c>
       <c r="D5" t="n">
-        <v>117.48723</v>
+        <v>116.07309</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>2518</v>
+        <v>903</v>
       </c>
       <c r="B6" t="n">
-        <v>167.5263</v>
+        <v>165.0349</v>
       </c>
       <c r="C6" t="n">
         <v>0</v>
       </c>
       <c r="D6" t="n">
-        <v>117.26841</v>
+        <v>115.52443</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>2257</v>
+        <v>967</v>
       </c>
       <c r="B7" t="n">
-        <v>167.1356</v>
+        <v>164.6438</v>
       </c>
       <c r="C7" t="n">
         <v>0</v>
       </c>
       <c r="D7" t="n">
-        <v>116.99492</v>
+        <v>115.25066</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>1349</v>
+        <v>509</v>
       </c>
       <c r="B8" t="n">
-        <v>167.1356</v>
+        <v>164.6222</v>
       </c>
       <c r="C8" t="n">
         <v>0</v>
       </c>
       <c r="D8" t="n">
-        <v>116.99492</v>
+        <v>115.23554</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>908</v>
+        <v>1586</v>
       </c>
       <c r="B9" t="n">
-        <v>166.4251</v>
+        <v>163.8001</v>
       </c>
       <c r="C9" t="n">
         <v>0</v>
       </c>
       <c r="D9" t="n">
-        <v>116.49757</v>
+        <v>114.66007</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>903</v>
+        <v>1469</v>
       </c>
       <c r="B10" t="n">
-        <v>165.0349</v>
+        <v>163.7061</v>
       </c>
       <c r="C10" t="n">
         <v>0</v>
       </c>
       <c r="D10" t="n">
-        <v>115.52443</v>
+        <v>114.59427</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>967</v>
+        <v>1580</v>
       </c>
       <c r="B11" t="n">
-        <v>164.6438</v>
+        <v>163.5039</v>
       </c>
       <c r="C11" t="n">
         <v>0</v>
       </c>
       <c r="D11" t="n">
-        <v>115.25066</v>
+        <v>114.45273</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>1548</v>
+        <v>2328</v>
       </c>
       <c r="B12" t="n">
-        <v>164.2457</v>
+        <v>163.3697</v>
       </c>
       <c r="C12" t="n">
         <v>0</v>
       </c>
       <c r="D12" t="n">
-        <v>114.97199</v>
+        <v>114.35879</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>1469</v>
+        <v>259</v>
       </c>
       <c r="B13" t="n">
-        <v>163.7061</v>
+        <v>162.6408</v>
       </c>
       <c r="C13" t="n">
         <v>0</v>
       </c>
       <c r="D13" t="n">
-        <v>114.59427</v>
+        <v>113.84856</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>1580</v>
+        <v>2451</v>
       </c>
       <c r="B14" t="n">
-        <v>163.5039</v>
+        <v>106.3287</v>
       </c>
       <c r="C14" t="n">
         <v>0</v>
       </c>
       <c r="D14" t="n">
-        <v>114.45273</v>
+        <v>74.43008999999999</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>2328</v>
+        <v>553</v>
       </c>
       <c r="B15" t="n">
-        <v>163.3697</v>
+        <v>105.20635</v>
       </c>
       <c r="C15" t="n">
         <v>0</v>
       </c>
       <c r="D15" t="n">
-        <v>114.35879</v>
+        <v>73.64444499999999</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>1418</v>
+        <v>2257</v>
       </c>
       <c r="B16" t="n">
-        <v>162.8837</v>
+        <v>102.63345</v>
       </c>
       <c r="C16" t="n">
         <v>0</v>
       </c>
       <c r="D16" t="n">
-        <v>114.01859</v>
+        <v>71.84341500000001</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>259</v>
+        <v>1349</v>
       </c>
       <c r="B17" t="n">
-        <v>162.6408</v>
+        <v>102.63345</v>
       </c>
       <c r="C17" t="n">
         <v>0</v>
       </c>
       <c r="D17" t="n">
-        <v>113.84856</v>
+        <v>71.84341500000001</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>1616</v>
+        <v>2551</v>
       </c>
       <c r="B18" t="n">
-        <v>162.6108</v>
+        <v>102.4392</v>
       </c>
       <c r="C18" t="n">
         <v>0</v>
       </c>
       <c r="D18" t="n">
-        <v>113.82756</v>
+        <v>71.70743999999999</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>1590</v>
+        <v>1207</v>
       </c>
       <c r="B19" t="n">
-        <v>105.6366</v>
+        <v>102.38385</v>
       </c>
       <c r="C19" t="n">
         <v>0</v>
       </c>
       <c r="D19" t="n">
-        <v>73.94561999999999</v>
+        <v>71.66869499999999</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>387</v>
+        <v>287</v>
       </c>
       <c r="B20" t="n">
-        <v>104.4184</v>
+        <v>102.2776</v>
       </c>
       <c r="C20" t="n">
         <v>0</v>
       </c>
       <c r="D20" t="n">
-        <v>73.09287999999999</v>
+        <v>71.59432</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>1689</v>
+        <v>2526</v>
       </c>
       <c r="B21" t="n">
-        <v>104.26165</v>
+        <v>102.0947</v>
       </c>
       <c r="C21" t="n">
         <v>0</v>
       </c>
       <c r="D21" t="n">
-        <v>72.983155</v>
+        <v>71.46629</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>287</v>
+        <v>1206</v>
       </c>
       <c r="B22" t="n">
-        <v>102.52505</v>
+        <v>101.69845</v>
       </c>
       <c r="C22" t="n">
         <v>0</v>
       </c>
       <c r="D22" t="n">
-        <v>71.767535</v>
+        <v>71.18891499999999</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>243</v>
+        <v>1623</v>
       </c>
       <c r="B23" t="n">
-        <v>102.47305</v>
+        <v>101.3795</v>
       </c>
       <c r="C23" t="n">
         <v>0</v>
       </c>
       <c r="D23" t="n">
-        <v>71.73113499999999</v>
+        <v>70.96565</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>509</v>
+        <v>1418</v>
       </c>
       <c r="B24" t="n">
-        <v>102.00805</v>
+        <v>100.3693</v>
       </c>
       <c r="C24" t="n">
         <v>0</v>
       </c>
       <c r="D24" t="n">
-        <v>71.40563499999999</v>
+        <v>70.25851</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>1623</v>
+        <v>1548</v>
       </c>
       <c r="B25" t="n">
-        <v>101.9785</v>
+        <v>99.9876</v>
       </c>
       <c r="C25" t="n">
         <v>0</v>
       </c>
       <c r="D25" t="n">
-        <v>71.38494999999999</v>
+        <v>69.99132</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>2526</v>
+        <v>527</v>
       </c>
       <c r="B26" t="n">
-        <v>101.40945</v>
+        <v>84.99496666666667</v>
       </c>
       <c r="C26" t="n">
-        <v>0.7846416831016541</v>
+        <v>0</v>
       </c>
       <c r="D26" t="n">
-        <v>71.15471597110285</v>
+        <v>59.49647666666667</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>1586</v>
+        <v>2462</v>
       </c>
       <c r="B27" t="n">
-        <v>99.85995</v>
+        <v>83.30613333333334</v>
       </c>
       <c r="C27" t="n">
         <v>0</v>
       </c>
       <c r="D27" t="n">
-        <v>69.90196499999999</v>
+        <v>58.31429333333333</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>527</v>
+        <v>1590</v>
       </c>
       <c r="B28" t="n">
-        <v>86.35820000000001</v>
+        <v>83.0939</v>
       </c>
       <c r="C28" t="n">
         <v>0</v>
       </c>
       <c r="D28" t="n">
-        <v>60.45074</v>
+        <v>58.16573</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>1567</v>
+        <v>548</v>
       </c>
       <c r="B29" t="n">
-        <v>84.1725</v>
+        <v>82.03213333333333</v>
       </c>
       <c r="C29" t="n">
         <v>0</v>
       </c>
       <c r="D29" t="n">
-        <v>58.92075</v>
+        <v>57.42249333333333</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>374</v>
+        <v>1567</v>
       </c>
       <c r="B30" t="n">
-        <v>82.08916666666667</v>
+        <v>81.82463333333332</v>
       </c>
       <c r="C30" t="n">
         <v>0</v>
       </c>
       <c r="D30" t="n">
-        <v>57.46241666666666</v>
+        <v>57.27724333333332</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>1626</v>
+        <v>2518</v>
       </c>
       <c r="B31" t="n">
-        <v>81.91876666666667</v>
+        <v>81.79363333333333</v>
       </c>
       <c r="C31" t="n">
         <v>0</v>
       </c>
       <c r="D31" t="n">
-        <v>57.34313666666667</v>
+        <v>57.25554333333333</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>780</v>
+        <v>437</v>
       </c>
       <c r="B32" t="n">
-        <v>81.89626666666668</v>
+        <v>81.72113333333333</v>
       </c>
       <c r="C32" t="n">
         <v>0</v>
       </c>
       <c r="D32" t="n">
-        <v>57.32738666666667</v>
+        <v>57.20479333333333</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>709</v>
+        <v>1626</v>
       </c>
       <c r="B33" t="n">
-        <v>81.4165</v>
+        <v>80.9735</v>
       </c>
       <c r="C33" t="n">
         <v>0</v>
       </c>
       <c r="D33" t="n">
-        <v>56.99155</v>
+        <v>56.68145</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>2543</v>
+        <v>780</v>
       </c>
       <c r="B34" t="n">
-        <v>80.7157</v>
+        <v>80.8253</v>
       </c>
       <c r="C34" t="n">
         <v>0</v>
       </c>
       <c r="D34" t="n">
-        <v>56.50098999999999</v>
+        <v>56.57771</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>1416</v>
+        <v>709</v>
       </c>
       <c r="B35" t="n">
-        <v>76.302975</v>
+        <v>80.79979999999999</v>
       </c>
       <c r="C35" t="n">
         <v>0</v>
       </c>
       <c r="D35" t="n">
-        <v>53.4120825</v>
+        <v>56.55985999999999</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>2451</v>
+        <v>387</v>
       </c>
       <c r="B36" t="n">
-        <v>73.94217499999999</v>
+        <v>80.2456</v>
       </c>
       <c r="C36" t="n">
         <v>0</v>
       </c>
       <c r="D36" t="n">
-        <v>51.75952249999999</v>
+        <v>56.17191999999999</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>2462</v>
+        <v>1141</v>
       </c>
       <c r="B37" t="n">
-        <v>73.26342500000001</v>
+        <v>80.22959999999999</v>
       </c>
       <c r="C37" t="n">
         <v>0</v>
       </c>
       <c r="D37" t="n">
-        <v>51.2843975</v>
+        <v>56.16071999999999</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>250</v>
+        <v>2543</v>
       </c>
       <c r="B38" t="n">
-        <v>72.60797500000001</v>
+        <v>80.20846666666667</v>
       </c>
       <c r="C38" t="n">
         <v>0</v>
       </c>
       <c r="D38" t="n">
-        <v>50.8255825</v>
+        <v>56.14592666666666</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="n">
-        <v>1624</v>
+        <v>1616</v>
       </c>
       <c r="B39" t="n">
-        <v>71.85972</v>
+        <v>79.84310000000001</v>
       </c>
       <c r="C39" t="n">
         <v>0</v>
       </c>
       <c r="D39" t="n">
-        <v>50.301804</v>
+        <v>55.89017</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="n">
-        <v>1141</v>
+        <v>374</v>
       </c>
       <c r="B40" t="n">
-        <v>70.7527</v>
+        <v>79.35626666666667</v>
       </c>
       <c r="C40" t="n">
         <v>0</v>
       </c>
       <c r="D40" t="n">
-        <v>49.52689</v>
+        <v>55.54938666666666</v>
       </c>
     </row>
     <row r="41">
@@ -1006,839 +1006,853 @@
         <v>521</v>
       </c>
       <c r="B41" t="n">
-        <v>70.460425</v>
+        <v>79.02629999999999</v>
       </c>
       <c r="C41" t="n">
         <v>0</v>
       </c>
       <c r="D41" t="n">
-        <v>49.3222975</v>
+        <v>55.31840999999999</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="n">
-        <v>553</v>
+        <v>1624</v>
       </c>
       <c r="B42" t="n">
-        <v>70.21334999999999</v>
+        <v>72.98238000000001</v>
       </c>
       <c r="C42" t="n">
         <v>0</v>
       </c>
       <c r="D42" t="n">
-        <v>49.14934499999999</v>
+        <v>51.087666</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="n">
-        <v>547</v>
+        <v>569</v>
       </c>
       <c r="B43" t="n">
-        <v>70.188075</v>
+        <v>69.35795</v>
       </c>
       <c r="C43" t="n">
         <v>0</v>
       </c>
       <c r="D43" t="n">
-        <v>49.13165249999999</v>
+        <v>48.550565</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="n">
-        <v>1128</v>
+        <v>1137</v>
       </c>
       <c r="B44" t="n">
-        <v>67.87804000000001</v>
+        <v>65.05354</v>
       </c>
       <c r="C44" t="n">
         <v>0</v>
       </c>
       <c r="D44" t="n">
-        <v>47.51462800000001</v>
+        <v>45.53747799999999</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="n">
-        <v>449</v>
+        <v>250</v>
       </c>
       <c r="B45" t="n">
-        <v>66.29274000000001</v>
+        <v>64.38118</v>
       </c>
       <c r="C45" t="n">
         <v>0</v>
       </c>
       <c r="D45" t="n">
-        <v>46.404918</v>
+        <v>45.066826</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="n">
-        <v>569</v>
+        <v>547</v>
       </c>
       <c r="B46" t="n">
-        <v>65.0853</v>
+        <v>62.93089999999999</v>
       </c>
       <c r="C46" t="n">
         <v>0</v>
       </c>
       <c r="D46" t="n">
-        <v>45.55971</v>
+        <v>44.05163</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="n">
-        <v>437</v>
+        <v>1416</v>
       </c>
       <c r="B47" t="n">
-        <v>64.6729</v>
+        <v>61.62113333333334</v>
       </c>
       <c r="C47" t="n">
         <v>0</v>
       </c>
       <c r="D47" t="n">
-        <v>45.27103</v>
+        <v>43.13479333333333</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="n">
-        <v>710</v>
+        <v>1128</v>
       </c>
       <c r="B48" t="n">
-        <v>62.77245</v>
+        <v>61.17085</v>
       </c>
       <c r="C48" t="n">
         <v>0</v>
       </c>
       <c r="D48" t="n">
-        <v>43.940715</v>
+        <v>42.819595</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="n">
-        <v>1137</v>
+        <v>486</v>
       </c>
       <c r="B49" t="n">
-        <v>62.60706666666666</v>
+        <v>60.68863333333334</v>
       </c>
       <c r="C49" t="n">
         <v>0</v>
       </c>
       <c r="D49" t="n">
-        <v>43.82494666666666</v>
+        <v>42.48204333333333</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="n">
-        <v>486</v>
+        <v>449</v>
       </c>
       <c r="B50" t="n">
-        <v>62.09870000000001</v>
+        <v>60.14265</v>
       </c>
       <c r="C50" t="n">
         <v>0</v>
       </c>
       <c r="D50" t="n">
-        <v>43.46909</v>
+        <v>42.099855</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="n">
-        <v>548</v>
+        <v>710</v>
       </c>
       <c r="B51" t="n">
-        <v>60.64171666666667</v>
+        <v>59.51236666666667</v>
       </c>
       <c r="C51" t="n">
         <v>0</v>
       </c>
       <c r="D51" t="n">
-        <v>42.44920166666667</v>
+        <v>41.65865666666667</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="n">
-        <v>971</v>
+        <v>34868</v>
       </c>
       <c r="B52" t="n">
         <v>0</v>
       </c>
       <c r="C52" t="n">
-        <v>0.7741959095001221</v>
+        <v>0.7822101712226868</v>
       </c>
       <c r="D52" t="n">
-        <v>0.1690906840634779</v>
+        <v>0.168330315270384</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="n">
-        <v>164</v>
+        <v>33624</v>
       </c>
       <c r="B53" t="n">
         <v>0</v>
       </c>
       <c r="C53" t="n">
-        <v>0.7744442820549011</v>
+        <v>0.7822558879852295</v>
       </c>
       <c r="D53" t="n">
-        <v>0.1690670160984621</v>
+        <v>0.1683259974184393</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="n">
-        <v>167</v>
+        <v>33483</v>
       </c>
       <c r="B54" t="n">
         <v>0</v>
       </c>
       <c r="C54" t="n">
-        <v>0.7745041847229004</v>
+        <v>0.7852948307991028</v>
       </c>
       <c r="D54" t="n">
-        <v>0.169061308833626</v>
+        <v>0.1680394715900898</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="n">
-        <v>2365</v>
+        <v>33507</v>
       </c>
       <c r="B55" t="n">
         <v>0</v>
       </c>
       <c r="C55" t="n">
-        <v>0.7750915288925171</v>
+        <v>0.7862100601196289</v>
       </c>
       <c r="D55" t="n">
-        <v>0.1690053696482741</v>
+        <v>0.1679533704898672</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="n">
-        <v>153</v>
+        <v>33516</v>
       </c>
       <c r="B56" t="n">
         <v>0</v>
       </c>
       <c r="C56" t="n">
-        <v>0.7755637168884277</v>
+        <v>0.7873714566230774</v>
       </c>
       <c r="D56" t="n">
-        <v>0.1689604248760684</v>
+        <v>0.1678442379105667</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="n">
-        <v>981</v>
+        <v>33541</v>
       </c>
       <c r="B57" t="n">
         <v>0</v>
       </c>
       <c r="C57" t="n">
-        <v>0.7759453654289246</v>
+        <v>0.7874562740325928</v>
       </c>
       <c r="D57" t="n">
-        <v>0.1689241154823163</v>
+        <v>0.1678362734564604</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="n">
-        <v>141</v>
+        <v>35894</v>
       </c>
       <c r="B58" t="n">
         <v>0</v>
       </c>
       <c r="C58" t="n">
-        <v>0.7761804461479187</v>
+        <v>0.7880964577198029</v>
       </c>
       <c r="D58" t="n">
-        <v>0.1689017580677815</v>
+        <v>0.1677761838321422</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="n">
-        <v>156</v>
+        <v>33535</v>
       </c>
       <c r="B59" t="n">
         <v>0</v>
       </c>
       <c r="C59" t="n">
-        <v>0.7775058746337891</v>
+        <v>0.7889856696128845</v>
       </c>
       <c r="D59" t="n">
-        <v>0.1687758135043056</v>
+        <v>0.1676927910020188</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="n">
-        <v>165</v>
+        <v>34243</v>
       </c>
       <c r="B60" t="n">
         <v>0</v>
       </c>
       <c r="C60" t="n">
-        <v>0.7775581479072571</v>
+        <v>0.7906647622585297</v>
       </c>
       <c r="D60" t="n">
-        <v>0.1687708502549939</v>
+        <v>0.1675355467550587</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="n">
-        <v>145</v>
+        <v>33412</v>
       </c>
       <c r="B61" t="n">
         <v>0</v>
       </c>
       <c r="C61" t="n">
-        <v>0.7780144214630127</v>
+        <v>0.7917564511299133</v>
       </c>
       <c r="D61" t="n">
-        <v>0.1687275403273442</v>
+        <v>0.1674334699957769</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="n">
-        <v>151</v>
+        <v>33363</v>
       </c>
       <c r="B62" t="n">
         <v>0</v>
       </c>
       <c r="C62" t="n">
-        <v>0.7782194018363953</v>
+        <v>0.7917799949645996</v>
       </c>
       <c r="D62" t="n">
-        <v>0.1687080906271663</v>
+        <v>0.1674312699344135</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="n">
-        <v>147</v>
+        <v>34601</v>
       </c>
       <c r="B63" t="n">
         <v>0</v>
       </c>
       <c r="C63" t="n">
-        <v>0.7794610261917114</v>
+        <v>0.7922704517841339</v>
       </c>
       <c r="D63" t="n">
-        <v>0.1685903740426621</v>
+        <v>0.167385452179587</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="n">
-        <v>169</v>
+        <v>35390</v>
       </c>
       <c r="B64" t="n">
         <v>0</v>
       </c>
       <c r="C64" t="n">
-        <v>0.7813576459884644</v>
+        <v>0.7928596287965775</v>
       </c>
       <c r="D64" t="n">
-        <v>0.1684108750848468</v>
+        <v>0.1673304452738273</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="n">
-        <v>136</v>
+        <v>35455</v>
       </c>
       <c r="B65" t="n">
         <v>0</v>
       </c>
       <c r="C65" t="n">
-        <v>0.7816736102104187</v>
+        <v>0.7935595512390137</v>
       </c>
       <c r="D65" t="n">
-        <v>0.1683810088900455</v>
+        <v>0.1672651458897789</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="n">
-        <v>1239</v>
+        <v>34026</v>
       </c>
       <c r="B66" t="n">
         <v>0</v>
       </c>
       <c r="C66" t="n">
-        <v>0.7825369238853455</v>
+        <v>0.794352650642395</v>
       </c>
       <c r="D66" t="n">
-        <v>0.1682994590351029</v>
+        <v>0.1671912151118105</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="n">
-        <v>174</v>
+        <v>35515</v>
       </c>
       <c r="B67" t="n">
         <v>0</v>
       </c>
       <c r="C67" t="n">
-        <v>0.7836213111877441</v>
+        <v>0.7945264577865601</v>
       </c>
       <c r="D67" t="n">
-        <v>0.1681971381022717</v>
+        <v>0.167175021966537</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="n">
-        <v>162</v>
+        <v>33499</v>
       </c>
       <c r="B68" t="n">
         <v>0</v>
       </c>
       <c r="C68" t="n">
-        <v>0.7852073907852173</v>
+        <v>0.7951120138168335</v>
       </c>
       <c r="D68" t="n">
-        <v>0.168047702215733</v>
+        <v>0.1671204903598906</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="n">
-        <v>50</v>
+        <v>33453</v>
       </c>
       <c r="B69" t="n">
         <v>0</v>
       </c>
       <c r="C69" t="n">
-        <v>0.7853376269340515</v>
+        <v>0.7951403458913168</v>
       </c>
       <c r="D69" t="n">
-        <v>0.1680354435341107</v>
+        <v>0.1671178527554318</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="n">
-        <v>160</v>
+        <v>35389</v>
       </c>
       <c r="B70" t="n">
         <v>0</v>
       </c>
       <c r="C70" t="n">
-        <v>0.7897295951843262</v>
+        <v>0.7951839566230774</v>
       </c>
       <c r="D70" t="n">
-        <v>0.1676230872011158</v>
+        <v>0.1671137929309096</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="n">
-        <v>30</v>
+        <v>35729</v>
       </c>
       <c r="B71" t="n">
         <v>0</v>
       </c>
       <c r="C71" t="n">
-        <v>0.7933701276779175</v>
+        <v>0.7954671025276184</v>
       </c>
       <c r="D71" t="n">
-        <v>0.1672828131627488</v>
+        <v>0.1670874390166585</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="n">
-        <v>2015</v>
+        <v>35971</v>
       </c>
       <c r="B72" t="n">
         <v>0</v>
       </c>
       <c r="C72" t="n">
-        <v>0.7937794923782349</v>
+        <v>0.7957391738891602</v>
       </c>
       <c r="D72" t="n">
-        <v>0.1672446369660816</v>
+        <v>0.167062123699328</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="n">
-        <v>1164</v>
+        <v>34273</v>
       </c>
       <c r="B73" t="n">
         <v>0</v>
       </c>
       <c r="C73" t="n">
-        <v>0.7942581176757812</v>
+        <v>0.796442449092865</v>
       </c>
       <c r="D73" t="n">
-        <v>0.1672000238118524</v>
+        <v>0.1669967218551802</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="n">
-        <v>171</v>
+        <v>33937</v>
       </c>
       <c r="B74" t="n">
         <v>0</v>
       </c>
       <c r="C74" t="n">
-        <v>0.7980104088783264</v>
+        <v>0.796589732170105</v>
       </c>
       <c r="D74" t="n">
-        <v>0.166851091917289</v>
+        <v>0.1669830315893152</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="n">
-        <v>176</v>
+        <v>35518</v>
       </c>
       <c r="B75" t="n">
         <v>0</v>
       </c>
       <c r="C75" t="n">
-        <v>0.7980753779411316</v>
+        <v>0.7966566483179728</v>
       </c>
       <c r="D75" t="n">
-        <v>0.16684506316054</v>
+        <v>0.1669768123368812</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="n">
-        <v>1</v>
+        <v>34581</v>
       </c>
       <c r="B76" t="n">
         <v>0</v>
       </c>
       <c r="C76" t="n">
-        <v>0.7995483875274658</v>
+        <v>0.7968798756599427</v>
       </c>
       <c r="D76" t="n">
-        <v>0.1667084931304306</v>
+        <v>0.1669560687187387</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="n">
-        <v>701</v>
+        <v>34199</v>
       </c>
       <c r="B77" t="n">
         <v>0</v>
       </c>
       <c r="C77" t="n">
-        <v>0.8026334842046102</v>
+        <v>0.7972601254781088</v>
       </c>
       <c r="D77" t="n">
-        <v>0.1664231817664095</v>
+        <v>0.1669207454987595</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="n">
-        <v>2274</v>
+        <v>34358</v>
       </c>
       <c r="B78" t="n">
         <v>0</v>
       </c>
       <c r="C78" t="n">
-        <v>0.8027173280715942</v>
+        <v>0.7972636620203654</v>
       </c>
       <c r="D78" t="n">
-        <v>0.1664154414718565</v>
+        <v>0.1669204170426279</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="n">
-        <v>1366</v>
+        <v>34413</v>
       </c>
       <c r="B79" t="n">
         <v>0</v>
       </c>
       <c r="C79" t="n">
-        <v>0.8027173280715942</v>
+        <v>0.7973665197690328</v>
       </c>
       <c r="D79" t="n">
-        <v>0.1664154414718565</v>
+        <v>0.1669108647014027</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="n">
-        <v>154</v>
+        <v>34284</v>
       </c>
       <c r="B80" t="n">
         <v>0</v>
       </c>
       <c r="C80" t="n">
-        <v>0.8027555346488953</v>
+        <v>0.7974677979946136</v>
       </c>
       <c r="D80" t="n">
-        <v>0.166411914557471</v>
+        <v>0.1669014601177845</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="n">
-        <v>173</v>
+        <v>34491</v>
       </c>
       <c r="B81" t="n">
         <v>0</v>
       </c>
       <c r="C81" t="n">
-        <v>0.804850697517395</v>
+        <v>0.7975214719772339</v>
       </c>
       <c r="D81" t="n">
-        <v>0.1662187351079264</v>
+        <v>0.1668964764409777</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="n">
-        <v>310</v>
+        <v>34454</v>
       </c>
       <c r="B82" t="n">
         <v>0</v>
       </c>
       <c r="C82" t="n">
-        <v>0.8053258657455444</v>
+        <v>0.7977633476257324</v>
       </c>
       <c r="D82" t="n">
-        <v>0.166174985742039</v>
+        <v>0.1668740217649912</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="n">
-        <v>2027</v>
+        <v>34279</v>
       </c>
       <c r="B83" t="n">
         <v>0</v>
       </c>
       <c r="C83" t="n">
-        <v>0.8054431875546774</v>
+        <v>0.7979708909988403</v>
       </c>
       <c r="D83" t="n">
-        <v>0.1661641873131023</v>
+        <v>0.1668547591631691</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="n">
-        <v>2367</v>
+        <v>33672</v>
       </c>
       <c r="B84" t="n">
         <v>0</v>
       </c>
       <c r="C84" t="n">
-        <v>0.8055684864521027</v>
+        <v>0.7980794191360474</v>
       </c>
       <c r="D84" t="n">
-        <v>0.1661526562138291</v>
+        <v>0.1668446881752008</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="n">
-        <v>1596</v>
+        <v>34958</v>
       </c>
       <c r="B85" t="n">
         <v>0</v>
       </c>
       <c r="C85" t="n">
-        <v>0.8056062757968903</v>
+        <v>0.7981067299842834</v>
       </c>
       <c r="D85" t="n">
-        <v>0.1661491788222753</v>
+        <v>0.166842154026431</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="n">
-        <v>1092</v>
+        <v>33568</v>
       </c>
       <c r="B86" t="n">
         <v>0</v>
       </c>
       <c r="C86" t="n">
-        <v>0.8056792020797729</v>
+        <v>0.7981388449668885</v>
       </c>
       <c r="D86" t="n">
-        <v>0.1661424685262262</v>
+        <v>0.1668391742048842</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="n">
-        <v>1059</v>
+        <v>34282</v>
       </c>
       <c r="B87" t="n">
         <v>0</v>
       </c>
       <c r="C87" t="n">
-        <v>0.8056823164224625</v>
+        <v>0.7989965528249741</v>
       </c>
       <c r="D87" t="n">
-        <v>0.1661421819727292</v>
+        <v>0.1667596302666108</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="n">
-        <v>2245</v>
+        <v>35524</v>
       </c>
       <c r="B88" t="n">
         <v>0</v>
       </c>
       <c r="C88" t="n">
-        <v>0.8067030906677246</v>
+        <v>0.799726402759552</v>
       </c>
       <c r="D88" t="n">
-        <v>0.1660483128354673</v>
+        <v>0.1666920035956603</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="n">
-        <v>1337</v>
+        <v>33880</v>
       </c>
       <c r="B89" t="n">
         <v>0</v>
       </c>
       <c r="C89" t="n">
-        <v>0.8067030906677246</v>
+        <v>0.7999083995819092</v>
       </c>
       <c r="D89" t="n">
-        <v>0.1660483128354673</v>
+        <v>0.1666751486184993</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="n">
-        <v>1219</v>
+        <v>35192</v>
       </c>
       <c r="B90" t="n">
         <v>0</v>
       </c>
       <c r="C90" t="n">
-        <v>0.8070415854454041</v>
+        <v>0.7999699115753174</v>
       </c>
       <c r="D90" t="n">
-        <v>0.1660172086886729</v>
+        <v>0.1666694526784855</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="n">
-        <v>91</v>
+        <v>34651</v>
       </c>
       <c r="B91" t="n">
         <v>0</v>
       </c>
       <c r="C91" t="n">
-        <v>0.8072275916735331</v>
+        <v>0.7999930580457052</v>
       </c>
       <c r="D91" t="n">
-        <v>0.1660001216129028</v>
+        <v>0.1666673094426914</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="n">
-        <v>206</v>
+        <v>34585</v>
       </c>
       <c r="B92" t="n">
         <v>0</v>
       </c>
       <c r="C92" t="n">
-        <v>0.8073083013296127</v>
+        <v>0.8001851141452789</v>
       </c>
       <c r="D92" t="n">
-        <v>0.1659927084821632</v>
+        <v>0.1666495282305669</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="n">
-        <v>1289</v>
+        <v>35607</v>
       </c>
       <c r="B93" t="n">
         <v>0</v>
       </c>
       <c r="C93" t="n">
-        <v>0.8080360094706217</v>
+        <v>0.8005949497222901</v>
       </c>
       <c r="D93" t="n">
-        <v>0.1659258988364052</v>
+        <v>0.1666115969314863</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="n">
-        <v>137</v>
+        <v>34699</v>
       </c>
       <c r="B94" t="n">
         <v>0</v>
       </c>
       <c r="C94" t="n">
-        <v>0.8086442152659098</v>
+        <v>0.8005949497222901</v>
       </c>
       <c r="D94" t="n">
-        <v>0.1658701017413165</v>
+        <v>0.1666115969314863</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="n">
-        <v>2156</v>
+        <v>34535</v>
       </c>
       <c r="B95" t="n">
         <v>0</v>
       </c>
       <c r="C95" t="n">
-        <v>0.8089435696601868</v>
+        <v>0.8007639348506927</v>
       </c>
       <c r="D95" t="n">
-        <v>0.1658426526021237</v>
+        <v>0.1665959619659275</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="n">
-        <v>1446</v>
+        <v>34063</v>
       </c>
       <c r="B96" t="n">
         <v>0</v>
       </c>
       <c r="C96" t="n">
-        <v>0.8096012473106384</v>
+        <v>0.8012737631797791</v>
       </c>
       <c r="D96" t="n">
-        <v>0.1657823790991793</v>
+        <v>0.1665488090330098</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="n">
-        <v>842</v>
+        <v>34421</v>
       </c>
       <c r="B97" t="n">
         <v>0</v>
       </c>
       <c r="C97" t="n">
-        <v>0.8100547790527344</v>
+        <v>0.8020230412483216</v>
       </c>
       <c r="D97" t="n">
-        <v>0.165740840261752</v>
+        <v>0.1664795583258358</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="n">
-        <v>1051</v>
+        <v>35527</v>
       </c>
       <c r="B98" t="n">
         <v>0</v>
       </c>
       <c r="C98" t="n">
-        <v>0.8104061285654703</v>
+        <v>0.8035422921180725</v>
       </c>
       <c r="D98" t="n">
-        <v>0.1657086745711107</v>
+        <v>0.1663393208526767</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="n">
-        <v>179</v>
+        <v>34808</v>
       </c>
       <c r="B99" t="n">
         <v>0</v>
       </c>
       <c r="C99" t="n">
-        <v>0.8107168674468994</v>
+        <v>0.8056413412094117</v>
       </c>
       <c r="D99" t="n">
-        <v>0.165680237144418</v>
+        <v>0.1661459522183188</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="n">
-        <v>1129</v>
+        <v>35893</v>
       </c>
       <c r="B100" t="n">
         <v>0</v>
       </c>
       <c r="C100" t="n">
-        <v>0.812219500541687</v>
+        <v>0.8110797762870788</v>
       </c>
       <c r="D100" t="n">
-        <v>0.1655428605145942</v>
+        <v>0.1656470377108591</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="n">
+        <v>35892</v>
+      </c>
+      <c r="B101" t="n">
+        <v>0</v>
+      </c>
+      <c r="C101" t="n">
+        <v>0.8112217903137207</v>
+      </c>
+      <c r="D101" t="n">
+        <v>0.1656340496809268</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added finetuning model, fixed reference number in db
</commit_message>
<xml_diff>
--- a/output/scores.xlsx
+++ b/output/scores.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D101"/>
+  <dimension ref="A1:D96"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -457,1402 +457,1332 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>2450</v>
+        <v>1756</v>
       </c>
       <c r="B2" t="n">
-        <v>169.6026</v>
+        <v>15.37518333333333</v>
       </c>
       <c r="C2" t="n">
-        <v>0</v>
+        <v>0.4433481047550837</v>
       </c>
       <c r="D2" t="n">
-        <v>118.72182</v>
+        <v>8.034008444679371</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>1689</v>
+        <v>1269</v>
       </c>
       <c r="B3" t="n">
-        <v>168.1452</v>
+        <v>12.21561666666667</v>
       </c>
       <c r="C3" t="n">
-        <v>0</v>
+        <v>0.3680493930975596</v>
       </c>
       <c r="D3" t="n">
-        <v>117.70164</v>
+        <v>6.473292213171833</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>908</v>
+        <v>454</v>
       </c>
       <c r="B4" t="n">
-        <v>166.4251</v>
+        <v>11.49596666666667</v>
       </c>
       <c r="C4" t="n">
         <v>0</v>
       </c>
       <c r="D4" t="n">
-        <v>116.49757</v>
+        <v>5.747983333333333</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>243</v>
+        <v>581</v>
       </c>
       <c r="B5" t="n">
-        <v>165.8187</v>
+        <v>10.83451666666667</v>
       </c>
       <c r="C5" t="n">
         <v>0</v>
       </c>
       <c r="D5" t="n">
-        <v>116.07309</v>
+        <v>5.417258333333334</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>903</v>
+        <v>514</v>
       </c>
       <c r="B6" t="n">
-        <v>165.0349</v>
+        <v>9.996700000000002</v>
       </c>
       <c r="C6" t="n">
-        <v>0</v>
+        <v>0.4255445698897044</v>
       </c>
       <c r="D6" t="n">
-        <v>115.52443</v>
+        <v>5.349093154974584</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>967</v>
+        <v>1270</v>
       </c>
       <c r="B7" t="n">
-        <v>164.6438</v>
+        <v>10.60906666666667</v>
       </c>
       <c r="C7" t="n">
         <v>0</v>
       </c>
       <c r="D7" t="n">
-        <v>115.25066</v>
+        <v>5.304533333333334</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>509</v>
+        <v>1260</v>
       </c>
       <c r="B8" t="n">
-        <v>164.6222</v>
+        <v>9.557866666666666</v>
       </c>
       <c r="C8" t="n">
         <v>0</v>
       </c>
       <c r="D8" t="n">
-        <v>115.23554</v>
+        <v>4.778933333333333</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>1586</v>
+        <v>456</v>
       </c>
       <c r="B9" t="n">
-        <v>163.8001</v>
+        <v>9.131783333333333</v>
       </c>
       <c r="C9" t="n">
         <v>0</v>
       </c>
       <c r="D9" t="n">
-        <v>114.66007</v>
+        <v>4.565891666666666</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>1469</v>
+        <v>824</v>
       </c>
       <c r="B10" t="n">
-        <v>163.7061</v>
+        <v>9.081416666666666</v>
       </c>
       <c r="C10" t="n">
         <v>0</v>
       </c>
       <c r="D10" t="n">
-        <v>114.59427</v>
+        <v>4.540708333333333</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>1580</v>
+        <v>680</v>
       </c>
       <c r="B11" t="n">
-        <v>163.5039</v>
+        <v>8.487866666666667</v>
       </c>
       <c r="C11" t="n">
         <v>0</v>
       </c>
       <c r="D11" t="n">
-        <v>114.45273</v>
+        <v>4.243933333333334</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>2328</v>
+        <v>569</v>
       </c>
       <c r="B12" t="n">
-        <v>163.3697</v>
+        <v>8.386316666666668</v>
       </c>
       <c r="C12" t="n">
         <v>0</v>
       </c>
       <c r="D12" t="n">
-        <v>114.35879</v>
+        <v>4.193158333333334</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>259</v>
+        <v>701</v>
       </c>
       <c r="B13" t="n">
-        <v>162.6408</v>
+        <v>8.357083333333334</v>
       </c>
       <c r="C13" t="n">
         <v>0</v>
       </c>
       <c r="D13" t="n">
-        <v>113.84856</v>
+        <v>4.178541666666667</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>2451</v>
+        <v>2175</v>
       </c>
       <c r="B14" t="n">
-        <v>106.3287</v>
+        <v>8.229366666666666</v>
       </c>
       <c r="C14" t="n">
         <v>0</v>
       </c>
       <c r="D14" t="n">
-        <v>74.43008999999999</v>
+        <v>4.114683333333333</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>553</v>
+        <v>382</v>
       </c>
       <c r="B15" t="n">
-        <v>105.20635</v>
+        <v>8.209300000000001</v>
       </c>
       <c r="C15" t="n">
         <v>0</v>
       </c>
       <c r="D15" t="n">
-        <v>73.64444499999999</v>
+        <v>4.10465</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>2257</v>
+        <v>618</v>
       </c>
       <c r="B16" t="n">
-        <v>102.63345</v>
+        <v>7.498083333333334</v>
       </c>
       <c r="C16" t="n">
-        <v>0</v>
+        <v>0.4561617374420166</v>
       </c>
       <c r="D16" t="n">
-        <v>71.84341500000001</v>
+        <v>4.092410117535546</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>1349</v>
+        <v>653</v>
       </c>
       <c r="B17" t="n">
-        <v>102.63345</v>
+        <v>7.737816666666667</v>
       </c>
       <c r="C17" t="n">
         <v>0</v>
       </c>
       <c r="D17" t="n">
-        <v>71.84341500000001</v>
+        <v>3.868908333333334</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>2551</v>
+        <v>511</v>
       </c>
       <c r="B18" t="n">
-        <v>102.4392</v>
+        <v>7.698266666666666</v>
       </c>
       <c r="C18" t="n">
         <v>0</v>
       </c>
       <c r="D18" t="n">
-        <v>71.70743999999999</v>
+        <v>3.849133333333333</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>1207</v>
+        <v>812</v>
       </c>
       <c r="B19" t="n">
-        <v>102.38385</v>
+        <v>7.67165</v>
       </c>
       <c r="C19" t="n">
         <v>0</v>
       </c>
       <c r="D19" t="n">
-        <v>71.66869499999999</v>
+        <v>3.835825</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>287</v>
+        <v>722</v>
       </c>
       <c r="B20" t="n">
-        <v>102.2776</v>
+        <v>7.6172</v>
       </c>
       <c r="C20" t="n">
         <v>0</v>
       </c>
       <c r="D20" t="n">
-        <v>71.59432</v>
+        <v>3.8086</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>2526</v>
+        <v>640</v>
       </c>
       <c r="B21" t="n">
-        <v>102.0947</v>
+        <v>7.498616666666667</v>
       </c>
       <c r="C21" t="n">
         <v>0</v>
       </c>
       <c r="D21" t="n">
-        <v>71.46629</v>
+        <v>3.749308333333333</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>1206</v>
+        <v>519</v>
       </c>
       <c r="B22" t="n">
-        <v>101.69845</v>
+        <v>7.398599999999999</v>
       </c>
       <c r="C22" t="n">
         <v>0</v>
       </c>
       <c r="D22" t="n">
-        <v>71.18891499999999</v>
+        <v>3.6993</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>1623</v>
+        <v>513</v>
       </c>
       <c r="B23" t="n">
-        <v>101.3795</v>
+        <v>6.66545</v>
       </c>
       <c r="C23" t="n">
-        <v>0</v>
+        <v>0.442608763774236</v>
       </c>
       <c r="D23" t="n">
-        <v>70.96565</v>
+        <v>3.679319317569423</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>1418</v>
+        <v>1761</v>
       </c>
       <c r="B24" t="n">
-        <v>100.3693</v>
+        <v>7.27375</v>
       </c>
       <c r="C24" t="n">
         <v>0</v>
       </c>
       <c r="D24" t="n">
-        <v>70.25851</v>
+        <v>3.636875</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>1548</v>
+        <v>459</v>
       </c>
       <c r="B25" t="n">
-        <v>99.9876</v>
+        <v>7.244016666666667</v>
       </c>
       <c r="C25" t="n">
         <v>0</v>
       </c>
       <c r="D25" t="n">
-        <v>69.99132</v>
+        <v>3.622008333333333</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>527</v>
+        <v>1312</v>
       </c>
       <c r="B26" t="n">
-        <v>84.99496666666667</v>
+        <v>7.053383333333334</v>
       </c>
       <c r="C26" t="n">
         <v>0</v>
       </c>
       <c r="D26" t="n">
-        <v>59.49647666666667</v>
+        <v>3.526691666666667</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>2462</v>
+        <v>627</v>
       </c>
       <c r="B27" t="n">
-        <v>83.30613333333334</v>
+        <v>7.034266666666666</v>
       </c>
       <c r="C27" t="n">
         <v>0</v>
       </c>
       <c r="D27" t="n">
-        <v>58.31429333333333</v>
+        <v>3.517133333333333</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>1590</v>
+        <v>620</v>
       </c>
       <c r="B28" t="n">
-        <v>83.0939</v>
+        <v>6.96295</v>
       </c>
       <c r="C28" t="n">
         <v>0</v>
       </c>
       <c r="D28" t="n">
-        <v>58.16573</v>
+        <v>3.481475</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>548</v>
+        <v>1356</v>
       </c>
       <c r="B29" t="n">
-        <v>82.03213333333333</v>
+        <v>6.932116666666666</v>
       </c>
       <c r="C29" t="n">
         <v>0</v>
       </c>
       <c r="D29" t="n">
-        <v>57.42249333333333</v>
+        <v>3.466058333333333</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>1567</v>
+        <v>1738</v>
       </c>
       <c r="B30" t="n">
-        <v>81.82463333333332</v>
+        <v>6.869116666666666</v>
       </c>
       <c r="C30" t="n">
         <v>0</v>
       </c>
       <c r="D30" t="n">
-        <v>57.27724333333332</v>
+        <v>3.434558333333333</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>2518</v>
+        <v>590</v>
       </c>
       <c r="B31" t="n">
-        <v>81.79363333333333</v>
+        <v>6.7714</v>
       </c>
       <c r="C31" t="n">
         <v>0</v>
       </c>
       <c r="D31" t="n">
-        <v>57.25554333333333</v>
+        <v>3.3857</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>437</v>
+        <v>565</v>
       </c>
       <c r="B32" t="n">
-        <v>81.72113333333333</v>
+        <v>6.691616666666666</v>
       </c>
       <c r="C32" t="n">
         <v>0</v>
       </c>
       <c r="D32" t="n">
-        <v>57.20479333333333</v>
+        <v>3.345808333333333</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>1626</v>
+        <v>1535</v>
       </c>
       <c r="B33" t="n">
-        <v>80.9735</v>
+        <v>6.46975</v>
       </c>
       <c r="C33" t="n">
         <v>0</v>
       </c>
       <c r="D33" t="n">
-        <v>56.68145</v>
+        <v>3.234875</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>780</v>
+        <v>2443</v>
       </c>
       <c r="B34" t="n">
-        <v>80.8253</v>
+        <v>6.46975</v>
       </c>
       <c r="C34" t="n">
         <v>0</v>
       </c>
       <c r="D34" t="n">
-        <v>56.57771</v>
+        <v>3.234875</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>709</v>
+        <v>608</v>
       </c>
       <c r="B35" t="n">
-        <v>80.79979999999999</v>
+        <v>6.3821</v>
       </c>
       <c r="C35" t="n">
         <v>0</v>
       </c>
       <c r="D35" t="n">
-        <v>56.55985999999999</v>
+        <v>3.19105</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>387</v>
+        <v>2684</v>
       </c>
       <c r="B36" t="n">
-        <v>80.2456</v>
+        <v>6.376516666666667</v>
       </c>
       <c r="C36" t="n">
         <v>0</v>
       </c>
       <c r="D36" t="n">
-        <v>56.17191999999999</v>
+        <v>3.188258333333334</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>1141</v>
+        <v>1354</v>
       </c>
       <c r="B37" t="n">
-        <v>80.22959999999999</v>
+        <v>6.374766666666667</v>
       </c>
       <c r="C37" t="n">
         <v>0</v>
       </c>
       <c r="D37" t="n">
-        <v>56.16071999999999</v>
+        <v>3.187383333333333</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>2543</v>
+        <v>1273</v>
       </c>
       <c r="B38" t="n">
-        <v>80.20846666666667</v>
+        <v>6.373016666666667</v>
       </c>
       <c r="C38" t="n">
         <v>0</v>
       </c>
       <c r="D38" t="n">
-        <v>56.14592666666666</v>
+        <v>3.186508333333334</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="n">
-        <v>1616</v>
+        <v>573</v>
       </c>
       <c r="B39" t="n">
-        <v>79.84310000000001</v>
+        <v>6.351216666666666</v>
       </c>
       <c r="C39" t="n">
         <v>0</v>
       </c>
       <c r="D39" t="n">
-        <v>55.89017</v>
+        <v>3.175608333333333</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="n">
-        <v>374</v>
+        <v>1712</v>
       </c>
       <c r="B40" t="n">
-        <v>79.35626666666667</v>
+        <v>6.278166666666666</v>
       </c>
       <c r="C40" t="n">
         <v>0</v>
       </c>
       <c r="D40" t="n">
-        <v>55.54938666666666</v>
+        <v>3.139083333333333</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="n">
-        <v>521</v>
+        <v>2675</v>
       </c>
       <c r="B41" t="n">
-        <v>79.02629999999999</v>
+        <v>6.241583333333334</v>
       </c>
       <c r="C41" t="n">
         <v>0</v>
       </c>
       <c r="D41" t="n">
-        <v>55.31840999999999</v>
+        <v>3.120791666666667</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="n">
-        <v>1624</v>
+        <v>912</v>
       </c>
       <c r="B42" t="n">
-        <v>72.98238000000001</v>
+        <v>6.237833333333334</v>
       </c>
       <c r="C42" t="n">
         <v>0</v>
       </c>
       <c r="D42" t="n">
-        <v>51.087666</v>
+        <v>3.118916666666667</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="n">
-        <v>569</v>
+        <v>378</v>
       </c>
       <c r="B43" t="n">
-        <v>69.35795</v>
+        <v>6.226633333333333</v>
       </c>
       <c r="C43" t="n">
         <v>0</v>
       </c>
       <c r="D43" t="n">
-        <v>48.550565</v>
+        <v>3.113316666666667</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="n">
-        <v>1137</v>
+        <v>1150</v>
       </c>
       <c r="B44" t="n">
-        <v>65.05354</v>
+        <v>6.218050000000001</v>
       </c>
       <c r="C44" t="n">
         <v>0</v>
       </c>
       <c r="D44" t="n">
-        <v>45.53747799999999</v>
+        <v>3.109025</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="n">
-        <v>250</v>
+        <v>1099</v>
       </c>
       <c r="B45" t="n">
-        <v>64.38118</v>
+        <v>6.16225</v>
       </c>
       <c r="C45" t="n">
         <v>0</v>
       </c>
       <c r="D45" t="n">
-        <v>45.066826</v>
+        <v>3.081125</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="n">
-        <v>547</v>
+        <v>1056</v>
       </c>
       <c r="B46" t="n">
-        <v>62.93089999999999</v>
+        <v>6.1053</v>
       </c>
       <c r="C46" t="n">
         <v>0</v>
       </c>
       <c r="D46" t="n">
-        <v>44.05163</v>
+        <v>3.05265</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="n">
-        <v>1416</v>
+        <v>842</v>
       </c>
       <c r="B47" t="n">
-        <v>61.62113333333334</v>
+        <v>6.098299999999999</v>
       </c>
       <c r="C47" t="n">
         <v>0</v>
       </c>
       <c r="D47" t="n">
-        <v>43.13479333333333</v>
+        <v>3.04915</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="n">
-        <v>1128</v>
+        <v>605</v>
       </c>
       <c r="B48" t="n">
-        <v>61.17085</v>
+        <v>6.083850000000001</v>
       </c>
       <c r="C48" t="n">
         <v>0</v>
       </c>
       <c r="D48" t="n">
-        <v>42.819595</v>
+        <v>3.041925</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="n">
-        <v>486</v>
+        <v>2170</v>
       </c>
       <c r="B49" t="n">
-        <v>60.68863333333334</v>
+        <v>6.054283333333333</v>
       </c>
       <c r="C49" t="n">
         <v>0</v>
       </c>
       <c r="D49" t="n">
-        <v>42.48204333333333</v>
+        <v>3.027141666666667</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="n">
-        <v>449</v>
+        <v>2425</v>
       </c>
       <c r="B50" t="n">
-        <v>60.14265</v>
+        <v>6.011333333333333</v>
       </c>
       <c r="C50" t="n">
         <v>0</v>
       </c>
       <c r="D50" t="n">
-        <v>42.099855</v>
+        <v>3.005666666666666</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="n">
-        <v>710</v>
+        <v>1517</v>
       </c>
       <c r="B51" t="n">
-        <v>59.51236666666667</v>
+        <v>6.011333333333333</v>
       </c>
       <c r="C51" t="n">
         <v>0</v>
       </c>
       <c r="D51" t="n">
-        <v>41.65865666666667</v>
+        <v>3.005666666666666</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="n">
-        <v>34868</v>
+        <v>1286</v>
       </c>
       <c r="B52" t="n">
         <v>0</v>
       </c>
       <c r="C52" t="n">
-        <v>0.7822101712226868</v>
+        <v>0.345382034778595</v>
       </c>
       <c r="D52" t="n">
-        <v>0.168330315270384</v>
+        <v>0.3716416505310949</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="n">
-        <v>33624</v>
+        <v>995</v>
       </c>
       <c r="B53" t="n">
         <v>0</v>
       </c>
       <c r="C53" t="n">
-        <v>0.7822558879852295</v>
+        <v>0.354933425784111</v>
       </c>
       <c r="D53" t="n">
-        <v>0.1683259974184393</v>
+        <v>0.3690218209139286</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="n">
-        <v>33483</v>
+        <v>1552</v>
       </c>
       <c r="B54" t="n">
         <v>0</v>
       </c>
       <c r="C54" t="n">
-        <v>0.7852948307991028</v>
+        <v>0.3577295541763306</v>
       </c>
       <c r="D54" t="n">
-        <v>0.1680394715900898</v>
+        <v>0.3682618518997519</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="n">
-        <v>33507</v>
+        <v>1755</v>
       </c>
       <c r="B55" t="n">
         <v>0</v>
       </c>
       <c r="C55" t="n">
-        <v>0.7862100601196289</v>
+        <v>0.3603252172470093</v>
       </c>
       <c r="D55" t="n">
-        <v>0.1679533704898672</v>
+        <v>0.3675591642797646</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="n">
-        <v>33516</v>
+        <v>998</v>
       </c>
       <c r="B56" t="n">
         <v>0</v>
       </c>
       <c r="C56" t="n">
-        <v>0.7873714566230774</v>
+        <v>0.3635201454162598</v>
       </c>
       <c r="D56" t="n">
-        <v>0.1678442379105667</v>
+        <v>0.3666979191182822</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="n">
-        <v>33541</v>
+        <v>417</v>
       </c>
       <c r="B57" t="n">
         <v>0</v>
       </c>
       <c r="C57" t="n">
-        <v>0.7874562740325928</v>
+        <v>0.3644525110721588</v>
       </c>
       <c r="D57" t="n">
-        <v>0.1678362734564604</v>
+        <v>0.3664473449553112</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="n">
-        <v>35894</v>
+        <v>2214</v>
       </c>
       <c r="B58" t="n">
         <v>0</v>
       </c>
       <c r="C58" t="n">
-        <v>0.7880964577198029</v>
+        <v>0.3648412227630615</v>
       </c>
       <c r="D58" t="n">
-        <v>0.1677761838321422</v>
+        <v>0.3663429794330009</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="n">
-        <v>33535</v>
+        <v>992</v>
       </c>
       <c r="B59" t="n">
         <v>0</v>
       </c>
       <c r="C59" t="n">
-        <v>0.7889856696128845</v>
+        <v>0.3714350983500481</v>
       </c>
       <c r="D59" t="n">
-        <v>0.1676927910020188</v>
+        <v>0.3645815982116413</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="n">
-        <v>34243</v>
+        <v>2769</v>
       </c>
       <c r="B60" t="n">
         <v>0</v>
       </c>
       <c r="C60" t="n">
-        <v>0.7906647622585297</v>
+        <v>0.3778933584690094</v>
       </c>
       <c r="D60" t="n">
-        <v>0.1675355467550587</v>
+        <v>0.3628727846947131</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="n">
-        <v>33412</v>
+        <v>1364</v>
       </c>
       <c r="B61" t="n">
         <v>0</v>
       </c>
       <c r="C61" t="n">
-        <v>0.7917564511299133</v>
+        <v>0.3788550347089767</v>
       </c>
       <c r="D61" t="n">
-        <v>0.1674334699957769</v>
+        <v>0.3626197007037297</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="n">
-        <v>33363</v>
+        <v>2530</v>
       </c>
       <c r="B62" t="n">
         <v>0</v>
       </c>
       <c r="C62" t="n">
-        <v>0.7917799949645996</v>
+        <v>0.3799591422080993</v>
       </c>
       <c r="D62" t="n">
-        <v>0.1674312699344135</v>
+        <v>0.3623295681058645</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="n">
-        <v>34601</v>
+        <v>648</v>
       </c>
       <c r="B63" t="n">
         <v>0</v>
       </c>
       <c r="C63" t="n">
-        <v>0.7922704517841339</v>
+        <v>0.380683034658432</v>
       </c>
       <c r="D63" t="n">
-        <v>0.167385452179587</v>
+        <v>0.3621395986253248</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="n">
-        <v>35390</v>
+        <v>432</v>
       </c>
       <c r="B64" t="n">
         <v>0</v>
       </c>
       <c r="C64" t="n">
-        <v>0.7928596287965775</v>
+        <v>0.3871363878250122</v>
       </c>
       <c r="D64" t="n">
-        <v>0.1673304452738273</v>
+        <v>0.3604548221707202</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="n">
-        <v>35455</v>
+        <v>415</v>
       </c>
       <c r="B65" t="n">
         <v>0</v>
       </c>
       <c r="C65" t="n">
-        <v>0.7935595512390137</v>
+        <v>0.3902910351753235</v>
       </c>
       <c r="D65" t="n">
-        <v>0.1672651458897789</v>
+        <v>0.3596369302179577</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="n">
-        <v>34026</v>
+        <v>810</v>
       </c>
       <c r="B66" t="n">
         <v>0</v>
       </c>
       <c r="C66" t="n">
-        <v>0.794352650642395</v>
+        <v>0.394643671810627</v>
       </c>
       <c r="D66" t="n">
-        <v>0.1671912151118105</v>
+        <v>0.3585145152889583</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="n">
-        <v>35515</v>
+        <v>2340</v>
       </c>
       <c r="B67" t="n">
         <v>0</v>
       </c>
       <c r="C67" t="n">
-        <v>0.7945264577865601</v>
+        <v>0.3988342061638832</v>
       </c>
       <c r="D67" t="n">
-        <v>0.167175021966537</v>
+        <v>0.3574405013809203</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="n">
-        <v>33499</v>
+        <v>2525</v>
       </c>
       <c r="B68" t="n">
         <v>0</v>
       </c>
       <c r="C68" t="n">
-        <v>0.7951120138168335</v>
+        <v>0.4003282338380814</v>
       </c>
       <c r="D68" t="n">
-        <v>0.1671204903598906</v>
+        <v>0.357059143647756</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="n">
-        <v>33453</v>
+        <v>510</v>
       </c>
       <c r="B69" t="n">
         <v>0</v>
       </c>
       <c r="C69" t="n">
-        <v>0.7951403458913168</v>
+        <v>0.4022790392239888</v>
       </c>
       <c r="D69" t="n">
-        <v>0.1671178527554318</v>
+        <v>0.3565624144797147</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="n">
-        <v>35389</v>
+        <v>385</v>
       </c>
       <c r="B70" t="n">
         <v>0</v>
       </c>
       <c r="C70" t="n">
-        <v>0.7951839566230774</v>
+        <v>0.4028065726161003</v>
       </c>
       <c r="D70" t="n">
-        <v>0.1671137929309096</v>
+        <v>0.3564283271552882</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="n">
-        <v>35729</v>
+        <v>499</v>
       </c>
       <c r="B71" t="n">
         <v>0</v>
       </c>
       <c r="C71" t="n">
-        <v>0.7954671025276184</v>
+        <v>0.4041951547066371</v>
       </c>
       <c r="D71" t="n">
-        <v>0.1670874390166585</v>
+        <v>0.3560758619085674</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="n">
-        <v>35971</v>
+        <v>471</v>
       </c>
       <c r="B72" t="n">
         <v>0</v>
       </c>
       <c r="C72" t="n">
-        <v>0.7957391738891602</v>
+        <v>0.4072804525494576</v>
       </c>
       <c r="D72" t="n">
-        <v>0.167062123699328</v>
+        <v>0.3552952072162943</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="n">
-        <v>34273</v>
+        <v>2321</v>
       </c>
       <c r="B73" t="n">
         <v>0</v>
       </c>
       <c r="C73" t="n">
-        <v>0.796442449092865</v>
+        <v>0.4078863561153412</v>
       </c>
       <c r="D73" t="n">
-        <v>0.1669967218551802</v>
+        <v>0.3551423009592952</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="n">
-        <v>33937</v>
+        <v>2527</v>
       </c>
       <c r="B74" t="n">
         <v>0</v>
       </c>
       <c r="C74" t="n">
-        <v>0.796589732170105</v>
+        <v>0.4148582319418589</v>
       </c>
       <c r="D74" t="n">
-        <v>0.1669830315893152</v>
+        <v>0.3533922966357994</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="n">
-        <v>35518</v>
+        <v>2508</v>
       </c>
       <c r="B75" t="n">
         <v>0</v>
       </c>
       <c r="C75" t="n">
-        <v>0.7966566483179728</v>
+        <v>0.4178962782025337</v>
       </c>
       <c r="D75" t="n">
-        <v>0.1669768123368812</v>
+        <v>0.3526351029243477</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="n">
-        <v>34581</v>
+        <v>2231</v>
       </c>
       <c r="B76" t="n">
         <v>0</v>
       </c>
       <c r="C76" t="n">
-        <v>0.7968798756599427</v>
+        <v>0.4182643353939056</v>
       </c>
       <c r="D76" t="n">
-        <v>0.1669560687187387</v>
+        <v>0.3525435897400121</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="n">
-        <v>34199</v>
+        <v>489</v>
       </c>
       <c r="B77" t="n">
         <v>0</v>
       </c>
       <c r="C77" t="n">
-        <v>0.7972601254781088</v>
+        <v>0.4194592783848445</v>
       </c>
       <c r="D77" t="n">
-        <v>0.1669207454987595</v>
+        <v>0.3522468080725312</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="n">
-        <v>34358</v>
+        <v>770</v>
       </c>
       <c r="B78" t="n">
         <v>0</v>
       </c>
       <c r="C78" t="n">
-        <v>0.7972636620203654</v>
+        <v>0.4211360514163971</v>
       </c>
       <c r="D78" t="n">
-        <v>0.1669204170426279</v>
+        <v>0.3518311983582904</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="n">
-        <v>34413</v>
+        <v>647</v>
       </c>
       <c r="B79" t="n">
         <v>0</v>
       </c>
       <c r="C79" t="n">
-        <v>0.7973665197690328</v>
+        <v>0.4252172559499741</v>
       </c>
       <c r="D79" t="n">
-        <v>0.1669108647014027</v>
+        <v>0.3508237062894152</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="n">
-        <v>34284</v>
+        <v>2029</v>
       </c>
       <c r="B80" t="n">
         <v>0</v>
       </c>
       <c r="C80" t="n">
-        <v>0.7974677979946136</v>
+        <v>0.4289175818363826</v>
       </c>
       <c r="D80" t="n">
-        <v>0.1669014601177845</v>
+        <v>0.3499152129945954</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="n">
-        <v>34491</v>
+        <v>410</v>
       </c>
       <c r="B81" t="n">
         <v>0</v>
       </c>
       <c r="C81" t="n">
-        <v>0.7975214719772339</v>
+        <v>0.4300993204116821</v>
       </c>
       <c r="D81" t="n">
-        <v>0.1668964764409777</v>
+        <v>0.349626066430173</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="n">
-        <v>34454</v>
+        <v>502</v>
       </c>
       <c r="B82" t="n">
         <v>0</v>
       </c>
       <c r="C82" t="n">
-        <v>0.7977633476257324</v>
+        <v>0.4328547716140747</v>
       </c>
       <c r="D82" t="n">
-        <v>0.1668740217649912</v>
+        <v>0.3489537180636685</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="n">
-        <v>34279</v>
+        <v>419</v>
       </c>
       <c r="B83" t="n">
         <v>0</v>
       </c>
       <c r="C83" t="n">
-        <v>0.7979708909988403</v>
+        <v>0.4380088200171788</v>
       </c>
       <c r="D83" t="n">
-        <v>0.1668547591631691</v>
+        <v>0.3477030133890465</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="n">
-        <v>33672</v>
+        <v>2535</v>
       </c>
       <c r="B84" t="n">
         <v>0</v>
       </c>
       <c r="C84" t="n">
-        <v>0.7980794191360474</v>
+        <v>0.4394298096497853</v>
       </c>
       <c r="D84" t="n">
-        <v>0.1668446881752008</v>
+        <v>0.3473597647124249</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="n">
-        <v>34958</v>
+        <v>508</v>
       </c>
       <c r="B85" t="n">
         <v>0</v>
       </c>
       <c r="C85" t="n">
-        <v>0.7981067299842834</v>
+        <v>0.4408751130104065</v>
       </c>
       <c r="D85" t="n">
-        <v>0.166842154026431</v>
+        <v>0.3470113374054708</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="n">
-        <v>33568</v>
+        <v>731</v>
       </c>
       <c r="B86" t="n">
         <v>0</v>
       </c>
       <c r="C86" t="n">
-        <v>0.7981388449668885</v>
+        <v>0.4429205358028412</v>
       </c>
       <c r="D86" t="n">
-        <v>0.1668391742048842</v>
+        <v>0.3465194288899631</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="n">
-        <v>34282</v>
+        <v>2224</v>
       </c>
       <c r="B87" t="n">
         <v>0</v>
       </c>
       <c r="C87" t="n">
-        <v>0.7989965528249741</v>
+        <v>0.4435210675001144</v>
       </c>
       <c r="D87" t="n">
-        <v>0.1667596302666108</v>
+        <v>0.3463752703421908</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="n">
-        <v>35524</v>
+        <v>661</v>
       </c>
       <c r="B88" t="n">
         <v>0</v>
       </c>
       <c r="C88" t="n">
-        <v>0.799726402759552</v>
+        <v>0.4471633732318878</v>
       </c>
       <c r="D88" t="n">
-        <v>0.1666920035956603</v>
+        <v>0.3455034927282408</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="n">
-        <v>33880</v>
+        <v>732</v>
       </c>
       <c r="B89" t="n">
         <v>0</v>
       </c>
       <c r="C89" t="n">
-        <v>0.7999083995819092</v>
+        <v>0.4496812969446182</v>
       </c>
       <c r="D89" t="n">
-        <v>0.1666751486184993</v>
+        <v>0.3449033943210908</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="n">
-        <v>35192</v>
+        <v>495</v>
       </c>
       <c r="B90" t="n">
         <v>0</v>
       </c>
       <c r="C90" t="n">
-        <v>0.7999699115753174</v>
+        <v>0.451386570930481</v>
       </c>
       <c r="D90" t="n">
-        <v>0.1666694526784855</v>
+        <v>0.3444981578405063</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="n">
-        <v>34651</v>
+        <v>2655</v>
       </c>
       <c r="B91" t="n">
         <v>0</v>
       </c>
       <c r="C91" t="n">
-        <v>0.7999930580457052</v>
+        <v>0.4538289755582809</v>
       </c>
       <c r="D91" t="n">
-        <v>0.1666673094426914</v>
+        <v>0.3439194075823095</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="n">
-        <v>34585</v>
+        <v>412</v>
       </c>
       <c r="B92" t="n">
         <v>0</v>
       </c>
       <c r="C92" t="n">
-        <v>0.8001851141452789</v>
+        <v>0.4563107440869014</v>
       </c>
       <c r="D92" t="n">
-        <v>0.1666495282305669</v>
+        <v>0.3433333181329354</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="n">
-        <v>35607</v>
+        <v>915</v>
       </c>
       <c r="B93" t="n">
         <v>0</v>
       </c>
       <c r="C93" t="n">
-        <v>0.8005949497222901</v>
+        <v>0.4571950336297353</v>
       </c>
       <c r="D93" t="n">
-        <v>0.1666115969314863</v>
+        <v>0.3431249684913811</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="n">
-        <v>34699</v>
+        <v>764</v>
       </c>
       <c r="B94" t="n">
         <v>0</v>
       </c>
       <c r="C94" t="n">
-        <v>0.8005949497222901</v>
+        <v>0.4578785747289658</v>
       </c>
       <c r="D94" t="n">
-        <v>0.1666115969314863</v>
+        <v>0.3429640908831896</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="n">
-        <v>34535</v>
+        <v>2693</v>
       </c>
       <c r="B95" t="n">
         <v>0</v>
       </c>
       <c r="C95" t="n">
-        <v>0.8007639348506927</v>
+        <v>0.4593606740236282</v>
       </c>
       <c r="D95" t="n">
-        <v>0.1665959619659275</v>
+        <v>0.3426157829931387</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="n">
-        <v>34063</v>
+        <v>771</v>
       </c>
       <c r="B96" t="n">
         <v>0</v>
       </c>
       <c r="C96" t="n">
-        <v>0.8012737631797791</v>
+        <v>0.4604487915833791</v>
       </c>
       <c r="D96" t="n">
-        <v>0.1665488090330098</v>
-      </c>
-    </row>
-    <row r="97">
-      <c r="A97" t="n">
-        <v>34421</v>
-      </c>
-      <c r="B97" t="n">
-        <v>0</v>
-      </c>
-      <c r="C97" t="n">
-        <v>0.8020230412483216</v>
-      </c>
-      <c r="D97" t="n">
-        <v>0.1664795583258358</v>
-      </c>
-    </row>
-    <row r="98">
-      <c r="A98" t="n">
-        <v>35527</v>
-      </c>
-      <c r="B98" t="n">
-        <v>0</v>
-      </c>
-      <c r="C98" t="n">
-        <v>0.8035422921180725</v>
-      </c>
-      <c r="D98" t="n">
-        <v>0.1663393208526767</v>
-      </c>
-    </row>
-    <row r="99">
-      <c r="A99" t="n">
-        <v>34808</v>
-      </c>
-      <c r="B99" t="n">
-        <v>0</v>
-      </c>
-      <c r="C99" t="n">
-        <v>0.8056413412094117</v>
-      </c>
-      <c r="D99" t="n">
-        <v>0.1661459522183188</v>
-      </c>
-    </row>
-    <row r="100">
-      <c r="A100" t="n">
-        <v>35893</v>
-      </c>
-      <c r="B100" t="n">
-        <v>0</v>
-      </c>
-      <c r="C100" t="n">
-        <v>0.8110797762870788</v>
-      </c>
-      <c r="D100" t="n">
-        <v>0.1656470377108591</v>
-      </c>
-    </row>
-    <row r="101">
-      <c r="A101" t="n">
-        <v>35892</v>
-      </c>
-      <c r="B101" t="n">
-        <v>0</v>
-      </c>
-      <c r="C101" t="n">
-        <v>0.8112217903137207</v>
-      </c>
-      <c r="D101" t="n">
-        <v>0.1656340496809268</v>
+        <v>0.3423605147140514</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Intergrated gemini/claude into query_llm
</commit_message>
<xml_diff>
--- a/output/scores.xlsx
+++ b/output/scores.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D101"/>
+  <dimension ref="A1:D100"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -457,1402 +457,1388 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>1418</v>
+        <v>1137</v>
       </c>
       <c r="B2" t="n">
-        <v>19.3074</v>
+        <v>27.3247</v>
       </c>
       <c r="C2" t="n">
         <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>9.653700000000001</v>
+        <v>13.66235</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>780</v>
+        <v>2526</v>
       </c>
       <c r="B3" t="n">
-        <v>18.6248</v>
+        <v>25.24983333333333</v>
       </c>
       <c r="C3" t="n">
         <v>0</v>
       </c>
       <c r="D3" t="n">
-        <v>9.3124</v>
+        <v>12.62491666666667</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>967</v>
+        <v>1418</v>
       </c>
       <c r="B4" t="n">
-        <v>17.7746</v>
+        <v>23.8757</v>
       </c>
       <c r="C4" t="n">
         <v>0</v>
       </c>
       <c r="D4" t="n">
-        <v>8.8873</v>
+        <v>11.93785</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>1586</v>
+        <v>548</v>
       </c>
       <c r="B5" t="n">
-        <v>17.4389</v>
+        <v>21.0437</v>
       </c>
       <c r="C5" t="n">
         <v>0</v>
       </c>
       <c r="D5" t="n">
-        <v>8.71945</v>
+        <v>10.52185</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>1424</v>
+        <v>437</v>
       </c>
       <c r="B6" t="n">
-        <v>16.6778</v>
+        <v>20.9372</v>
       </c>
       <c r="C6" t="n">
         <v>0</v>
       </c>
       <c r="D6" t="n">
-        <v>8.338900000000001</v>
+        <v>10.4686</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>2543</v>
+        <v>1416</v>
       </c>
       <c r="B7" t="n">
-        <v>16.3458</v>
+        <v>20.4617</v>
       </c>
       <c r="C7" t="n">
         <v>0</v>
       </c>
       <c r="D7" t="n">
-        <v>8.1729</v>
+        <v>10.23085</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>527</v>
+        <v>1582</v>
       </c>
       <c r="B8" t="n">
-        <v>16.1238</v>
+        <v>20.38293333333333</v>
       </c>
       <c r="C8" t="n">
         <v>0</v>
       </c>
       <c r="D8" t="n">
-        <v>8.0619</v>
+        <v>10.19146666666667</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>1624</v>
+        <v>1207</v>
       </c>
       <c r="B9" t="n">
-        <v>15.69866666666667</v>
+        <v>19.17853333333333</v>
       </c>
       <c r="C9" t="n">
         <v>0</v>
       </c>
       <c r="D9" t="n">
-        <v>7.849333333333333</v>
+        <v>9.589266666666665</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>1149</v>
+        <v>486</v>
       </c>
       <c r="B10" t="n">
-        <v>15.6831</v>
+        <v>18.875</v>
       </c>
       <c r="C10" t="n">
         <v>0</v>
       </c>
       <c r="D10" t="n">
-        <v>7.84155</v>
+        <v>9.4375</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>764</v>
+        <v>780</v>
       </c>
       <c r="B11" t="n">
-        <v>15.3426</v>
+        <v>18.6248</v>
       </c>
       <c r="C11" t="n">
         <v>0</v>
       </c>
       <c r="D11" t="n">
-        <v>7.6713</v>
+        <v>9.3124</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>1580</v>
+        <v>527</v>
       </c>
       <c r="B12" t="n">
-        <v>14.8251</v>
+        <v>18.5818</v>
       </c>
       <c r="C12" t="n">
         <v>0</v>
       </c>
       <c r="D12" t="n">
-        <v>7.41255</v>
+        <v>9.290900000000001</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>486</v>
+        <v>1141</v>
       </c>
       <c r="B13" t="n">
-        <v>14.7919</v>
+        <v>18.4093</v>
       </c>
       <c r="C13" t="n">
         <v>0</v>
       </c>
       <c r="D13" t="n">
-        <v>7.39595</v>
+        <v>9.204650000000001</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>1685</v>
+        <v>521</v>
       </c>
       <c r="B14" t="n">
-        <v>14.3492</v>
+        <v>18.2293</v>
       </c>
       <c r="C14" t="n">
         <v>0</v>
       </c>
       <c r="D14" t="n">
-        <v>7.1746</v>
+        <v>9.114649999999999</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>1574</v>
+        <v>2117</v>
       </c>
       <c r="B15" t="n">
-        <v>13.8132</v>
+        <v>18.1017</v>
       </c>
       <c r="C15" t="n">
         <v>0</v>
       </c>
       <c r="D15" t="n">
-        <v>6.9066</v>
+        <v>9.050850000000001</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>1137</v>
+        <v>2552</v>
       </c>
       <c r="B16" t="n">
-        <v>13.66238333333333</v>
+        <v>17.9203</v>
       </c>
       <c r="C16" t="n">
         <v>0</v>
       </c>
       <c r="D16" t="n">
-        <v>6.831191666666666</v>
+        <v>8.960150000000001</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>1148</v>
+        <v>967</v>
       </c>
       <c r="B17" t="n">
-        <v>13.5578</v>
+        <v>17.7746</v>
       </c>
       <c r="C17" t="n">
         <v>0</v>
       </c>
       <c r="D17" t="n">
-        <v>6.7789</v>
+        <v>8.8873</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>2117</v>
+        <v>1180</v>
       </c>
       <c r="B18" t="n">
-        <v>13.5256</v>
+        <v>17.67</v>
       </c>
       <c r="C18" t="n">
         <v>0</v>
       </c>
       <c r="D18" t="n">
-        <v>6.7628</v>
+        <v>8.835000000000001</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>1688</v>
+        <v>246</v>
       </c>
       <c r="B19" t="n">
-        <v>13.4018</v>
+        <v>17.6562</v>
       </c>
       <c r="C19" t="n">
         <v>0</v>
       </c>
       <c r="D19" t="n">
-        <v>6.7009</v>
+        <v>8.828100000000001</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>2551</v>
+        <v>387</v>
       </c>
       <c r="B20" t="n">
-        <v>13.3024</v>
+        <v>17.3399</v>
       </c>
       <c r="C20" t="n">
         <v>0</v>
       </c>
       <c r="D20" t="n">
-        <v>6.6512</v>
+        <v>8.66995</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>437</v>
+        <v>1152</v>
       </c>
       <c r="B21" t="n">
-        <v>13.2796</v>
+        <v>17.06301666666667</v>
       </c>
       <c r="C21" t="n">
         <v>0</v>
       </c>
       <c r="D21" t="n">
-        <v>6.639800000000001</v>
+        <v>8.531508333333333</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>322</v>
+        <v>1128</v>
       </c>
       <c r="B22" t="n">
-        <v>13.0708</v>
+        <v>16.9528</v>
       </c>
       <c r="C22" t="n">
         <v>0</v>
       </c>
       <c r="D22" t="n">
-        <v>6.5354</v>
+        <v>8.4764</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>1416</v>
+        <v>2397</v>
       </c>
       <c r="B23" t="n">
-        <v>12.5782</v>
+        <v>16.70228333333333</v>
       </c>
       <c r="C23" t="n">
         <v>0</v>
       </c>
       <c r="D23" t="n">
-        <v>6.2891</v>
+        <v>8.351141666666667</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>2311</v>
+        <v>1424</v>
       </c>
       <c r="B24" t="n">
-        <v>12.56125</v>
+        <v>16.6778</v>
       </c>
       <c r="C24" t="n">
         <v>0</v>
       </c>
       <c r="D24" t="n">
-        <v>6.280625000000001</v>
+        <v>8.338900000000001</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>1403</v>
+        <v>1206</v>
       </c>
       <c r="B25" t="n">
-        <v>12.56125</v>
+        <v>16.4878</v>
       </c>
       <c r="C25" t="n">
         <v>0</v>
       </c>
       <c r="D25" t="n">
-        <v>6.280625000000001</v>
+        <v>8.2439</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>441</v>
+        <v>324</v>
       </c>
       <c r="B26" t="n">
-        <v>12.44855</v>
+        <v>16.47103333333333</v>
       </c>
       <c r="C26" t="n">
         <v>0</v>
       </c>
       <c r="D26" t="n">
-        <v>6.224275</v>
+        <v>8.235516666666667</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>1138</v>
+        <v>2543</v>
       </c>
       <c r="B27" t="n">
-        <v>12.40758333333333</v>
+        <v>16.3458</v>
       </c>
       <c r="C27" t="n">
         <v>0</v>
       </c>
       <c r="D27" t="n">
-        <v>6.203791666666667</v>
+        <v>8.1729</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>433</v>
+        <v>590</v>
       </c>
       <c r="B28" t="n">
-        <v>12.37695</v>
+        <v>16.2456</v>
       </c>
       <c r="C28" t="n">
         <v>0</v>
       </c>
       <c r="D28" t="n">
-        <v>6.188475</v>
+        <v>8.1228</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>449</v>
+        <v>1552</v>
       </c>
       <c r="B29" t="n">
-        <v>12.28618333333333</v>
+        <v>16.1635</v>
       </c>
       <c r="C29" t="n">
         <v>0</v>
       </c>
       <c r="D29" t="n">
-        <v>6.143091666666666</v>
+        <v>8.08175</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>590</v>
+        <v>217</v>
       </c>
       <c r="B30" t="n">
-        <v>12.18583333333333</v>
+        <v>16.0601</v>
       </c>
       <c r="C30" t="n">
         <v>0</v>
       </c>
       <c r="D30" t="n">
-        <v>6.092916666666667</v>
+        <v>8.030049999999999</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>1141</v>
+        <v>729</v>
       </c>
       <c r="B31" t="n">
-        <v>11.93525</v>
+        <v>16.0269</v>
       </c>
       <c r="C31" t="n">
         <v>0</v>
       </c>
       <c r="D31" t="n">
-        <v>5.967625</v>
+        <v>8.013450000000001</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>387</v>
+        <v>379</v>
       </c>
       <c r="B32" t="n">
-        <v>11.74676666666667</v>
+        <v>15.8564</v>
       </c>
       <c r="C32" t="n">
         <v>0</v>
       </c>
       <c r="D32" t="n">
-        <v>5.873383333333334</v>
+        <v>7.9282</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>1180</v>
+        <v>250</v>
       </c>
       <c r="B33" t="n">
-        <v>11.74523333333333</v>
+        <v>15.83211666666667</v>
       </c>
       <c r="C33" t="n">
         <v>0</v>
       </c>
       <c r="D33" t="n">
-        <v>5.872616666666667</v>
+        <v>7.916058333333335</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>485</v>
+        <v>1624</v>
       </c>
       <c r="B34" t="n">
-        <v>11.5971</v>
+        <v>15.82224</v>
       </c>
       <c r="C34" t="n">
         <v>0</v>
       </c>
       <c r="D34" t="n">
-        <v>5.79855</v>
+        <v>7.911119999999999</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>508</v>
+        <v>322</v>
       </c>
       <c r="B35" t="n">
-        <v>11.3368</v>
+        <v>15.8208</v>
       </c>
       <c r="C35" t="n">
         <v>0</v>
       </c>
       <c r="D35" t="n">
-        <v>5.668400000000001</v>
+        <v>7.910399999999999</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>692</v>
+        <v>680</v>
       </c>
       <c r="B36" t="n">
-        <v>11.2902</v>
+        <v>15.60504</v>
       </c>
       <c r="C36" t="n">
         <v>0</v>
       </c>
       <c r="D36" t="n">
-        <v>5.645099999999999</v>
+        <v>7.802519999999999</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>250</v>
+        <v>449</v>
       </c>
       <c r="B37" t="n">
-        <v>11.27685</v>
+        <v>15.55305</v>
       </c>
       <c r="C37" t="n">
         <v>0</v>
       </c>
       <c r="D37" t="n">
-        <v>5.638425</v>
+        <v>7.776524999999999</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>548</v>
+        <v>2456</v>
       </c>
       <c r="B38" t="n">
-        <v>11.212775</v>
+        <v>15.52345</v>
       </c>
       <c r="C38" t="n">
         <v>0</v>
       </c>
       <c r="D38" t="n">
-        <v>5.6063875</v>
+        <v>7.761724999999999</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="n">
-        <v>1590</v>
+        <v>496</v>
       </c>
       <c r="B39" t="n">
-        <v>11.0792</v>
+        <v>15.51408</v>
       </c>
       <c r="C39" t="n">
         <v>0</v>
       </c>
       <c r="D39" t="n">
-        <v>5.5396</v>
+        <v>7.757039999999999</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="n">
-        <v>1128</v>
+        <v>245</v>
       </c>
       <c r="B40" t="n">
-        <v>10.92496666666667</v>
+        <v>15.43988</v>
       </c>
       <c r="C40" t="n">
         <v>0</v>
       </c>
       <c r="D40" t="n">
-        <v>5.462483333333334</v>
+        <v>7.719939999999999</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="n">
-        <v>1222</v>
+        <v>492</v>
       </c>
       <c r="B41" t="n">
-        <v>10.8884</v>
+        <v>15.40115</v>
       </c>
       <c r="C41" t="n">
         <v>0</v>
       </c>
       <c r="D41" t="n">
-        <v>5.4442</v>
+        <v>7.700575</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="n">
-        <v>521</v>
+        <v>254</v>
       </c>
       <c r="B42" t="n">
-        <v>10.8278</v>
+        <v>15.23838</v>
       </c>
       <c r="C42" t="n">
         <v>0</v>
       </c>
       <c r="D42" t="n">
-        <v>5.4139</v>
+        <v>7.619190000000001</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="n">
-        <v>324</v>
+        <v>1129</v>
       </c>
       <c r="B43" t="n">
-        <v>10.57726666666667</v>
+        <v>13.87706</v>
       </c>
       <c r="C43" t="n">
-        <v>0</v>
+        <v>0.9463884631792704</v>
       </c>
       <c r="D43" t="n">
-        <v>5.288633333333333</v>
+        <v>7.195416027357195</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="n">
-        <v>379</v>
+        <v>567</v>
       </c>
       <c r="B44" t="n">
-        <v>10.57093333333333</v>
+        <v>14.08405</v>
       </c>
       <c r="C44" t="n">
         <v>0</v>
       </c>
       <c r="D44" t="n">
-        <v>5.285466666666667</v>
+        <v>7.042025000000001</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="n">
-        <v>2552</v>
+        <v>2540</v>
       </c>
       <c r="B45" t="n">
-        <v>10.493525</v>
+        <v>13.93604</v>
       </c>
       <c r="C45" t="n">
         <v>0</v>
       </c>
       <c r="D45" t="n">
-        <v>5.2467625</v>
+        <v>6.96802</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="n">
-        <v>495</v>
+        <v>727</v>
       </c>
       <c r="B46" t="n">
-        <v>10.40853333333333</v>
+        <v>13.9322</v>
       </c>
       <c r="C46" t="n">
         <v>0</v>
       </c>
       <c r="D46" t="n">
-        <v>5.204266666666666</v>
+        <v>6.9661</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="n">
-        <v>710</v>
+        <v>1431</v>
       </c>
       <c r="B47" t="n">
-        <v>10.3645</v>
+        <v>13.93125</v>
       </c>
       <c r="C47" t="n">
         <v>0</v>
       </c>
       <c r="D47" t="n">
-        <v>5.18225</v>
+        <v>6.965624999999999</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="n">
-        <v>488</v>
+        <v>1232</v>
       </c>
       <c r="B48" t="n">
-        <v>10.303</v>
+        <v>13.74234</v>
       </c>
       <c r="C48" t="n">
         <v>0</v>
       </c>
       <c r="D48" t="n">
-        <v>5.1515</v>
+        <v>6.871170000000001</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="n">
-        <v>1018</v>
+        <v>383</v>
       </c>
       <c r="B49" t="n">
-        <v>9.965299999999999</v>
+        <v>13.60773333333333</v>
       </c>
       <c r="C49" t="n">
         <v>0</v>
       </c>
       <c r="D49" t="n">
-        <v>4.98265</v>
+        <v>6.803866666666667</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="n">
-        <v>382</v>
+        <v>1174</v>
       </c>
       <c r="B50" t="n">
-        <v>9.8978</v>
+        <v>13.4645</v>
       </c>
       <c r="C50" t="n">
         <v>0</v>
       </c>
       <c r="D50" t="n">
-        <v>4.9489</v>
+        <v>6.732250000000001</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="n">
-        <v>2521</v>
+        <v>708</v>
       </c>
       <c r="B51" t="n">
-        <v>9.842599999999999</v>
+        <v>13.23223333333333</v>
       </c>
       <c r="C51" t="n">
         <v>0</v>
       </c>
       <c r="D51" t="n">
-        <v>4.9213</v>
+        <v>6.616116666666667</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="n">
-        <v>2329</v>
+        <v>850</v>
       </c>
       <c r="B52" t="n">
         <v>0</v>
       </c>
       <c r="C52" t="n">
-        <v>0.9453446269035339</v>
+        <v>0.912351131439209</v>
       </c>
       <c r="D52" t="n">
-        <v>0.2570238676916931</v>
+        <v>0.2614582603476732</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="n">
-        <v>1858</v>
+        <v>1817</v>
       </c>
       <c r="B53" t="n">
         <v>0</v>
       </c>
       <c r="C53" t="n">
-        <v>0.9528844356536865</v>
+        <v>0.9150002002716064</v>
       </c>
       <c r="D53" t="n">
-        <v>0.2560315351341492</v>
+        <v>0.2610965784385216</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="n">
-        <v>770</v>
+        <v>2431</v>
       </c>
       <c r="B54" t="n">
         <v>0</v>
       </c>
       <c r="C54" t="n">
-        <v>0.9569736272096634</v>
+        <v>0.9183939695358276</v>
       </c>
       <c r="D54" t="n">
-        <v>0.2554965447914193</v>
+        <v>0.2606346808528487</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="n">
-        <v>355</v>
+        <v>1851</v>
       </c>
       <c r="B55" t="n">
         <v>0</v>
       </c>
       <c r="C55" t="n">
-        <v>0.9574544827143351</v>
+        <v>0.9198936820030212</v>
       </c>
       <c r="D55" t="n">
-        <v>0.2554337811761871</v>
+        <v>0.2604310877664596</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="n">
-        <v>518</v>
+        <v>391</v>
       </c>
       <c r="B56" t="n">
         <v>0</v>
       </c>
       <c r="C56" t="n">
-        <v>0.957507848739624</v>
+        <v>0.9204611778259277</v>
       </c>
       <c r="D56" t="n">
-        <v>0.2554268174822051</v>
+        <v>0.2603541304417456</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="n">
-        <v>2081</v>
+        <v>1907</v>
       </c>
       <c r="B57" t="n">
         <v>0</v>
       </c>
       <c r="C57" t="n">
-        <v>0.9575464129447937</v>
+        <v>0.9270520210266113</v>
       </c>
       <c r="D57" t="n">
-        <v>0.2554217855033309</v>
+        <v>0.2594636753675345</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="n">
-        <v>1673</v>
+        <v>1787</v>
       </c>
       <c r="B58" t="n">
         <v>0</v>
       </c>
       <c r="C58" t="n">
-        <v>0.9583358764648438</v>
+        <v>0.9284092783927917</v>
       </c>
       <c r="D58" t="n">
-        <v>0.2553188173739593</v>
+        <v>0.259281059058541</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="n">
-        <v>632</v>
+        <v>835</v>
       </c>
       <c r="B59" t="n">
         <v>0</v>
       </c>
       <c r="C59" t="n">
-        <v>0.9590025544166565</v>
+        <v>0.9287458658218384</v>
       </c>
       <c r="D59" t="n">
-        <v>0.2552319285509497</v>
+        <v>0.2592358116536779</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="n">
-        <v>1425</v>
+        <v>2568</v>
       </c>
       <c r="B60" t="n">
         <v>0</v>
       </c>
       <c r="C60" t="n">
-        <v>0.9594849348068237</v>
+        <v>0.9297153949737549</v>
       </c>
       <c r="D60" t="n">
-        <v>0.2551690962856484</v>
+        <v>0.2591055661898786</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="n">
-        <v>2190</v>
+        <v>104</v>
       </c>
       <c r="B61" t="n">
         <v>0</v>
       </c>
       <c r="C61" t="n">
-        <v>0.9601365625858307</v>
+        <v>0.9297687709331512</v>
       </c>
       <c r="D61" t="n">
-        <v>0.2550842678738645</v>
+        <v>0.2590983995239088</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="n">
-        <v>2489</v>
+        <v>1909</v>
       </c>
       <c r="B62" t="n">
         <v>0</v>
       </c>
       <c r="C62" t="n">
-        <v>0.9602958957354227</v>
+        <v>0.9307088454564413</v>
       </c>
       <c r="D62" t="n">
-        <v>0.25506353458564</v>
+        <v>0.2589722428509382</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="n">
-        <v>611</v>
+        <v>1799</v>
       </c>
       <c r="B63" t="n">
         <v>0</v>
       </c>
       <c r="C63" t="n">
-        <v>0.9604105353355408</v>
+        <v>0.9329041242599487</v>
       </c>
       <c r="D63" t="n">
-        <v>0.2550486191477342</v>
+        <v>0.2586781174112477</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="n">
-        <v>1887</v>
+        <v>2515</v>
       </c>
       <c r="B64" t="n">
         <v>0</v>
       </c>
       <c r="C64" t="n">
-        <v>0.9604355335235596</v>
+        <v>0.9349757432937622</v>
       </c>
       <c r="D64" t="n">
-        <v>0.2550453669350364</v>
+        <v>0.2584011720730349</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="n">
-        <v>2199</v>
+        <v>2073</v>
       </c>
       <c r="B65" t="n">
         <v>0</v>
       </c>
       <c r="C65" t="n">
-        <v>0.9604778289794922</v>
+        <v>0.9355558753013611</v>
       </c>
       <c r="D65" t="n">
-        <v>0.2550398645723375</v>
+        <v>0.2583237231124373</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="n">
-        <v>2523</v>
+        <v>2567</v>
       </c>
       <c r="B66" t="n">
         <v>0</v>
       </c>
       <c r="C66" t="n">
-        <v>0.960755243897438</v>
+        <v>0.9369664788246155</v>
       </c>
       <c r="D66" t="n">
-        <v>0.2550037805871877</v>
+        <v>0.2581355978361632</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="n">
-        <v>862</v>
+        <v>1980</v>
       </c>
       <c r="B67" t="n">
         <v>0</v>
       </c>
       <c r="C67" t="n">
-        <v>0.9607909818490347</v>
+        <v>0.9372656345367432</v>
       </c>
       <c r="D67" t="n">
-        <v>0.2549991328134821</v>
+        <v>0.2580957361170372</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="n">
-        <v>1417</v>
+        <v>1855</v>
       </c>
       <c r="B68" t="n">
         <v>0</v>
       </c>
       <c r="C68" t="n">
-        <v>0.9613137245178223</v>
+        <v>0.9380872845649719</v>
       </c>
       <c r="D68" t="n">
-        <v>0.2549311687108711</v>
+        <v>0.2579863167061804</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="n">
-        <v>2200</v>
+        <v>1198</v>
       </c>
       <c r="B69" t="n">
         <v>0</v>
       </c>
       <c r="C69" t="n">
-        <v>0.9613693952560425</v>
+        <v>0.9380983114242554</v>
       </c>
       <c r="D69" t="n">
-        <v>0.2549239328447503</v>
+        <v>0.2579848488865168</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="n">
-        <v>2188</v>
+        <v>2416</v>
       </c>
       <c r="B70" t="n">
         <v>0</v>
       </c>
       <c r="C70" t="n">
-        <v>0.962033212184906</v>
+        <v>0.9386406242847443</v>
       </c>
       <c r="D70" t="n">
-        <v>0.2548376841405267</v>
+        <v>0.2579126805332853</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="n">
-        <v>285</v>
+        <v>2478</v>
       </c>
       <c r="B71" t="n">
         <v>0</v>
       </c>
       <c r="C71" t="n">
-        <v>0.9629416366418203</v>
+        <v>0.9386791586875916</v>
       </c>
       <c r="D71" t="n">
-        <v>0.2547197484971558</v>
+        <v>0.2579075540990909</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="n">
-        <v>606</v>
+        <v>1853</v>
       </c>
       <c r="B72" t="n">
         <v>0</v>
       </c>
       <c r="C72" t="n">
-        <v>0.9631214241186777</v>
+        <v>0.9387034177780151</v>
       </c>
       <c r="D72" t="n">
-        <v>0.2546964206375923</v>
+        <v>0.2579043268892874</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="n">
-        <v>2198</v>
+        <v>292</v>
       </c>
       <c r="B73" t="n">
         <v>0</v>
       </c>
       <c r="C73" t="n">
-        <v>0.9634656310081482</v>
+        <v>0.9387832581996918</v>
       </c>
       <c r="D73" t="n">
-        <v>0.2546517708808956</v>
+        <v>0.2578937062125697</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="n">
-        <v>994</v>
+        <v>1675</v>
       </c>
       <c r="B74" t="n">
         <v>0</v>
       </c>
       <c r="C74" t="n">
-        <v>0.9639216164747874</v>
+        <v>0.9388269782066345</v>
       </c>
       <c r="D74" t="n">
-        <v>0.254592645554507</v>
+        <v>0.2578878907815112</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="n">
-        <v>1166</v>
+        <v>1801</v>
       </c>
       <c r="B75" t="n">
         <v>0</v>
       </c>
       <c r="C75" t="n">
-        <v>0.9644019961357116</v>
+        <v>0.9389307796955109</v>
       </c>
       <c r="D75" t="n">
-        <v>0.2545303868472842</v>
+        <v>0.257874084642939</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="n">
-        <v>1246</v>
+        <v>2151</v>
       </c>
       <c r="B76" t="n">
         <v>0</v>
       </c>
       <c r="C76" t="n">
-        <v>0.9644186993439993</v>
+        <v>0.9389899174372355</v>
       </c>
       <c r="D76" t="n">
-        <v>0.2545282226070087</v>
+        <v>0.2578662196762995</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="n">
-        <v>2384</v>
+        <v>2219</v>
       </c>
       <c r="B77" t="n">
         <v>0</v>
       </c>
       <c r="C77" t="n">
-        <v>0.9648047089576721</v>
+        <v>0.9390560507774353</v>
       </c>
       <c r="D77" t="n">
-        <v>0.2544782174637854</v>
+        <v>0.2578574249050369</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="n">
-        <v>1810</v>
+        <v>417</v>
       </c>
       <c r="B78" t="n">
         <v>0</v>
       </c>
       <c r="C78" t="n">
-        <v>0.964876389503479</v>
+        <v>0.9396763741970062</v>
       </c>
       <c r="D78" t="n">
-        <v>0.2544689338581493</v>
+        <v>0.2577749601177628</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="n">
-        <v>608</v>
+        <v>1183</v>
       </c>
       <c r="B79" t="n">
         <v>0</v>
       </c>
       <c r="C79" t="n">
-        <v>0.9650090932846069</v>
+        <v>0.9398043553034464</v>
       </c>
       <c r="D79" t="n">
-        <v>0.2544517487011859</v>
+        <v>0.2577579530806777</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="n">
-        <v>963</v>
+        <v>1617</v>
       </c>
       <c r="B80" t="n">
         <v>0</v>
       </c>
       <c r="C80" t="n">
-        <v>0.9653818607330322</v>
+        <v>0.9402076005935669</v>
       </c>
       <c r="D80" t="n">
-        <v>0.2544034876833116</v>
+        <v>0.2577043816584551</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="n">
-        <v>1811</v>
+        <v>1613</v>
       </c>
       <c r="B81" t="n">
         <v>0</v>
       </c>
       <c r="C81" t="n">
-        <v>0.9659088015556335</v>
+        <v>0.9402670661608378</v>
       </c>
       <c r="D81" t="n">
-        <v>0.2543352975500936</v>
+        <v>0.2576964834997373</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="n">
-        <v>1154</v>
+        <v>1523</v>
       </c>
       <c r="B82" t="n">
         <v>0</v>
       </c>
       <c r="C82" t="n">
-        <v>0.9659820318222045</v>
+        <v>0.9407958507537841</v>
       </c>
       <c r="D82" t="n">
-        <v>0.2543258238919744</v>
+        <v>0.2576262721325406</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="n">
-        <v>483</v>
+        <v>98</v>
       </c>
       <c r="B83" t="n">
         <v>0</v>
       </c>
       <c r="C83" t="n">
-        <v>0.9667567610740662</v>
+        <v>0.941187858581543</v>
       </c>
       <c r="D83" t="n">
-        <v>0.2542256418770081</v>
+        <v>0.2575742465056206</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="n">
-        <v>2328</v>
+        <v>583</v>
       </c>
       <c r="B84" t="n">
         <v>0</v>
       </c>
       <c r="C84" t="n">
-        <v>0.967527449131012</v>
+        <v>0.9416183352470398</v>
       </c>
       <c r="D84" t="n">
-        <v>0.2541260607168823</v>
+        <v>0.2575171396578221</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="n">
-        <v>2402</v>
+        <v>584</v>
       </c>
       <c r="B85" t="n">
         <v>0</v>
       </c>
       <c r="C85" t="n">
-        <v>0.9678566753864288</v>
+        <v>0.9417591293652853</v>
       </c>
       <c r="D85" t="n">
-        <v>0.2540835449318558</v>
+        <v>0.2574984674661672</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="n">
-        <v>1470</v>
+        <v>1091</v>
       </c>
       <c r="B86" t="n">
         <v>0</v>
       </c>
       <c r="C86" t="n">
-        <v>0.96910480260849</v>
+        <v>0.9428647607564926</v>
       </c>
       <c r="D86" t="n">
-        <v>0.2539224927681075</v>
+        <v>0.2573519321053078</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="n">
-        <v>2325</v>
+        <v>268</v>
       </c>
       <c r="B87" t="n">
         <v>0</v>
       </c>
       <c r="C87" t="n">
-        <v>0.9695784449577332</v>
+        <v>0.9430677195390066</v>
       </c>
       <c r="D87" t="n">
-        <v>0.2538614297288017</v>
+        <v>0.2573250509861927</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="n">
-        <v>82</v>
+        <v>346</v>
       </c>
       <c r="B88" t="n">
         <v>0</v>
       </c>
       <c r="C88" t="n">
-        <v>0.9699375629425049</v>
+        <v>0.9431021809577942</v>
       </c>
       <c r="D88" t="n">
-        <v>0.253815151000597</v>
+        <v>0.2573204872599855</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="n">
-        <v>636</v>
+        <v>2106</v>
       </c>
       <c r="B89" t="n">
         <v>0</v>
       </c>
       <c r="C89" t="n">
-        <v>0.9700133800506592</v>
+        <v>0.9437994956970215</v>
       </c>
       <c r="D89" t="n">
-        <v>0.2538053827772187</v>
+        <v>0.2572281766235907</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="n">
-        <v>1075</v>
+        <v>450</v>
       </c>
       <c r="B90" t="n">
         <v>0</v>
       </c>
       <c r="C90" t="n">
-        <v>0.9702716469764709</v>
+        <v>0.9445163488388062</v>
       </c>
       <c r="D90" t="n">
-        <v>0.253772113488659</v>
+        <v>0.2571333485051857</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="n">
-        <v>2367</v>
+        <v>1179</v>
       </c>
       <c r="B91" t="n">
         <v>0</v>
       </c>
       <c r="C91" t="n">
-        <v>0.9706962108612061</v>
+        <v>0.9445422887802124</v>
       </c>
       <c r="D91" t="n">
-        <v>0.2537174411988629</v>
+        <v>0.2571299183797355</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="n">
-        <v>2389</v>
+        <v>1505</v>
       </c>
       <c r="B92" t="n">
         <v>0</v>
       </c>
       <c r="C92" t="n">
-        <v>0.9709201355775198</v>
+        <v>0.945213258266449</v>
       </c>
       <c r="D92" t="n">
-        <v>0.2536886152687713</v>
+        <v>0.2570412256215003</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="n">
-        <v>2518</v>
+        <v>266</v>
       </c>
       <c r="B93" t="n">
         <v>0</v>
       </c>
       <c r="C93" t="n">
-        <v>0.9711668690045675</v>
+        <v>0.945323626200358</v>
       </c>
       <c r="D93" t="n">
-        <v>0.2536568607469028</v>
+        <v>0.257026642387832</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="n">
-        <v>1813</v>
+        <v>1800</v>
       </c>
       <c r="B94" t="n">
         <v>0</v>
       </c>
       <c r="C94" t="n">
-        <v>0.9712480505307516</v>
+        <v>0.9473799367745718</v>
       </c>
       <c r="D94" t="n">
-        <v>0.2536464144455979</v>
+        <v>0.2567552384400887</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="n">
-        <v>1886</v>
+        <v>2422</v>
       </c>
       <c r="B95" t="n">
         <v>0</v>
       </c>
       <c r="C95" t="n">
-        <v>0.9713016152381897</v>
+        <v>0.9480330348014832</v>
       </c>
       <c r="D95" t="n">
-        <v>0.2536395223008964</v>
+        <v>0.2566691586166829</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="n">
-        <v>2361</v>
+        <v>723</v>
       </c>
       <c r="B96" t="n">
         <v>0</v>
       </c>
       <c r="C96" t="n">
-        <v>0.9720018406709036</v>
+        <v>0.9484446744124094</v>
       </c>
       <c r="D96" t="n">
-        <v>0.2535494590765152</v>
+        <v>0.2566149332163021</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="n">
-        <v>2349</v>
+        <v>728</v>
       </c>
       <c r="B97" t="n">
         <v>0</v>
       </c>
       <c r="C97" t="n">
-        <v>0.9720470905303955</v>
+        <v>0.9484995007514954</v>
       </c>
       <c r="D97" t="n">
-        <v>0.2535436412248764</v>
+        <v>0.256607712656411</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="n">
-        <v>287</v>
+        <v>846</v>
       </c>
       <c r="B98" t="n">
         <v>0</v>
       </c>
       <c r="C98" t="n">
-        <v>0.9725315570831299</v>
+        <v>0.9486296296119689</v>
       </c>
       <c r="D98" t="n">
-        <v>0.2534813692610182</v>
+        <v>0.2565905764758207</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="n">
-        <v>2087</v>
+        <v>526</v>
       </c>
       <c r="B99" t="n">
         <v>0</v>
       </c>
       <c r="C99" t="n">
-        <v>0.9740772247314453</v>
+        <v>0.9488712052504221</v>
       </c>
       <c r="D99" t="n">
-        <v>0.2532828978197751</v>
+        <v>0.2565587703553515</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="n">
-        <v>1421</v>
+        <v>528</v>
       </c>
       <c r="B100" t="n">
         <v>0</v>
       </c>
       <c r="C100" t="n">
-        <v>0.9744594931602478</v>
+        <v>0.9502724707126617</v>
       </c>
       <c r="D100" t="n">
-        <v>0.2532338605740239</v>
-      </c>
-    </row>
-    <row r="101">
-      <c r="A101" t="n">
-        <v>1469</v>
-      </c>
-      <c r="B101" t="n">
-        <v>0</v>
-      </c>
-      <c r="C101" t="n">
-        <v>0.9744958380858103</v>
-      </c>
-      <c r="D101" t="n">
-        <v>0.2532291992495303</v>
+        <v>0.2563744335771154</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changed dirs, added tqdm, tested the environment
</commit_message>
<xml_diff>
--- a/output/scores.xlsx
+++ b/output/scores.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -457,329 +457,329 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>1137</v>
+        <v>1048</v>
       </c>
       <c r="B2" t="n">
-        <v>27.3247</v>
+        <v>26.41443333333333</v>
       </c>
       <c r="C2" t="n">
         <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>13.66235</v>
+        <v>13.20721666666667</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>2526</v>
+        <v>2318</v>
       </c>
       <c r="B3" t="n">
-        <v>25.24983333333333</v>
+        <v>20.9372</v>
       </c>
       <c r="C3" t="n">
         <v>0</v>
       </c>
       <c r="D3" t="n">
-        <v>12.62491666666667</v>
+        <v>10.4686</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>1418</v>
+        <v>2002</v>
       </c>
       <c r="B4" t="n">
-        <v>23.8757</v>
+        <v>20.21796666666667</v>
       </c>
       <c r="C4" t="n">
         <v>0</v>
       </c>
       <c r="D4" t="n">
-        <v>11.93785</v>
+        <v>10.10898333333333</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>548</v>
+        <v>500</v>
       </c>
       <c r="B5" t="n">
-        <v>21.0437</v>
+        <v>18.88663333333333</v>
       </c>
       <c r="C5" t="n">
         <v>0</v>
       </c>
       <c r="D5" t="n">
-        <v>10.52185</v>
+        <v>9.443316666666666</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>437</v>
+        <v>2083</v>
       </c>
       <c r="B6" t="n">
-        <v>20.9372</v>
+        <v>18.875</v>
       </c>
       <c r="C6" t="n">
         <v>0</v>
       </c>
       <c r="D6" t="n">
-        <v>10.4686</v>
+        <v>9.4375</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>1416</v>
+        <v>369</v>
       </c>
       <c r="B7" t="n">
-        <v>20.4617</v>
+        <v>18.8174</v>
       </c>
       <c r="C7" t="n">
         <v>0</v>
       </c>
       <c r="D7" t="n">
-        <v>10.23085</v>
+        <v>9.4087</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>1582</v>
+        <v>1625</v>
       </c>
       <c r="B8" t="n">
-        <v>20.38293333333333</v>
+        <v>18.6248</v>
       </c>
       <c r="C8" t="n">
         <v>0</v>
       </c>
       <c r="D8" t="n">
-        <v>10.19146666666667</v>
+        <v>9.3124</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>1207</v>
+        <v>426</v>
       </c>
       <c r="B9" t="n">
-        <v>19.17853333333333</v>
+        <v>18.5818</v>
       </c>
       <c r="C9" t="n">
         <v>0</v>
       </c>
       <c r="D9" t="n">
-        <v>9.589266666666665</v>
+        <v>9.290900000000001</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>486</v>
+        <v>2381</v>
       </c>
       <c r="B10" t="n">
-        <v>18.875</v>
+        <v>18.32926666666667</v>
       </c>
       <c r="C10" t="n">
         <v>0</v>
       </c>
       <c r="D10" t="n">
-        <v>9.4375</v>
+        <v>9.164633333333333</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>780</v>
+        <v>2118</v>
       </c>
       <c r="B11" t="n">
-        <v>18.6248</v>
+        <v>18.2293</v>
       </c>
       <c r="C11" t="n">
         <v>0</v>
       </c>
       <c r="D11" t="n">
-        <v>9.3124</v>
+        <v>9.114649999999999</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>527</v>
+        <v>56</v>
       </c>
       <c r="B12" t="n">
-        <v>18.5818</v>
+        <v>18.1017</v>
       </c>
       <c r="C12" t="n">
         <v>0</v>
       </c>
       <c r="D12" t="n">
-        <v>9.290900000000001</v>
+        <v>9.050850000000001</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>1141</v>
+        <v>1074</v>
       </c>
       <c r="B13" t="n">
-        <v>18.4093</v>
+        <v>17.9203</v>
       </c>
       <c r="C13" t="n">
         <v>0</v>
       </c>
       <c r="D13" t="n">
-        <v>9.204650000000001</v>
+        <v>8.960150000000001</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>521</v>
+        <v>779</v>
       </c>
       <c r="B14" t="n">
-        <v>18.2293</v>
+        <v>17.7746</v>
       </c>
       <c r="C14" t="n">
         <v>0</v>
       </c>
       <c r="D14" t="n">
-        <v>9.114649999999999</v>
+        <v>8.8873</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>2117</v>
+        <v>1718</v>
       </c>
       <c r="B15" t="n">
-        <v>18.1017</v>
+        <v>17.67</v>
       </c>
       <c r="C15" t="n">
         <v>0</v>
       </c>
       <c r="D15" t="n">
-        <v>9.050850000000001</v>
+        <v>8.835000000000001</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>2552</v>
+        <v>1690</v>
       </c>
       <c r="B16" t="n">
-        <v>17.9203</v>
+        <v>17.48663333333333</v>
       </c>
       <c r="C16" t="n">
         <v>0</v>
       </c>
       <c r="D16" t="n">
-        <v>8.960150000000001</v>
+        <v>8.743316666666667</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>967</v>
+        <v>2006</v>
       </c>
       <c r="B17" t="n">
-        <v>17.7746</v>
+        <v>17.4389</v>
       </c>
       <c r="C17" t="n">
         <v>0</v>
       </c>
       <c r="D17" t="n">
-        <v>8.8873</v>
+        <v>8.71945</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>1180</v>
+        <v>2268</v>
       </c>
       <c r="B18" t="n">
-        <v>17.67</v>
+        <v>17.3399</v>
       </c>
       <c r="C18" t="n">
         <v>0</v>
       </c>
       <c r="D18" t="n">
-        <v>8.835000000000001</v>
+        <v>8.66995</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>246</v>
+        <v>933</v>
       </c>
       <c r="B19" t="n">
-        <v>17.6562</v>
+        <v>17.014775</v>
       </c>
       <c r="C19" t="n">
         <v>0</v>
       </c>
       <c r="D19" t="n">
-        <v>8.828100000000001</v>
+        <v>8.5073875</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>387</v>
+        <v>1666</v>
       </c>
       <c r="B20" t="n">
-        <v>17.3399</v>
+        <v>16.9528</v>
       </c>
       <c r="C20" t="n">
         <v>0</v>
       </c>
       <c r="D20" t="n">
-        <v>8.66995</v>
+        <v>8.4764</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>1152</v>
+        <v>371</v>
       </c>
       <c r="B21" t="n">
-        <v>17.06301666666667</v>
+        <v>16.9369</v>
       </c>
       <c r="C21" t="n">
         <v>0</v>
       </c>
       <c r="D21" t="n">
-        <v>8.531508333333333</v>
+        <v>8.468450000000001</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>1128</v>
+        <v>466</v>
       </c>
       <c r="B22" t="n">
-        <v>16.9528</v>
+        <v>16.8992</v>
       </c>
       <c r="C22" t="n">
         <v>0</v>
       </c>
       <c r="D22" t="n">
-        <v>8.4764</v>
+        <v>8.4496</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>2397</v>
+        <v>568</v>
       </c>
       <c r="B23" t="n">
-        <v>16.70228333333333</v>
+        <v>16.6778</v>
       </c>
       <c r="C23" t="n">
         <v>0</v>
       </c>
       <c r="D23" t="n">
-        <v>8.351141666666667</v>
+        <v>8.338900000000001</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>1424</v>
+        <v>2385</v>
       </c>
       <c r="B24" t="n">
-        <v>16.6778</v>
+        <v>16.66301666666667</v>
       </c>
       <c r="C24" t="n">
         <v>0</v>
       </c>
       <c r="D24" t="n">
-        <v>8.338900000000001</v>
+        <v>8.331508333333334</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>1206</v>
+        <v>499</v>
       </c>
       <c r="B25" t="n">
         <v>16.4878</v>
@@ -793,1052 +793,1052 @@
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>324</v>
+        <v>1065</v>
       </c>
       <c r="B26" t="n">
-        <v>16.47103333333333</v>
+        <v>16.3458</v>
       </c>
       <c r="C26" t="n">
         <v>0</v>
       </c>
       <c r="D26" t="n">
-        <v>8.235516666666667</v>
+        <v>8.1729</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>2543</v>
+        <v>489</v>
       </c>
       <c r="B27" t="n">
-        <v>16.3458</v>
+        <v>16.2456</v>
       </c>
       <c r="C27" t="n">
         <v>0</v>
       </c>
       <c r="D27" t="n">
-        <v>8.1729</v>
+        <v>8.1228</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>590</v>
+        <v>1972</v>
       </c>
       <c r="B28" t="n">
-        <v>16.2456</v>
+        <v>16.1635</v>
       </c>
       <c r="C28" t="n">
         <v>0</v>
       </c>
       <c r="D28" t="n">
-        <v>8.1228</v>
+        <v>8.08175</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>1552</v>
+        <v>1675</v>
       </c>
       <c r="B29" t="n">
-        <v>16.1635</v>
+        <v>16.1279</v>
       </c>
       <c r="C29" t="n">
         <v>0</v>
       </c>
       <c r="D29" t="n">
-        <v>8.08175</v>
+        <v>8.06395</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>217</v>
+        <v>2380</v>
       </c>
       <c r="B30" t="n">
-        <v>16.0601</v>
+        <v>16.09614</v>
       </c>
       <c r="C30" t="n">
         <v>0</v>
       </c>
       <c r="D30" t="n">
-        <v>8.030049999999999</v>
+        <v>8.048069999999999</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>729</v>
+        <v>1919</v>
       </c>
       <c r="B31" t="n">
-        <v>16.0269</v>
+        <v>16.0766</v>
       </c>
       <c r="C31" t="n">
         <v>0</v>
       </c>
       <c r="D31" t="n">
-        <v>8.013450000000001</v>
+        <v>8.0383</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>379</v>
+        <v>1873</v>
       </c>
       <c r="B32" t="n">
-        <v>15.8564</v>
+        <v>16.0601</v>
       </c>
       <c r="C32" t="n">
         <v>0</v>
       </c>
       <c r="D32" t="n">
-        <v>7.9282</v>
+        <v>8.030049999999999</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>250</v>
+        <v>2061</v>
       </c>
       <c r="B33" t="n">
-        <v>15.83211666666667</v>
+        <v>16.0269</v>
       </c>
       <c r="C33" t="n">
         <v>0</v>
       </c>
       <c r="D33" t="n">
-        <v>7.916058333333335</v>
+        <v>8.013450000000001</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>1624</v>
+        <v>2260</v>
       </c>
       <c r="B34" t="n">
-        <v>15.82224</v>
+        <v>15.8564</v>
       </c>
       <c r="C34" t="n">
         <v>0</v>
       </c>
       <c r="D34" t="n">
-        <v>7.911119999999999</v>
+        <v>7.9282</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>322</v>
+        <v>2089</v>
       </c>
       <c r="B35" t="n">
-        <v>15.8208</v>
+        <v>15.7945</v>
       </c>
       <c r="C35" t="n">
         <v>0</v>
       </c>
       <c r="D35" t="n">
-        <v>7.910399999999999</v>
+        <v>7.89725</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>680</v>
+        <v>2378</v>
       </c>
       <c r="B36" t="n">
-        <v>15.60504</v>
+        <v>15.18585</v>
       </c>
       <c r="C36" t="n">
         <v>0</v>
       </c>
       <c r="D36" t="n">
-        <v>7.802519999999999</v>
+        <v>7.592925</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>449</v>
+        <v>901</v>
       </c>
       <c r="B37" t="n">
-        <v>15.55305</v>
+        <v>15.08018333333333</v>
       </c>
       <c r="C37" t="n">
         <v>0</v>
       </c>
       <c r="D37" t="n">
-        <v>7.776524999999999</v>
+        <v>7.540091666666666</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>2456</v>
+        <v>1241</v>
       </c>
       <c r="B38" t="n">
-        <v>15.52345</v>
+        <v>14.62103333333333</v>
       </c>
       <c r="C38" t="n">
         <v>0</v>
       </c>
       <c r="D38" t="n">
-        <v>7.761724999999999</v>
+        <v>7.310516666666667</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="n">
-        <v>496</v>
+        <v>1326</v>
       </c>
       <c r="B39" t="n">
-        <v>15.51408</v>
+        <v>14.45098333333333</v>
       </c>
       <c r="C39" t="n">
         <v>0</v>
       </c>
       <c r="D39" t="n">
-        <v>7.757039999999999</v>
+        <v>7.225491666666667</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="n">
-        <v>245</v>
+        <v>1062</v>
       </c>
       <c r="B40" t="n">
-        <v>15.43988</v>
+        <v>14.42726</v>
       </c>
       <c r="C40" t="n">
         <v>0</v>
       </c>
       <c r="D40" t="n">
-        <v>7.719939999999999</v>
+        <v>7.21363</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="n">
-        <v>492</v>
+        <v>1667</v>
       </c>
       <c r="B41" t="n">
-        <v>15.40115</v>
+        <v>13.82794</v>
       </c>
       <c r="C41" t="n">
-        <v>0</v>
+        <v>0.948314905166626</v>
       </c>
       <c r="D41" t="n">
-        <v>7.700575</v>
+        <v>7.170602025281991</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="n">
-        <v>254</v>
+        <v>1712</v>
       </c>
       <c r="B42" t="n">
-        <v>15.23838</v>
+        <v>14.20155</v>
       </c>
       <c r="C42" t="n">
         <v>0</v>
       </c>
       <c r="D42" t="n">
-        <v>7.619190000000001</v>
+        <v>7.100775</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="n">
-        <v>1129</v>
+        <v>1671</v>
       </c>
       <c r="B43" t="n">
-        <v>13.87706</v>
+        <v>14.08696</v>
       </c>
       <c r="C43" t="n">
-        <v>0.9463884631792704</v>
+        <v>0</v>
       </c>
       <c r="D43" t="n">
-        <v>7.195416027357195</v>
+        <v>7.04348</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="n">
-        <v>567</v>
+        <v>2330</v>
       </c>
       <c r="B44" t="n">
-        <v>14.08405</v>
+        <v>14.0525</v>
       </c>
       <c r="C44" t="n">
         <v>0</v>
       </c>
       <c r="D44" t="n">
-        <v>7.042025000000001</v>
+        <v>7.02625</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="n">
-        <v>2540</v>
+        <v>468</v>
       </c>
       <c r="B45" t="n">
-        <v>13.93604</v>
+        <v>13.993</v>
       </c>
       <c r="C45" t="n">
         <v>0</v>
       </c>
       <c r="D45" t="n">
-        <v>6.96802</v>
+        <v>6.9965</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="n">
-        <v>727</v>
+        <v>2203</v>
       </c>
       <c r="B46" t="n">
-        <v>13.9322</v>
+        <v>13.98746666666667</v>
       </c>
       <c r="C46" t="n">
         <v>0</v>
       </c>
       <c r="D46" t="n">
-        <v>6.9661</v>
+        <v>6.993733333333334</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="n">
-        <v>1431</v>
+        <v>2059</v>
       </c>
       <c r="B47" t="n">
-        <v>13.93125</v>
+        <v>13.9322</v>
       </c>
       <c r="C47" t="n">
         <v>0</v>
       </c>
       <c r="D47" t="n">
-        <v>6.965624999999999</v>
+        <v>6.9661</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="n">
-        <v>1232</v>
+        <v>2389</v>
       </c>
       <c r="B48" t="n">
-        <v>13.74234</v>
+        <v>13.88698</v>
       </c>
       <c r="C48" t="n">
         <v>0</v>
       </c>
       <c r="D48" t="n">
-        <v>6.871170000000001</v>
+        <v>6.94349</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="n">
-        <v>383</v>
+        <v>2205</v>
       </c>
       <c r="B49" t="n">
-        <v>13.60773333333333</v>
+        <v>13.88444</v>
       </c>
       <c r="C49" t="n">
         <v>0</v>
       </c>
       <c r="D49" t="n">
-        <v>6.803866666666667</v>
+        <v>6.942220000000001</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="n">
-        <v>1174</v>
+        <v>447</v>
       </c>
       <c r="B50" t="n">
-        <v>13.4645</v>
+        <v>13.86583333333333</v>
       </c>
       <c r="C50" t="n">
         <v>0</v>
       </c>
       <c r="D50" t="n">
-        <v>6.732250000000001</v>
+        <v>6.932916666666666</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="n">
-        <v>708</v>
+        <v>525</v>
       </c>
       <c r="B51" t="n">
-        <v>13.23223333333333</v>
+        <v>13.74234</v>
       </c>
       <c r="C51" t="n">
         <v>0</v>
       </c>
       <c r="D51" t="n">
-        <v>6.616116666666667</v>
+        <v>6.871170000000001</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="n">
-        <v>850</v>
+        <v>275</v>
       </c>
       <c r="B52" t="n">
         <v>0</v>
       </c>
       <c r="C52" t="n">
-        <v>0.912351131439209</v>
+        <v>0.9123510122299194</v>
       </c>
       <c r="D52" t="n">
-        <v>0.2614582603476732</v>
+        <v>0.2614582766460688</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="n">
-        <v>1817</v>
+        <v>329</v>
       </c>
       <c r="B53" t="n">
         <v>0</v>
       </c>
       <c r="C53" t="n">
-        <v>0.9150002002716064</v>
+        <v>0.915000319480896</v>
       </c>
       <c r="D53" t="n">
-        <v>0.2610965784385216</v>
+        <v>0.2610965621851887</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="n">
-        <v>2431</v>
+        <v>743</v>
       </c>
       <c r="B54" t="n">
         <v>0</v>
       </c>
       <c r="C54" t="n">
-        <v>0.9183939695358276</v>
+        <v>0.9168971180915833</v>
       </c>
       <c r="D54" t="n">
-        <v>0.2606346808528487</v>
+        <v>0.2608382031988175</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="n">
-        <v>1851</v>
+        <v>1216</v>
       </c>
       <c r="B55" t="n">
         <v>0</v>
       </c>
       <c r="C55" t="n">
-        <v>0.9198936820030212</v>
+        <v>0.9183937907218933</v>
       </c>
       <c r="D55" t="n">
-        <v>0.2604310877664596</v>
+        <v>0.2606347051466683</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="n">
-        <v>391</v>
+        <v>363</v>
       </c>
       <c r="B56" t="n">
         <v>0</v>
       </c>
       <c r="C56" t="n">
-        <v>0.9204611778259277</v>
+        <v>0.919893741607666</v>
       </c>
       <c r="D56" t="n">
-        <v>0.2603541304417456</v>
+        <v>0.260431079681167</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="n">
-        <v>1907</v>
+        <v>2272</v>
       </c>
       <c r="B57" t="n">
         <v>0</v>
       </c>
       <c r="C57" t="n">
-        <v>0.9270520210266113</v>
+        <v>0.9204613566398621</v>
       </c>
       <c r="D57" t="n">
-        <v>0.2594636753675345</v>
+        <v>0.2603541062002027</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="n">
-        <v>1787</v>
+        <v>1365</v>
       </c>
       <c r="B58" t="n">
         <v>0</v>
       </c>
       <c r="C58" t="n">
-        <v>0.9284092783927917</v>
+        <v>0.9250795245170593</v>
       </c>
       <c r="D58" t="n">
-        <v>0.259281059058541</v>
+        <v>0.259729529940034</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="n">
-        <v>835</v>
+        <v>1363</v>
       </c>
       <c r="B59" t="n">
         <v>0</v>
       </c>
       <c r="C59" t="n">
-        <v>0.9287458658218384</v>
+        <v>0.927051842212677</v>
       </c>
       <c r="D59" t="n">
-        <v>0.2592358116536779</v>
+        <v>0.2594636994435451</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="n">
-        <v>2568</v>
+        <v>2171</v>
       </c>
       <c r="B60" t="n">
         <v>0</v>
       </c>
       <c r="C60" t="n">
-        <v>0.9297153949737549</v>
+        <v>0.9276847839355469</v>
       </c>
       <c r="D60" t="n">
-        <v>0.2591055661898786</v>
+        <v>0.2593785063651349</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="n">
-        <v>104</v>
+        <v>918</v>
       </c>
       <c r="B61" t="n">
         <v>0</v>
       </c>
       <c r="C61" t="n">
-        <v>0.9297687709331512</v>
+        <v>0.9284694790840149</v>
       </c>
       <c r="D61" t="n">
-        <v>0.2590983995239088</v>
+        <v>0.2592729651275011</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="n">
-        <v>1909</v>
+        <v>1090</v>
       </c>
       <c r="B62" t="n">
         <v>0</v>
       </c>
       <c r="C62" t="n">
-        <v>0.9307088454564413</v>
+        <v>0.9293221433957418</v>
       </c>
       <c r="D62" t="n">
-        <v>0.2589722428509382</v>
+        <v>0.2591583793880917</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="n">
-        <v>1799</v>
+        <v>920</v>
       </c>
       <c r="B63" t="n">
         <v>0</v>
       </c>
       <c r="C63" t="n">
-        <v>0.9329041242599487</v>
+        <v>0.9314544995625814</v>
       </c>
       <c r="D63" t="n">
-        <v>0.2586781174112477</v>
+        <v>0.2588722644583321</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="n">
-        <v>2515</v>
+        <v>926</v>
       </c>
       <c r="B64" t="n">
         <v>0</v>
       </c>
       <c r="C64" t="n">
-        <v>0.9349757432937622</v>
+        <v>0.9321381449699402</v>
       </c>
       <c r="D64" t="n">
-        <v>0.2584011720730349</v>
+        <v>0.2587806680912968</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="n">
-        <v>2073</v>
+        <v>1159</v>
       </c>
       <c r="B65" t="n">
         <v>0</v>
       </c>
       <c r="C65" t="n">
-        <v>0.9355558753013611</v>
+        <v>0.9333501607179642</v>
       </c>
       <c r="D65" t="n">
-        <v>0.2583237231124373</v>
+        <v>0.2586184386869274</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="n">
-        <v>2567</v>
+        <v>367</v>
       </c>
       <c r="B66" t="n">
         <v>0</v>
       </c>
       <c r="C66" t="n">
-        <v>0.9369664788246155</v>
+        <v>0.9338849782943726</v>
       </c>
       <c r="D66" t="n">
-        <v>0.2581355978361632</v>
+        <v>0.258546917532285</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="n">
-        <v>1980</v>
+        <v>1171</v>
       </c>
       <c r="B67" t="n">
         <v>0</v>
       </c>
       <c r="C67" t="n">
-        <v>0.9372656345367432</v>
+        <v>0.9345224698384603</v>
       </c>
       <c r="D67" t="n">
-        <v>0.2580957361170372</v>
+        <v>0.2584617174499668</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="n">
-        <v>1855</v>
+        <v>1300</v>
       </c>
       <c r="B68" t="n">
         <v>0</v>
       </c>
       <c r="C68" t="n">
-        <v>0.9380872845649719</v>
+        <v>0.9349758625030518</v>
       </c>
       <c r="D68" t="n">
-        <v>0.2579863167061804</v>
+        <v>0.2584011561535494</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="n">
-        <v>1198</v>
+        <v>2033</v>
       </c>
       <c r="B69" t="n">
         <v>0</v>
       </c>
       <c r="C69" t="n">
-        <v>0.9380983114242554</v>
+        <v>0.9366790890693665</v>
       </c>
       <c r="D69" t="n">
-        <v>0.2579848488865168</v>
+        <v>0.2581739033699513</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="n">
-        <v>2416</v>
+        <v>427</v>
       </c>
       <c r="B70" t="n">
         <v>0</v>
       </c>
       <c r="C70" t="n">
-        <v>0.9386406242847443</v>
+        <v>0.9371526598930359</v>
       </c>
       <c r="D70" t="n">
-        <v>0.2579126805332853</v>
+        <v>0.2581107882471217</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="n">
-        <v>2478</v>
+        <v>1551</v>
       </c>
       <c r="B71" t="n">
         <v>0</v>
       </c>
       <c r="C71" t="n">
-        <v>0.9386791586875916</v>
+        <v>0.9375317096710205</v>
       </c>
       <c r="D71" t="n">
-        <v>0.2579075540990909</v>
+        <v>0.2580602926415571</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="n">
-        <v>1853</v>
+        <v>1089</v>
       </c>
       <c r="B72" t="n">
         <v>0</v>
       </c>
       <c r="C72" t="n">
-        <v>0.9387034177780151</v>
+        <v>0.9376453161239624</v>
       </c>
       <c r="D72" t="n">
-        <v>0.2579043268892874</v>
+        <v>0.2580451622592068</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="n">
-        <v>292</v>
+        <v>2195</v>
       </c>
       <c r="B73" t="n">
         <v>0</v>
       </c>
       <c r="C73" t="n">
-        <v>0.9387832581996918</v>
+        <v>0.9380930066108704</v>
       </c>
       <c r="D73" t="n">
-        <v>0.2578937062125697</v>
+        <v>0.2579855550247026</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="n">
-        <v>1675</v>
+        <v>2167</v>
       </c>
       <c r="B74" t="n">
         <v>0</v>
       </c>
       <c r="C74" t="n">
-        <v>0.9388269782066345</v>
+        <v>0.9383246064186096</v>
       </c>
       <c r="D74" t="n">
-        <v>0.2578878907815112</v>
+        <v>0.2579547297414939</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="n">
-        <v>1801</v>
+        <v>1831</v>
       </c>
       <c r="B75" t="n">
         <v>0</v>
       </c>
       <c r="C75" t="n">
-        <v>0.9389307796955109</v>
+        <v>0.9383735259373983</v>
       </c>
       <c r="D75" t="n">
-        <v>0.257874084642939</v>
+        <v>0.2579482196333649</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="n">
-        <v>2151</v>
+        <v>1173</v>
       </c>
       <c r="B76" t="n">
         <v>0</v>
       </c>
       <c r="C76" t="n">
-        <v>0.9389899174372355</v>
+        <v>0.9387868543465933</v>
       </c>
       <c r="D76" t="n">
-        <v>0.2578662196762995</v>
+        <v>0.257893227860011</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="n">
-        <v>2219</v>
+        <v>408</v>
       </c>
       <c r="B77" t="n">
         <v>0</v>
       </c>
       <c r="C77" t="n">
-        <v>0.9390560507774353</v>
+        <v>0.9388494849205017</v>
       </c>
       <c r="D77" t="n">
-        <v>0.2578574249050369</v>
+        <v>0.2578848971458459</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="n">
-        <v>417</v>
+        <v>146</v>
       </c>
       <c r="B78" t="n">
         <v>0</v>
       </c>
       <c r="C78" t="n">
-        <v>0.9396763741970062</v>
+        <v>0.9388811826705933</v>
       </c>
       <c r="D78" t="n">
-        <v>0.2577749601177628</v>
+        <v>0.2578806811211121</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="n">
-        <v>1183</v>
+        <v>737</v>
       </c>
       <c r="B79" t="n">
         <v>0</v>
       </c>
       <c r="C79" t="n">
-        <v>0.9398043553034464</v>
+        <v>0.9393596649169922</v>
       </c>
       <c r="D79" t="n">
-        <v>0.2577579530806777</v>
+        <v>0.2578170563433889</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="n">
-        <v>1617</v>
+        <v>2060</v>
       </c>
       <c r="B80" t="n">
         <v>0</v>
       </c>
       <c r="C80" t="n">
-        <v>0.9402076005935669</v>
+        <v>0.9398925503094991</v>
       </c>
       <c r="D80" t="n">
-        <v>0.2577043816584551</v>
+        <v>0.2577462344088222</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="n">
-        <v>1613</v>
+        <v>1207</v>
       </c>
       <c r="B81" t="n">
         <v>0</v>
       </c>
       <c r="C81" t="n">
-        <v>0.9402670661608378</v>
+        <v>0.9413907726605734</v>
       </c>
       <c r="D81" t="n">
-        <v>0.2576964834997373</v>
+        <v>0.2575473248565905</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="n">
-        <v>1523</v>
+        <v>1721</v>
       </c>
       <c r="B82" t="n">
         <v>0</v>
       </c>
       <c r="C82" t="n">
-        <v>0.9407958507537841</v>
+        <v>0.9419825077056885</v>
       </c>
       <c r="D82" t="n">
-        <v>0.2576262721325406</v>
+        <v>0.2574688484659493</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="n">
-        <v>98</v>
+        <v>649</v>
       </c>
       <c r="B83" t="n">
         <v>0</v>
       </c>
       <c r="C83" t="n">
-        <v>0.941187858581543</v>
+        <v>0.9420952796936035</v>
       </c>
       <c r="D83" t="n">
-        <v>0.2575742465056206</v>
+        <v>0.2574538979770771</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="n">
-        <v>583</v>
+        <v>2298</v>
       </c>
       <c r="B84" t="n">
         <v>0</v>
       </c>
       <c r="C84" t="n">
-        <v>0.9416183352470398</v>
+        <v>0.9429007768630981</v>
       </c>
       <c r="D84" t="n">
-        <v>0.2575171396578221</v>
+        <v>0.257347161499041</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="n">
-        <v>584</v>
+        <v>2134</v>
       </c>
       <c r="B85" t="n">
         <v>0</v>
       </c>
       <c r="C85" t="n">
-        <v>0.9417591293652853</v>
+        <v>0.9436931014060974</v>
       </c>
       <c r="D85" t="n">
-        <v>0.2574984674661672</v>
+        <v>0.2572422568348328</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="n">
-        <v>1091</v>
+        <v>1172</v>
       </c>
       <c r="B86" t="n">
         <v>0</v>
       </c>
       <c r="C86" t="n">
-        <v>0.9428647607564926</v>
+        <v>0.9439693689346313</v>
       </c>
       <c r="D86" t="n">
-        <v>0.2573519321053078</v>
+        <v>0.257205698808937</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="n">
-        <v>268</v>
+        <v>482</v>
       </c>
       <c r="B87" t="n">
         <v>0</v>
       </c>
       <c r="C87" t="n">
-        <v>0.9430677195390066</v>
+        <v>0.9442408800125122</v>
       </c>
       <c r="D87" t="n">
-        <v>0.2573250509861927</v>
+        <v>0.257169780318981</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="n">
-        <v>346</v>
+        <v>483</v>
       </c>
       <c r="B88" t="n">
         <v>0</v>
       </c>
       <c r="C88" t="n">
-        <v>0.9431021809577942</v>
+        <v>0.9442528386910757</v>
       </c>
       <c r="D88" t="n">
-        <v>0.2573204872599855</v>
+        <v>0.257168198523302</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="n">
-        <v>2106</v>
+        <v>1263</v>
       </c>
       <c r="B89" t="n">
         <v>0</v>
       </c>
       <c r="C89" t="n">
-        <v>0.9437994956970215</v>
+        <v>0.9447107911109924</v>
       </c>
       <c r="D89" t="n">
-        <v>0.2572281766235907</v>
+        <v>0.2571076389792414</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="n">
-        <v>450</v>
+        <v>2403</v>
       </c>
       <c r="B90" t="n">
         <v>0</v>
       </c>
       <c r="C90" t="n">
-        <v>0.9445163488388062</v>
+        <v>0.9451493720213572</v>
       </c>
       <c r="D90" t="n">
-        <v>0.2571333485051857</v>
+        <v>0.2570496678516832</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="n">
-        <v>1179</v>
+        <v>425</v>
       </c>
       <c r="B91" t="n">
         <v>0</v>
       </c>
       <c r="C91" t="n">
-        <v>0.9445422887802124</v>
+        <v>0.9458949069182078</v>
       </c>
       <c r="D91" t="n">
-        <v>0.2571299183797355</v>
+        <v>0.2569511838601141</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="n">
-        <v>1505</v>
+        <v>2401</v>
       </c>
       <c r="B92" t="n">
         <v>0</v>
       </c>
       <c r="C92" t="n">
-        <v>0.945213258266449</v>
+        <v>0.9473140041033427</v>
       </c>
       <c r="D92" t="n">
-        <v>0.2570412256215003</v>
+        <v>0.2567639317266808</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="n">
-        <v>266</v>
+        <v>49</v>
       </c>
       <c r="B93" t="n">
         <v>0</v>
       </c>
       <c r="C93" t="n">
-        <v>0.945323626200358</v>
+        <v>0.9487814903259277</v>
       </c>
       <c r="D93" t="n">
-        <v>0.257026642387832</v>
+        <v>0.2565705814028316</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="n">
-        <v>1800</v>
+        <v>2065</v>
       </c>
       <c r="B94" t="n">
         <v>0</v>
       </c>
       <c r="C94" t="n">
-        <v>0.9473799367745718</v>
+        <v>0.9507782558600107</v>
       </c>
       <c r="D94" t="n">
-        <v>0.2567552384400887</v>
+        <v>0.256307962474993</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="n">
-        <v>2422</v>
+        <v>667</v>
       </c>
       <c r="B95" t="n">
         <v>0</v>
       </c>
       <c r="C95" t="n">
-        <v>0.9480330348014832</v>
+        <v>0.9515478372573852</v>
       </c>
       <c r="D95" t="n">
-        <v>0.2566691586166829</v>
+        <v>0.2562068889393338</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="n">
-        <v>723</v>
+        <v>2331</v>
       </c>
       <c r="B96" t="n">
         <v>0</v>
       </c>
       <c r="C96" t="n">
-        <v>0.9484446744124094</v>
+        <v>0.9522557973861694</v>
       </c>
       <c r="D96" t="n">
-        <v>0.2566149332163021</v>
+        <v>0.2561139788492054</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="n">
-        <v>728</v>
+        <v>1726</v>
       </c>
       <c r="B97" t="n">
         <v>0</v>
       </c>
       <c r="C97" t="n">
-        <v>0.9484995007514954</v>
+        <v>0.9525412718454996</v>
       </c>
       <c r="D97" t="n">
-        <v>0.256607712656411</v>
+        <v>0.2560765332900804</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="n">
-        <v>846</v>
+        <v>175</v>
       </c>
       <c r="B98" t="n">
         <v>0</v>
       </c>
       <c r="C98" t="n">
-        <v>0.9486296296119689</v>
+        <v>0.9526031414667765</v>
       </c>
       <c r="D98" t="n">
-        <v>0.2565905764758207</v>
+        <v>0.2560684193227329</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="n">
-        <v>526</v>
+        <v>2197</v>
       </c>
       <c r="B99" t="n">
         <v>0</v>
       </c>
       <c r="C99" t="n">
-        <v>0.9488712052504221</v>
+        <v>0.9529149830341339</v>
       </c>
       <c r="D99" t="n">
-        <v>0.2565587703553515</v>
+        <v>0.2560275303040475</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="n">
-        <v>528</v>
+        <v>2055</v>
       </c>
       <c r="B100" t="n">
         <v>0</v>
       </c>
       <c r="C100" t="n">
-        <v>0.9502724707126617</v>
+        <v>0.9530443648497263</v>
       </c>
       <c r="D100" t="n">
-        <v>0.2563744335771154</v>
+        <v>0.2560105694467784</v>
       </c>
     </row>
   </sheetData>

</xml_diff>